<commit_message>
Assume leaders are unique
</commit_message>
<xml_diff>
--- a/cards.xlsx
+++ b/cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\witcher-3-gwent-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3021DD6D-0DFD-46BF-8C11-6A4E7B0A1C7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAFB4472-A05A-4A11-BE0C-7AC4C40871D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{C7211A38-802B-4C9D-8105-50DCB0156070}"/>
   </bookViews>
@@ -797,13 +797,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{60D01DD4-478E-4205-AEF9-F85464A53457}" name="Table2" displayName="Table2" ref="A1:M183" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:M183" xr:uid="{60D01DD4-478E-4205-AEF9-F85464A53457}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="Leader"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:M183" xr:uid="{60D01DD4-478E-4205-AEF9-F85464A53457}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{4610AC45-9F14-4FA0-AE17-310E1E3CEC88}" name="Name"/>
     <tableColumn id="2" xr3:uid="{3B3D3B39-7AE0-4A02-B928-703B22442C21}" name="Occurrences"/>
@@ -1123,8 +1117,8 @@
   <dimension ref="A1:M183"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L152" sqref="L152"/>
+      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E175" sqref="E175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1184,7 +1178,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="2" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -1204,7 +1198,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1227,7 +1221,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -1250,7 +1244,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -1273,7 +1267,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -1293,7 +1287,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -1316,7 +1310,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -1340,9 +1334,6 @@
       <c r="A9" t="s">
         <v>39</v>
       </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
@@ -1354,9 +1345,6 @@
       <c r="A10" t="s">
         <v>40</v>
       </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
@@ -1368,9 +1356,6 @@
       <c r="A11" t="s">
         <v>41</v>
       </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
@@ -1382,9 +1367,6 @@
       <c r="A12" t="s">
         <v>42</v>
       </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
@@ -1392,7 +1374,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -1412,7 +1394,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -1435,7 +1417,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -1455,7 +1437,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -1475,7 +1457,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>46</v>
       </c>
@@ -1498,7 +1480,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>47</v>
       </c>
@@ -1521,7 +1503,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -1541,7 +1523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -1561,7 +1543,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -1581,7 +1563,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>50</v>
       </c>
@@ -1601,7 +1583,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>51</v>
       </c>
@@ -1621,7 +1603,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>52</v>
       </c>
@@ -1644,7 +1626,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>53</v>
       </c>
@@ -1664,7 +1646,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>54</v>
       </c>
@@ -1687,7 +1669,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>55</v>
       </c>
@@ -1707,7 +1689,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>56</v>
       </c>
@@ -1727,7 +1709,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>57</v>
       </c>
@@ -1747,7 +1729,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>58</v>
       </c>
@@ -1767,7 +1749,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>59</v>
       </c>
@@ -1787,7 +1769,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>60</v>
       </c>
@@ -1807,7 +1789,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>61</v>
       </c>
@@ -1827,7 +1809,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>62</v>
       </c>
@@ -1847,7 +1829,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>63</v>
       </c>
@@ -1871,9 +1853,6 @@
       <c r="A36" t="s">
         <v>64</v>
       </c>
-      <c r="B36">
-        <v>1</v>
-      </c>
       <c r="C36" t="s">
         <v>9</v>
       </c>
@@ -1885,9 +1864,6 @@
       <c r="A37" t="s">
         <v>65</v>
       </c>
-      <c r="B37">
-        <v>1</v>
-      </c>
       <c r="C37" t="s">
         <v>9</v>
       </c>
@@ -1899,9 +1875,6 @@
       <c r="A38" t="s">
         <v>66</v>
       </c>
-      <c r="B38">
-        <v>1</v>
-      </c>
       <c r="C38" t="s">
         <v>9</v>
       </c>
@@ -1913,9 +1886,6 @@
       <c r="A39" t="s">
         <v>67</v>
       </c>
-      <c r="B39">
-        <v>1</v>
-      </c>
       <c r="C39" t="s">
         <v>9</v>
       </c>
@@ -1923,7 +1893,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>68</v>
       </c>
@@ -1946,7 +1916,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>69</v>
       </c>
@@ -1966,7 +1936,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>70</v>
       </c>
@@ -1986,7 +1956,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>71</v>
       </c>
@@ -2009,7 +1979,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>72</v>
       </c>
@@ -2029,7 +1999,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>73</v>
       </c>
@@ -2052,7 +2022,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>74</v>
       </c>
@@ -2072,7 +2042,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>75</v>
       </c>
@@ -2092,7 +2062,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>76</v>
       </c>
@@ -2112,7 +2082,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>77</v>
       </c>
@@ -2132,7 +2102,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>78</v>
       </c>
@@ -2152,7 +2122,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>79</v>
       </c>
@@ -2172,7 +2142,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>80</v>
       </c>
@@ -2192,7 +2162,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>81</v>
       </c>
@@ -2215,7 +2185,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>82</v>
       </c>
@@ -2235,7 +2205,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>83</v>
       </c>
@@ -2258,7 +2228,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>84</v>
       </c>
@@ -2281,7 +2251,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>85</v>
       </c>
@@ -2301,7 +2271,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>86</v>
       </c>
@@ -2321,7 +2291,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>87</v>
       </c>
@@ -2341,7 +2311,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>88</v>
       </c>
@@ -2364,7 +2334,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>89</v>
       </c>
@@ -2384,7 +2354,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>90</v>
       </c>
@@ -2407,7 +2377,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>91</v>
       </c>
@@ -2427,7 +2397,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>92</v>
       </c>
@@ -2453,7 +2423,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>93</v>
       </c>
@@ -2479,7 +2449,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>94</v>
       </c>
@@ -2499,7 +2469,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>95</v>
       </c>
@@ -2519,7 +2489,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>96</v>
       </c>
@@ -2545,7 +2515,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="69" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>97</v>
       </c>
@@ -2568,7 +2538,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="70" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>98</v>
       </c>
@@ -2588,7 +2558,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>99</v>
       </c>
@@ -2611,7 +2581,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="72" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>100</v>
       </c>
@@ -2641,9 +2611,6 @@
       <c r="A73" t="s">
         <v>101</v>
       </c>
-      <c r="B73">
-        <v>1</v>
-      </c>
       <c r="C73" t="s">
         <v>5</v>
       </c>
@@ -2655,9 +2622,6 @@
       <c r="A74" t="s">
         <v>102</v>
       </c>
-      <c r="B74">
-        <v>1</v>
-      </c>
       <c r="C74" t="s">
         <v>5</v>
       </c>
@@ -2669,9 +2633,6 @@
       <c r="A75" t="s">
         <v>103</v>
       </c>
-      <c r="B75">
-        <v>1</v>
-      </c>
       <c r="C75" t="s">
         <v>5</v>
       </c>
@@ -2683,9 +2644,6 @@
       <c r="A76" t="s">
         <v>104</v>
       </c>
-      <c r="B76">
-        <v>1</v>
-      </c>
       <c r="C76" t="s">
         <v>5</v>
       </c>
@@ -2693,7 +2651,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>105</v>
       </c>
@@ -2716,7 +2674,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>106</v>
       </c>
@@ -2739,7 +2697,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="79" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>107</v>
       </c>
@@ -2759,7 +2717,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>108</v>
       </c>
@@ -2779,7 +2737,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="81" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>109</v>
       </c>
@@ -2802,7 +2760,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="82" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>110</v>
       </c>
@@ -2822,7 +2780,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>111</v>
       </c>
@@ -2845,7 +2803,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="84" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>112</v>
       </c>
@@ -2865,7 +2823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>113</v>
       </c>
@@ -2885,7 +2843,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="86" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>114</v>
       </c>
@@ -2905,7 +2863,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>115</v>
       </c>
@@ -2925,7 +2883,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="88" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>116</v>
       </c>
@@ -2951,7 +2909,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="89" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>117</v>
       </c>
@@ -2977,7 +2935,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="90" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>118</v>
       </c>
@@ -2997,7 +2955,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="91" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>119</v>
       </c>
@@ -3023,7 +2981,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="92" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>120</v>
       </c>
@@ -3043,7 +3001,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>121</v>
       </c>
@@ -3069,7 +3027,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="94" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>122</v>
       </c>
@@ -3089,7 +3047,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>123</v>
       </c>
@@ -3115,7 +3073,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="96" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>124</v>
       </c>
@@ -3141,7 +3099,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="97" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>125</v>
       </c>
@@ -3167,7 +3125,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="98" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>126</v>
       </c>
@@ -3187,7 +3145,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="99" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>127</v>
       </c>
@@ -3207,7 +3165,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="100" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>128</v>
       </c>
@@ -3231,9 +3189,6 @@
       <c r="A101" t="s">
         <v>129</v>
       </c>
-      <c r="B101">
-        <v>1</v>
-      </c>
       <c r="C101" t="s">
         <v>7</v>
       </c>
@@ -3245,9 +3200,6 @@
       <c r="A102" t="s">
         <v>130</v>
       </c>
-      <c r="B102">
-        <v>1</v>
-      </c>
       <c r="C102" t="s">
         <v>7</v>
       </c>
@@ -3259,9 +3211,6 @@
       <c r="A103" t="s">
         <v>131</v>
       </c>
-      <c r="B103">
-        <v>1</v>
-      </c>
       <c r="C103" t="s">
         <v>7</v>
       </c>
@@ -3273,9 +3222,6 @@
       <c r="A104" t="s">
         <v>132</v>
       </c>
-      <c r="B104">
-        <v>1</v>
-      </c>
       <c r="C104" t="s">
         <v>7</v>
       </c>
@@ -3283,7 +3229,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="105" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>133</v>
       </c>
@@ -3303,7 +3249,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="106" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>134</v>
       </c>
@@ -3323,7 +3269,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="107" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>135</v>
       </c>
@@ -3343,7 +3289,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>136</v>
       </c>
@@ -3363,7 +3309,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="109" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>137</v>
       </c>
@@ -3383,7 +3329,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="110" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>138</v>
       </c>
@@ -3403,7 +3349,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="111" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>139</v>
       </c>
@@ -3426,7 +3372,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="112" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>140</v>
       </c>
@@ -3446,7 +3392,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="113" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>141</v>
       </c>
@@ -3466,7 +3412,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="114" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>142</v>
       </c>
@@ -3492,7 +3438,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="115" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>143</v>
       </c>
@@ -3512,7 +3458,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="116" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>144</v>
       </c>
@@ -3532,7 +3478,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="117" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>145</v>
       </c>
@@ -3555,7 +3501,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="118" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>146</v>
       </c>
@@ -3575,7 +3521,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="119" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>147</v>
       </c>
@@ -3598,7 +3544,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="120" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>148</v>
       </c>
@@ -3618,7 +3564,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="121" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>214</v>
       </c>
@@ -3644,7 +3590,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="122" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>215</v>
       </c>
@@ -3667,7 +3613,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="123" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>216</v>
       </c>
@@ -3690,7 +3636,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="124" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>217</v>
       </c>
@@ -3713,7 +3659,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="125" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>218</v>
       </c>
@@ -3736,7 +3682,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="126" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>149</v>
       </c>
@@ -3756,7 +3702,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="127" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>150</v>
       </c>
@@ -3776,7 +3722,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="128" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>151</v>
       </c>
@@ -3799,7 +3745,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="129" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>152</v>
       </c>
@@ -3819,7 +3765,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="130" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>153</v>
       </c>
@@ -3845,7 +3791,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="131" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>154</v>
       </c>
@@ -3862,7 +3808,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="132" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>155</v>
       </c>
@@ -3879,7 +3825,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="133" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>156</v>
       </c>
@@ -3902,7 +3848,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="134" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>25</v>
       </c>
@@ -3919,7 +3865,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="135" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>157</v>
       </c>
@@ -3939,7 +3885,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="136" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>158</v>
       </c>
@@ -3965,7 +3911,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="137" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>159</v>
       </c>
@@ -3985,7 +3931,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="138" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>24</v>
       </c>
@@ -4002,7 +3948,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="139" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>160</v>
       </c>
@@ -4022,7 +3968,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="140" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>161</v>
       </c>
@@ -4042,7 +3988,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="141" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>162</v>
       </c>
@@ -4062,7 +4008,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="142" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>163</v>
       </c>
@@ -4091,7 +4037,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="143" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>164</v>
       </c>
@@ -4114,7 +4060,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="144" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>165</v>
       </c>
@@ -4138,9 +4084,6 @@
       <c r="A145" t="s">
         <v>167</v>
       </c>
-      <c r="B145">
-        <v>1</v>
-      </c>
       <c r="C145" t="s">
         <v>7</v>
       </c>
@@ -4151,7 +4094,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="146" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>168</v>
       </c>
@@ -4183,7 +4126,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="147" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>169</v>
       </c>
@@ -4209,7 +4152,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="148" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>170</v>
       </c>
@@ -4238,7 +4181,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="149" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>171</v>
       </c>
@@ -4264,7 +4207,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="150" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>172</v>
       </c>
@@ -4300,9 +4243,6 @@
       <c r="A151" t="s">
         <v>174</v>
       </c>
-      <c r="B151">
-        <v>1</v>
-      </c>
       <c r="C151" t="s">
         <v>9</v>
       </c>
@@ -4317,9 +4257,6 @@
       <c r="A152" t="s">
         <v>175</v>
       </c>
-      <c r="B152">
-        <v>1</v>
-      </c>
       <c r="C152" t="s">
         <v>4</v>
       </c>
@@ -4334,9 +4271,6 @@
       <c r="A153" t="s">
         <v>176</v>
       </c>
-      <c r="B153">
-        <v>1</v>
-      </c>
       <c r="C153" t="s">
         <v>5</v>
       </c>
@@ -4347,7 +4281,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="154" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>177</v>
       </c>
@@ -4379,7 +4313,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="155" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>178</v>
       </c>
@@ -4405,7 +4339,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="156" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>179</v>
       </c>
@@ -4431,7 +4365,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="157" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>180</v>
       </c>
@@ -4454,7 +4388,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="158" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>181</v>
       </c>
@@ -4483,7 +4417,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="159" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>182</v>
       </c>
@@ -4509,7 +4443,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="160" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>183</v>
       </c>
@@ -4532,7 +4466,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="161" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>184</v>
       </c>
@@ -4558,7 +4492,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="162" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>185</v>
       </c>
@@ -4584,7 +4518,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="163" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>186</v>
       </c>
@@ -4607,7 +4541,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="164" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>187</v>
       </c>
@@ -4634,9 +4568,6 @@
       <c r="A165" t="s">
         <v>188</v>
       </c>
-      <c r="B165">
-        <v>1</v>
-      </c>
       <c r="C165" t="s">
         <v>8</v>
       </c>
@@ -4647,7 +4578,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="166" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>189</v>
       </c>
@@ -4670,7 +4601,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="167" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>190</v>
       </c>
@@ -4696,7 +4627,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="168" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>191</v>
       </c>
@@ -4722,7 +4653,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="169" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>192</v>
       </c>
@@ -4745,7 +4676,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="170" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>193</v>
       </c>
@@ -4768,7 +4699,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="171" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>194</v>
       </c>
@@ -4798,9 +4729,6 @@
       <c r="A172" t="s">
         <v>195</v>
       </c>
-      <c r="B172">
-        <v>1</v>
-      </c>
       <c r="C172" t="s">
         <v>8</v>
       </c>
@@ -4811,7 +4739,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="173" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>196</v>
       </c>
@@ -4837,7 +4765,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="174" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>197</v>
       </c>
@@ -4860,7 +4788,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="175" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>27</v>
       </c>
@@ -4880,7 +4808,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="176" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>198</v>
       </c>
@@ -4912,7 +4840,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="177" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>173</v>
       </c>
@@ -4938,7 +4866,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="178" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>199</v>
       </c>
@@ -4961,7 +4889,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="179" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>200</v>
       </c>
@@ -4984,7 +4912,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="180" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>201</v>
       </c>
@@ -5010,7 +4938,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="181" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>202</v>
       </c>
@@ -5036,7 +4964,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="182" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>205</v>
       </c>
@@ -5062,7 +4990,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="183" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>210</v>
       </c>
@@ -5140,7 +5068,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5284,5 +5212,6 @@
     <sortCondition ref="E2:E4"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
DLC field for factions
</commit_message>
<xml_diff>
--- a/cards.xlsx
+++ b/cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\witcher-3-gwent-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE2A971-A4A5-4A16-92F8-12BAE3BDC4B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{731122A5-5822-40A6-A3D0-8327DAE288E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{C7211A38-802B-4C9D-8105-50DCB0156070}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="926" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="252">
   <si>
     <t>Name</t>
   </si>
@@ -907,10 +907,11 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C3E9AFB8-AB37-483D-9378-0815904A62C0}" name="Table1" displayName="Table1" ref="A1:B7" totalsRowShown="0">
-  <autoFilter ref="A1:B7" xr:uid="{C3E9AFB8-AB37-483D-9378-0815904A62C0}"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C3E9AFB8-AB37-483D-9378-0815904A62C0}" name="Table1" displayName="Table1" ref="A1:C7" totalsRowShown="0">
+  <autoFilter ref="A1:C7" xr:uid="{C3E9AFB8-AB37-483D-9378-0815904A62C0}"/>
+  <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{D50DA91B-9B0F-4643-8E68-44DCD7661CE8}" name="Name"/>
+    <tableColumn id="3" xr3:uid="{50A907EC-4626-4634-A720-386984346DC4}" name="DLC"/>
     <tableColumn id="2" xr3:uid="{02801729-CABB-4FE6-8F85-EF4F262DC81A}" name="Ability"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -5235,68 +5236,75 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25A54F22-A8E1-4D1D-A0B0-55BC53600CD0}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="79.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.21875" customWidth="1"/>
+    <col min="3" max="3" width="79.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C1" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" t="s">
+        <v>203</v>
+      </c>
+      <c r="C7" t="s">
         <v>251</v>
       </c>
     </row>
@@ -5305,6 +5313,18 @@
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B2A12E8C-C164-4586-A1BF-A068E74D5998}">
+          <x14:formula1>
+            <xm:f>Types!$E$2:$E$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B7</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Rename Muster Prefix to Effect Prefix
</commit_message>
<xml_diff>
--- a/cards.xlsx
+++ b/cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\witcher-3-gwent-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{894F6896-1475-4423-B002-7C845461ABB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D64B05DC-830B-4E93-84D0-93E8223ED5D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{C7211A38-802B-4C9D-8105-50DCB0156070}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1150" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1152" uniqueCount="456">
   <si>
     <t>Name</t>
   </si>
@@ -620,9 +620,6 @@
     <t>Close</t>
   </si>
   <si>
-    <t>Muster Prefix</t>
-  </si>
-  <si>
     <t>Roach</t>
   </si>
   <si>
@@ -632,9 +629,6 @@
     <t>Crone</t>
   </si>
   <si>
-    <t>Vampire:</t>
-  </si>
-  <si>
     <t>Vampire: Bruxa</t>
   </si>
   <si>
@@ -1407,6 +1401,12 @@
   </si>
   <si>
     <t>Can be placed in either the Close or Ranged rows. Cannot be moved once placed.</t>
+  </si>
+  <si>
+    <t>Vampire</t>
+  </si>
+  <si>
+    <t>Effect Prefix</t>
   </si>
 </sst>
 </file>
@@ -1513,7 +1513,7 @@
     <tableColumn id="8" xr3:uid="{74F42BAF-52A5-4B72-9FBE-9DB1F1E47E42}" name="DLC"/>
     <tableColumn id="9" xr3:uid="{C7D13E95-46CD-4D77-8615-90FD10CFB28C}" name="Scorch Scope"/>
     <tableColumn id="10" xr3:uid="{194C12E8-B167-4FF4-9837-5D2A810105A1}" name="Scorch Minimum Strength"/>
-    <tableColumn id="11" xr3:uid="{47B4D91E-5615-4877-B62D-75BC91E9D750}" name="Muster Prefix"/>
+    <tableColumn id="11" xr3:uid="{47B4D91E-5615-4877-B62D-75BC91E9D750}" name="Effect Prefix"/>
     <tableColumn id="16" xr3:uid="{E8DAC3F3-3911-422B-91ED-DAB8FBA3BFC6}" name="Art Styles"/>
     <tableColumn id="12" xr3:uid="{78655D30-08D8-421C-B89F-96A6B89868F7}" name="Ability"/>
     <tableColumn id="15" xr3:uid="{097E4903-2E6B-4199-A1E2-3C8F7ABF4644}" name="Quote"/>
@@ -1846,7 +1846,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1875,28 +1875,28 @@
         <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>152</v>
@@ -1908,16 +1908,16 @@
         <v>191</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>193</v>
+        <v>455</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
@@ -1943,7 +1943,7 @@
         <v>1</v>
       </c>
       <c r="Q2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
@@ -1972,7 +1972,7 @@
         <v>3</v>
       </c>
       <c r="Q3" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
@@ -2004,7 +2004,7 @@
         <v>1</v>
       </c>
       <c r="Q4" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
@@ -2030,7 +2030,7 @@
         <v>1</v>
       </c>
       <c r="Q5" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
@@ -2056,7 +2056,7 @@
         <v>1</v>
       </c>
       <c r="Q6" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
@@ -2088,7 +2088,7 @@
         <v>1</v>
       </c>
       <c r="Q7" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
@@ -2120,7 +2120,7 @@
         <v>1</v>
       </c>
       <c r="Q8" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
@@ -2152,7 +2152,7 @@
         <v>1</v>
       </c>
       <c r="Q9" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
@@ -2178,7 +2178,7 @@
         <v>1</v>
       </c>
       <c r="Q10" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
@@ -2204,7 +2204,7 @@
         <v>2</v>
       </c>
       <c r="Q11" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
@@ -2233,7 +2233,7 @@
         <v>3</v>
       </c>
       <c r="Q12" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
@@ -2262,7 +2262,7 @@
         <v>1</v>
       </c>
       <c r="Q13" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
@@ -2288,18 +2288,18 @@
         <v>1</v>
       </c>
       <c r="Q14" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D15" t="s">
         <v>5</v>
@@ -2320,12 +2320,12 @@
         <v>1</v>
       </c>
       <c r="Q15" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -2346,7 +2346,7 @@
         <v>1</v>
       </c>
       <c r="Q16" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
@@ -2375,12 +2375,12 @@
         <v>2</v>
       </c>
       <c r="Q17" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -2407,7 +2407,7 @@
         <v>1</v>
       </c>
       <c r="Q18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
@@ -2442,7 +2442,7 @@
         <v>1</v>
       </c>
       <c r="Q19" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
@@ -2474,12 +2474,12 @@
         <v>1</v>
       </c>
       <c r="Q20" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -2500,13 +2500,13 @@
         <v>19</v>
       </c>
       <c r="N21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O21">
         <v>2</v>
       </c>
       <c r="Q21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
@@ -2538,7 +2538,7 @@
         <v>1</v>
       </c>
       <c r="Q22" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.3">
@@ -2567,12 +2567,12 @@
         <v>1</v>
       </c>
       <c r="Q23" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -2599,7 +2599,7 @@
         <v>1</v>
       </c>
       <c r="Q24" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.3">
@@ -2631,7 +2631,7 @@
         <v>3</v>
       </c>
       <c r="Q25" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.3">
@@ -2660,7 +2660,7 @@
         <v>1</v>
       </c>
       <c r="Q26" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.3">
@@ -2689,7 +2689,7 @@
         <v>1</v>
       </c>
       <c r="Q27" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.3">
@@ -2712,7 +2712,7 @@
         <v>1</v>
       </c>
       <c r="Q28" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.3">
@@ -2738,7 +2738,7 @@
         <v>1</v>
       </c>
       <c r="Q29" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.3">
@@ -2761,7 +2761,7 @@
         <v>1</v>
       </c>
       <c r="Q30" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.3">
@@ -2789,11 +2789,14 @@
       <c r="K31" t="s">
         <v>187</v>
       </c>
+      <c r="N31" t="s">
+        <v>346</v>
+      </c>
       <c r="O31">
         <v>1</v>
       </c>
       <c r="Q31" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.3">
@@ -2813,10 +2816,10 @@
         <v>1</v>
       </c>
       <c r="P32" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="Q32" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.3">
@@ -2845,7 +2848,7 @@
         <v>3</v>
       </c>
       <c r="Q33" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.3">
@@ -2871,13 +2874,13 @@
         <v>19</v>
       </c>
       <c r="N34" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="O34">
         <v>1</v>
       </c>
       <c r="Q34" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.3">
@@ -2903,13 +2906,13 @@
         <v>19</v>
       </c>
       <c r="N35" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="O35">
         <v>1</v>
       </c>
       <c r="Q35" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.3">
@@ -2935,13 +2938,13 @@
         <v>19</v>
       </c>
       <c r="N36" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="O36">
         <v>1</v>
       </c>
       <c r="Q36" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.3">
@@ -2967,7 +2970,7 @@
         <v>1</v>
       </c>
       <c r="Q37" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.3">
@@ -2996,7 +2999,7 @@
         <v>2</v>
       </c>
       <c r="Q38" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.3">
@@ -3019,7 +3022,7 @@
         <v>1</v>
       </c>
       <c r="Q39" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.3">
@@ -3045,7 +3048,7 @@
         <v>1</v>
       </c>
       <c r="Q40" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.3">
@@ -3071,7 +3074,7 @@
         <v>1</v>
       </c>
       <c r="Q41" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.3">
@@ -3097,7 +3100,7 @@
         <v>1</v>
       </c>
       <c r="Q42" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.3">
@@ -3129,7 +3132,7 @@
         <v>3</v>
       </c>
       <c r="Q43" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.3">
@@ -3158,7 +3161,7 @@
         <v>1</v>
       </c>
       <c r="Q44" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.3">
@@ -3190,7 +3193,7 @@
         <v>1</v>
       </c>
       <c r="Q45" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.3">
@@ -3216,7 +3219,7 @@
         <v>1</v>
       </c>
       <c r="Q46" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.3">
@@ -3245,7 +3248,7 @@
         <v>1</v>
       </c>
       <c r="Q47" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.3">
@@ -3274,7 +3277,7 @@
         <v>3</v>
       </c>
       <c r="Q48" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.3">
@@ -3300,7 +3303,7 @@
         <v>1</v>
       </c>
       <c r="Q49" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.3">
@@ -3326,7 +3329,7 @@
         <v>1</v>
       </c>
       <c r="Q50" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.3">
@@ -3355,12 +3358,12 @@
         <v>3</v>
       </c>
       <c r="Q51" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D52" t="s">
         <v>8</v>
@@ -3372,10 +3375,10 @@
         <v>1</v>
       </c>
       <c r="P52" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="Q52" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.3">
@@ -3392,10 +3395,10 @@
         <v>1</v>
       </c>
       <c r="P53" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="Q53" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.3">
@@ -3415,10 +3418,10 @@
         <v>1</v>
       </c>
       <c r="P54" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="Q54" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.3">
@@ -3435,10 +3438,10 @@
         <v>1</v>
       </c>
       <c r="P55" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="Q55" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.3">
@@ -3455,10 +3458,10 @@
         <v>1</v>
       </c>
       <c r="P56" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="Q56" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.3">
@@ -3484,7 +3487,7 @@
         <v>2</v>
       </c>
       <c r="Q57" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.3">
@@ -3510,7 +3513,7 @@
         <v>1</v>
       </c>
       <c r="Q58" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.3">
@@ -3530,10 +3533,10 @@
         <v>1</v>
       </c>
       <c r="P59" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="Q59" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.3">
@@ -3550,10 +3553,10 @@
         <v>1</v>
       </c>
       <c r="P60" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="Q60" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.3">
@@ -3570,10 +3573,10 @@
         <v>1</v>
       </c>
       <c r="P61" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="Q61" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.3">
@@ -3590,10 +3593,10 @@
         <v>1</v>
       </c>
       <c r="P62" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="Q62" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.3">
@@ -3610,10 +3613,10 @@
         <v>1</v>
       </c>
       <c r="P63" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="Q63" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.3">
@@ -3645,7 +3648,7 @@
         <v>1</v>
       </c>
       <c r="Q64" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.3">
@@ -3671,7 +3674,7 @@
         <v>1</v>
       </c>
       <c r="Q65" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.3">
@@ -3700,7 +3703,7 @@
         <v>2</v>
       </c>
       <c r="Q66" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.3">
@@ -3726,7 +3729,7 @@
         <v>1</v>
       </c>
       <c r="Q67" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.3">
@@ -3758,7 +3761,7 @@
         <v>1</v>
       </c>
       <c r="Q68" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.3">
@@ -3784,7 +3787,7 @@
         <v>1</v>
       </c>
       <c r="Q69" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.3">
@@ -3810,7 +3813,7 @@
         <v>1</v>
       </c>
       <c r="Q70" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.3">
@@ -3827,10 +3830,10 @@
         <v>1</v>
       </c>
       <c r="P71" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="Q71" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.3">
@@ -3847,15 +3850,15 @@
         <v>1</v>
       </c>
       <c r="P72" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="Q72" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D73" t="s">
         <v>3</v>
@@ -3870,10 +3873,10 @@
         <v>1</v>
       </c>
       <c r="P73" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="Q73" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.3">
@@ -3890,10 +3893,10 @@
         <v>1</v>
       </c>
       <c r="P74" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="Q74" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.3">
@@ -3910,10 +3913,10 @@
         <v>1</v>
       </c>
       <c r="P75" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="Q75" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.3">
@@ -3939,7 +3942,7 @@
         <v>1</v>
       </c>
       <c r="Q76" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.3">
@@ -3956,10 +3959,10 @@
         <v>1</v>
       </c>
       <c r="P77" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="Q77" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.3">
@@ -3979,10 +3982,10 @@
         <v>1</v>
       </c>
       <c r="P78" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="Q78" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.3">
@@ -3999,10 +4002,10 @@
         <v>1</v>
       </c>
       <c r="P79" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="Q79" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.3">
@@ -4019,10 +4022,10 @@
         <v>1</v>
       </c>
       <c r="P80" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="Q80" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.3">
@@ -4039,10 +4042,10 @@
         <v>1</v>
       </c>
       <c r="P81" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="Q81" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.3">
@@ -4068,7 +4071,7 @@
         <v>1</v>
       </c>
       <c r="Q82" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.3">
@@ -4094,7 +4097,7 @@
         <v>1</v>
       </c>
       <c r="Q83" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.3">
@@ -4120,7 +4123,7 @@
         <v>1</v>
       </c>
       <c r="Q84" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.3">
@@ -4155,7 +4158,7 @@
         <v>1</v>
       </c>
       <c r="Q85" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.3">
@@ -4187,7 +4190,7 @@
         <v>1</v>
       </c>
       <c r="Q86" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.3">
@@ -4213,13 +4216,13 @@
         <v>19</v>
       </c>
       <c r="N87" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O87">
         <v>2</v>
       </c>
       <c r="Q87" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.3">
@@ -4248,7 +4251,7 @@
         <v>3</v>
       </c>
       <c r="Q88" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.3">
@@ -4274,7 +4277,7 @@
         <v>1</v>
       </c>
       <c r="Q89" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.3">
@@ -4300,7 +4303,7 @@
         <v>1</v>
       </c>
       <c r="Q90" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.3">
@@ -4332,7 +4335,7 @@
         <v>1</v>
       </c>
       <c r="Q91" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.3">
@@ -4361,7 +4364,7 @@
         <v>3</v>
       </c>
       <c r="Q92" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.3">
@@ -4390,7 +4393,7 @@
         <v>3</v>
       </c>
       <c r="Q93" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.3">
@@ -4416,12 +4419,12 @@
         <v>1</v>
       </c>
       <c r="Q94" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B95">
         <v>1</v>
@@ -4445,7 +4448,7 @@
         <v>1</v>
       </c>
       <c r="Q95" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.3">
@@ -4474,7 +4477,7 @@
         <v>1</v>
       </c>
       <c r="Q96" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.3">
@@ -4503,7 +4506,7 @@
         <v>1</v>
       </c>
       <c r="Q97" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.3">
@@ -4529,7 +4532,7 @@
         <v>1</v>
       </c>
       <c r="Q98" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.3">
@@ -4555,7 +4558,7 @@
         <v>1</v>
       </c>
       <c r="Q99" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.3">
@@ -4581,7 +4584,7 @@
         <v>1</v>
       </c>
       <c r="Q100" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="101" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -4607,7 +4610,7 @@
         <v>1</v>
       </c>
       <c r="Q101" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.3">
@@ -4636,7 +4639,7 @@
         <v>4</v>
       </c>
       <c r="Q102" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.3">
@@ -4662,12 +4665,12 @@
         <v>1</v>
       </c>
       <c r="Q103" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B104">
         <v>1</v>
@@ -4691,7 +4694,7 @@
         <v>1</v>
       </c>
       <c r="Q104" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.3">
@@ -4717,7 +4720,7 @@
         <v>1</v>
       </c>
       <c r="Q105" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.3">
@@ -4746,7 +4749,7 @@
         <v>3</v>
       </c>
       <c r="Q106" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.3">
@@ -4774,11 +4777,14 @@
       <c r="K107" t="s">
         <v>188</v>
       </c>
+      <c r="N107" t="s">
+        <v>421</v>
+      </c>
       <c r="O107">
         <v>1</v>
       </c>
       <c r="Q107" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.3">
@@ -4807,7 +4813,7 @@
         <v>1</v>
       </c>
       <c r="Q108" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="109" spans="1:17" x14ac:dyDescent="0.3">
@@ -4833,7 +4839,7 @@
         <v>1</v>
       </c>
       <c r="Q109" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="110" spans="1:17" x14ac:dyDescent="0.3">
@@ -4853,10 +4859,10 @@
         <v>1</v>
       </c>
       <c r="P110" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="Q110" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.3">
@@ -4882,7 +4888,7 @@
         <v>1</v>
       </c>
       <c r="Q111" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="112" spans="1:17" x14ac:dyDescent="0.3">
@@ -4908,7 +4914,7 @@
         <v>1</v>
       </c>
       <c r="Q112" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="113" spans="1:17" x14ac:dyDescent="0.3">
@@ -4940,7 +4946,7 @@
         <v>1</v>
       </c>
       <c r="Q113" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="114" spans="1:17" x14ac:dyDescent="0.3">
@@ -4969,7 +4975,7 @@
         <v>1</v>
       </c>
       <c r="Q114" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="115" spans="1:17" x14ac:dyDescent="0.3">
@@ -4995,7 +5001,7 @@
         <v>5</v>
       </c>
       <c r="Q115" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.3">
@@ -5021,12 +5027,12 @@
         <v>1</v>
       </c>
       <c r="Q116" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B117">
         <v>1</v>
@@ -5050,7 +5056,7 @@
         <v>1</v>
       </c>
       <c r="Q117" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.3">
@@ -5079,7 +5085,7 @@
         <v>1</v>
       </c>
       <c r="Q118" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.3">
@@ -5105,7 +5111,7 @@
         <v>1</v>
       </c>
       <c r="Q119" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="120" spans="1:17" x14ac:dyDescent="0.3">
@@ -5131,12 +5137,12 @@
         <v>1</v>
       </c>
       <c r="Q120" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B121">
         <v>1</v>
@@ -5160,7 +5166,7 @@
         <v>2</v>
       </c>
       <c r="Q121" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="122" spans="1:17" x14ac:dyDescent="0.3">
@@ -5186,7 +5192,7 @@
         <v>1</v>
       </c>
       <c r="Q122" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.3">
@@ -5215,7 +5221,7 @@
         <v>3</v>
       </c>
       <c r="Q123" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="124" spans="1:17" x14ac:dyDescent="0.3">
@@ -5253,7 +5259,7 @@
         <v>1</v>
       </c>
       <c r="Q124" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="125" spans="1:17" x14ac:dyDescent="0.3">
@@ -5291,12 +5297,12 @@
         <v>1</v>
       </c>
       <c r="Q125" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="126" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B126">
         <v>1</v>
@@ -5317,7 +5323,7 @@
         <v>1</v>
       </c>
       <c r="Q126" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="127" spans="1:17" x14ac:dyDescent="0.3">
@@ -5343,7 +5349,7 @@
         <v>1</v>
       </c>
       <c r="Q127" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="128" spans="1:17" x14ac:dyDescent="0.3">
@@ -5372,7 +5378,7 @@
         <v>3</v>
       </c>
       <c r="Q128" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="129" spans="1:17" x14ac:dyDescent="0.3">
@@ -5401,7 +5407,7 @@
         <v>1</v>
       </c>
       <c r="Q129" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="130" spans="1:17" x14ac:dyDescent="0.3">
@@ -5427,7 +5433,7 @@
         <v>1</v>
       </c>
       <c r="Q130" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="131" spans="1:17" x14ac:dyDescent="0.3">
@@ -5453,7 +5459,7 @@
         <v>1</v>
       </c>
       <c r="Q131" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="132" spans="1:17" x14ac:dyDescent="0.3">
@@ -5479,12 +5485,12 @@
         <v>2</v>
       </c>
       <c r="Q132" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="133" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B133">
         <v>1</v>
@@ -5505,7 +5511,7 @@
         <v>1</v>
       </c>
       <c r="Q133" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="134" spans="1:17" x14ac:dyDescent="0.3">
@@ -5531,12 +5537,12 @@
         <v>1</v>
       </c>
       <c r="Q134" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="135" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B135">
         <v>1</v>
@@ -5554,13 +5560,13 @@
         <v>3</v>
       </c>
       <c r="K135" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O135">
         <v>1</v>
       </c>
       <c r="Q135" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="136" spans="1:17" x14ac:dyDescent="0.3">
@@ -5586,7 +5592,7 @@
         <v>1</v>
       </c>
       <c r="Q136" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="137" spans="1:17" x14ac:dyDescent="0.3">
@@ -5612,7 +5618,7 @@
         <v>1</v>
       </c>
       <c r="Q137" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="138" spans="1:17" x14ac:dyDescent="0.3">
@@ -5638,7 +5644,7 @@
         <v>1</v>
       </c>
       <c r="Q138" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="139" spans="1:17" x14ac:dyDescent="0.3">
@@ -5676,7 +5682,7 @@
         <v>1</v>
       </c>
       <c r="Q139" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="140" spans="1:17" x14ac:dyDescent="0.3">
@@ -5699,7 +5705,7 @@
         <v>1</v>
       </c>
       <c r="Q140" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="141" spans="1:17" x14ac:dyDescent="0.3">
@@ -5725,12 +5731,12 @@
         <v>1</v>
       </c>
       <c r="Q141" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="142" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B142">
         <v>1</v>
@@ -5754,7 +5760,7 @@
         <v>1</v>
       </c>
       <c r="Q142" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="143" spans="1:17" x14ac:dyDescent="0.3">
@@ -5780,7 +5786,7 @@
         <v>1</v>
       </c>
       <c r="Q143" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="144" spans="1:17" x14ac:dyDescent="0.3">
@@ -5809,7 +5815,7 @@
         <v>1</v>
       </c>
       <c r="Q144" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="145" spans="1:17" x14ac:dyDescent="0.3">
@@ -5835,7 +5841,7 @@
         <v>2</v>
       </c>
       <c r="Q145" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="146" spans="1:17" x14ac:dyDescent="0.3">
@@ -5861,12 +5867,12 @@
         <v>1</v>
       </c>
       <c r="Q146" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="147" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B147">
         <v>1</v>
@@ -5890,7 +5896,7 @@
         <v>1</v>
       </c>
       <c r="Q147" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="148" spans="1:17" x14ac:dyDescent="0.3">
@@ -5916,7 +5922,7 @@
         <v>1</v>
       </c>
       <c r="Q148" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="149" spans="1:17" x14ac:dyDescent="0.3">
@@ -5948,7 +5954,7 @@
         <v>1</v>
       </c>
       <c r="Q149" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="150" spans="1:17" x14ac:dyDescent="0.3">
@@ -5977,7 +5983,7 @@
         <v>1</v>
       </c>
       <c r="Q150" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="151" spans="1:17" x14ac:dyDescent="0.3">
@@ -6006,7 +6012,7 @@
         <v>1</v>
       </c>
       <c r="Q151" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="152" spans="1:17" x14ac:dyDescent="0.3">
@@ -6032,7 +6038,7 @@
         <v>1</v>
       </c>
       <c r="Q152" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="153" spans="1:17" x14ac:dyDescent="0.3">
@@ -6061,7 +6067,7 @@
         <v>1</v>
       </c>
       <c r="Q153" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="154" spans="1:17" x14ac:dyDescent="0.3">
@@ -6087,7 +6093,7 @@
         <v>1</v>
       </c>
       <c r="Q154" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="155" spans="1:17" x14ac:dyDescent="0.3">
@@ -6125,7 +6131,7 @@
         <v>1</v>
       </c>
       <c r="Q155" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="156" spans="1:17" x14ac:dyDescent="0.3">
@@ -6151,7 +6157,7 @@
         <v>1</v>
       </c>
       <c r="Q156" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="157" spans="1:17" x14ac:dyDescent="0.3">
@@ -6177,7 +6183,7 @@
         <v>1</v>
       </c>
       <c r="Q157" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="158" spans="1:17" x14ac:dyDescent="0.3">
@@ -6188,7 +6194,7 @@
         <v>1</v>
       </c>
       <c r="C158" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D158" t="s">
         <v>7</v>
@@ -6212,18 +6218,18 @@
         <v>1</v>
       </c>
       <c r="Q158" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="159" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B159">
         <v>1</v>
       </c>
       <c r="C159" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D159" t="s">
         <v>7</v>
@@ -6247,7 +6253,7 @@
         <v>1</v>
       </c>
       <c r="Q159" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="160" spans="1:17" x14ac:dyDescent="0.3">
@@ -6273,7 +6279,7 @@
         <v>2</v>
       </c>
       <c r="Q160" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="161" spans="1:17" x14ac:dyDescent="0.3">
@@ -6299,7 +6305,7 @@
         <v>2</v>
       </c>
       <c r="Q161" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="162" spans="1:17" x14ac:dyDescent="0.3">
@@ -6328,12 +6334,12 @@
         <v>1</v>
       </c>
       <c r="Q162" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="163" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B163">
         <v>1</v>
@@ -6354,18 +6360,18 @@
         <v>19</v>
       </c>
       <c r="N163" t="s">
-        <v>197</v>
+        <v>454</v>
       </c>
       <c r="O163">
         <v>1</v>
       </c>
       <c r="Q163" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="164" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B164">
         <v>1</v>
@@ -6389,12 +6395,12 @@
         <v>1</v>
       </c>
       <c r="Q164" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="165" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B165">
         <v>1</v>
@@ -6418,12 +6424,12 @@
         <v>1</v>
       </c>
       <c r="Q165" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="166" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B166">
         <v>1</v>
@@ -6447,12 +6453,12 @@
         <v>1</v>
       </c>
       <c r="Q166" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="167" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B167">
         <v>1</v>
@@ -6476,7 +6482,7 @@
         <v>1</v>
       </c>
       <c r="Q167" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="168" spans="1:17" x14ac:dyDescent="0.3">
@@ -6502,7 +6508,7 @@
         <v>1</v>
       </c>
       <c r="Q168" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="169" spans="1:17" x14ac:dyDescent="0.3">
@@ -6531,7 +6537,7 @@
         <v>1</v>
       </c>
       <c r="Q169" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="170" spans="1:17" x14ac:dyDescent="0.3">
@@ -6557,7 +6563,7 @@
         <v>1</v>
       </c>
       <c r="Q170" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="171" spans="1:17" x14ac:dyDescent="0.3">
@@ -6583,7 +6589,7 @@
         <v>1</v>
       </c>
       <c r="Q171" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="172" spans="1:17" x14ac:dyDescent="0.3">
@@ -6609,7 +6615,7 @@
         <v>2</v>
       </c>
       <c r="Q172" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="173" spans="1:17" x14ac:dyDescent="0.3">
@@ -6644,7 +6650,7 @@
         <v>2</v>
       </c>
       <c r="Q173" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="174" spans="1:17" x14ac:dyDescent="0.3">
@@ -6670,7 +6676,7 @@
         <v>1</v>
       </c>
       <c r="Q174" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="175" spans="1:17" x14ac:dyDescent="0.3">
@@ -6696,7 +6702,7 @@
         <v>1</v>
       </c>
       <c r="Q175" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="176" spans="1:17" x14ac:dyDescent="0.3">
@@ -6728,7 +6734,7 @@
         <v>2</v>
       </c>
       <c r="Q176" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="177" spans="1:17" x14ac:dyDescent="0.3">
@@ -6760,7 +6766,7 @@
         <v>1</v>
       </c>
       <c r="Q177" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="178" spans="1:17" x14ac:dyDescent="0.3">
@@ -6786,7 +6792,7 @@
         <v>1</v>
       </c>
       <c r="Q178" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="179" spans="1:17" x14ac:dyDescent="0.3">
@@ -6812,7 +6818,7 @@
         <v>1</v>
       </c>
       <c r="Q179" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="180" spans="1:17" x14ac:dyDescent="0.3">
@@ -6844,7 +6850,7 @@
         <v>1</v>
       </c>
       <c r="Q180" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="181" spans="1:17" x14ac:dyDescent="0.3">
@@ -6870,12 +6876,12 @@
         <v>1</v>
       </c>
       <c r="Q181" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="182" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B182">
         <v>1</v>
@@ -6899,7 +6905,7 @@
         <v>2</v>
       </c>
       <c r="Q182" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="183" spans="1:17" x14ac:dyDescent="0.3">
@@ -6931,12 +6937,12 @@
         <v>1</v>
       </c>
       <c r="Q183" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="184" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B184">
         <v>2</v>
@@ -6960,7 +6966,7 @@
         <v>2</v>
       </c>
       <c r="Q184" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="185" spans="1:17" x14ac:dyDescent="0.3">
@@ -6986,7 +6992,7 @@
         <v>1</v>
       </c>
       <c r="Q185" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="186" spans="1:17" x14ac:dyDescent="0.3">
@@ -7012,7 +7018,7 @@
         <v>2</v>
       </c>
       <c r="Q186" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
   </sheetData>
@@ -7093,7 +7099,7 @@
         <v>152</v>
       </c>
       <c r="C1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -7101,7 +7107,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -7114,7 +7120,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -7122,7 +7128,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -7130,7 +7136,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -7141,7 +7147,7 @@
         <v>188</v>
       </c>
       <c r="C7" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -7183,7 +7189,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -7191,7 +7197,7 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -7199,7 +7205,7 @@
         <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -7207,7 +7213,7 @@
         <v>163</v>
       </c>
       <c r="B4" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -7215,7 +7221,7 @@
         <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -7223,7 +7229,7 @@
         <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -7231,7 +7237,7 @@
         <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -7239,7 +7245,7 @@
         <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -7247,7 +7253,7 @@
         <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -7255,7 +7261,7 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -7263,7 +7269,7 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -7271,7 +7277,7 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -7279,7 +7285,7 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -7287,7 +7293,7 @@
         <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
   </sheetData>
@@ -7314,7 +7320,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -7351,7 +7357,7 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
All vampires muster all vampires
</commit_message>
<xml_diff>
--- a/cards.xlsx
+++ b/cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\witcher-3-gwent-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B4DC1D2-4C6E-4B59-BC87-7498708945B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB5512D-075A-4C33-82A1-D2E4B5E8F3F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{C7211A38-802B-4C9D-8105-50DCB0156070}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1154" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1158" uniqueCount="456">
   <si>
     <t>Name</t>
   </si>
@@ -1845,8 +1845,8 @@
   <dimension ref="A1:Q186"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G108" sqref="G108"/>
+      <pane ySplit="1" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N164" sqref="N164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6397,6 +6397,9 @@
       <c r="I164" t="s">
         <v>19</v>
       </c>
+      <c r="N164" t="s">
+        <v>454</v>
+      </c>
       <c r="O164">
         <v>1</v>
       </c>
@@ -6426,6 +6429,9 @@
       <c r="I165" t="s">
         <v>19</v>
       </c>
+      <c r="N165" t="s">
+        <v>454</v>
+      </c>
       <c r="O165">
         <v>1</v>
       </c>
@@ -6455,6 +6461,9 @@
       <c r="I166" t="s">
         <v>19</v>
       </c>
+      <c r="N166" t="s">
+        <v>454</v>
+      </c>
       <c r="O166">
         <v>1</v>
       </c>
@@ -6483,6 +6492,9 @@
       </c>
       <c r="I167" t="s">
         <v>19</v>
+      </c>
+      <c r="N167" t="s">
+        <v>454</v>
       </c>
       <c r="O167">
         <v>1</v>

</xml_diff>

<commit_message>
Improve weather ability wording
</commit_message>
<xml_diff>
--- a/cards.xlsx
+++ b/cards.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\witcher-3-gwent-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDBFCF87-7972-4389-A637-B543C8EEA953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60387866-83DC-4D32-8277-2F7644106A34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{C7211A38-802B-4C9D-8105-50DCB0156070}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="3" xr2:uid="{C7211A38-802B-4C9D-8105-50DCB0156070}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -930,9 +930,6 @@
     <t>Swap with a card on the battlefield to return it to your hand.</t>
   </si>
   <si>
-    <t>Reduce the strength of all cards of the given row(s) on the battlefield, including your own.</t>
-  </si>
-  <si>
     <t>Can be placed in either the Close or Ranged rows. Cannot be moved once placed.</t>
   </si>
   <si>
@@ -1399,6 +1396,9 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>Reduce the strength of all cards in the given row(s) on the battlefield, including your own.</t>
   </si>
 </sst>
 </file>
@@ -2074,7 +2074,7 @@
         <v>187</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>233</v>
@@ -2091,7 +2091,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -2109,7 +2109,7 @@
         <v>1</v>
       </c>
       <c r="P2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
@@ -2120,7 +2120,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -2141,7 +2141,7 @@
         <v>3</v>
       </c>
       <c r="P3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
@@ -2152,7 +2152,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
@@ -2176,7 +2176,7 @@
         <v>1</v>
       </c>
       <c r="P4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
@@ -2187,7 +2187,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -2205,7 +2205,7 @@
         <v>1</v>
       </c>
       <c r="P5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
@@ -2216,7 +2216,7 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D6" t="s">
         <v>2</v>
@@ -2234,7 +2234,7 @@
         <v>1</v>
       </c>
       <c r="P6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
@@ -2245,7 +2245,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D7" t="s">
         <v>3</v>
@@ -2269,7 +2269,7 @@
         <v>1</v>
       </c>
       <c r="P7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
@@ -2280,7 +2280,7 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D8" t="s">
         <v>6</v>
@@ -2315,7 +2315,7 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D9" t="s">
         <v>6</v>
@@ -2350,7 +2350,7 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D10" t="s">
         <v>4</v>
@@ -2368,7 +2368,7 @@
         <v>1</v>
       </c>
       <c r="P10" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
@@ -2379,7 +2379,7 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D11" t="s">
         <v>7</v>
@@ -2397,7 +2397,7 @@
         <v>2</v>
       </c>
       <c r="P11" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
@@ -2408,7 +2408,7 @@
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D12" t="s">
         <v>2</v>
@@ -2429,7 +2429,7 @@
         <v>3</v>
       </c>
       <c r="P12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
@@ -2440,7 +2440,7 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D13" t="s">
         <v>6</v>
@@ -2472,7 +2472,7 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>
@@ -2490,7 +2490,7 @@
         <v>1</v>
       </c>
       <c r="P14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
@@ -2522,7 +2522,7 @@
         <v>1</v>
       </c>
       <c r="P15" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
@@ -2533,7 +2533,7 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D16" t="s">
         <v>7</v>
@@ -2551,7 +2551,7 @@
         <v>1</v>
       </c>
       <c r="P16" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
@@ -2562,7 +2562,7 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D17" t="s">
         <v>2</v>
@@ -2583,7 +2583,7 @@
         <v>2</v>
       </c>
       <c r="P17" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
@@ -2594,7 +2594,7 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D18" t="s">
         <v>5</v>
@@ -2618,7 +2618,7 @@
         <v>1</v>
       </c>
       <c r="P18" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
@@ -2629,13 +2629,13 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D19" t="s">
         <v>6</v>
       </c>
       <c r="E19" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F19" t="s">
         <v>188</v>
@@ -2667,7 +2667,7 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D20" t="s">
         <v>3</v>
@@ -2691,7 +2691,7 @@
         <v>1</v>
       </c>
       <c r="P20" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.3">
@@ -2702,13 +2702,13 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D21" t="s">
         <v>4</v>
       </c>
       <c r="E21" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F21" t="s">
         <v>188</v>
@@ -2726,7 +2726,7 @@
         <v>2</v>
       </c>
       <c r="P21" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
@@ -2737,7 +2737,7 @@
         <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D22" t="s">
         <v>6</v>
@@ -2772,7 +2772,7 @@
         <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D23" t="s">
         <v>6</v>
@@ -2804,7 +2804,7 @@
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D24" t="s">
         <v>6</v>
@@ -2839,7 +2839,7 @@
         <v>3</v>
       </c>
       <c r="C25" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D25" t="s">
         <v>6</v>
@@ -2874,7 +2874,7 @@
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D26" t="s">
         <v>6</v>
@@ -2906,7 +2906,7 @@
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D27" t="s">
         <v>6</v>
@@ -2938,7 +2938,7 @@
         <v>2</v>
       </c>
       <c r="C28" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D28" t="s">
         <v>4</v>
@@ -2953,7 +2953,7 @@
         <v>1</v>
       </c>
       <c r="P28" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
@@ -2964,7 +2964,7 @@
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D29" t="s">
         <v>5</v>
@@ -2982,7 +2982,7 @@
         <v>1</v>
       </c>
       <c r="P29" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
@@ -2993,7 +2993,7 @@
         <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D30" t="s">
         <v>4</v>
@@ -3008,7 +3008,7 @@
         <v>1</v>
       </c>
       <c r="P30" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
@@ -3019,7 +3019,7 @@
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D31" t="s">
         <v>4</v>
@@ -3046,7 +3046,7 @@
         <v>1</v>
       </c>
       <c r="P31" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
@@ -3057,7 +3057,7 @@
         <v>3</v>
       </c>
       <c r="C32" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D32" t="s">
         <v>2</v>
@@ -3078,7 +3078,7 @@
         <v>3</v>
       </c>
       <c r="P32" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.3">
@@ -3089,7 +3089,7 @@
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D33" t="s">
         <v>5</v>
@@ -3113,7 +3113,7 @@
         <v>1</v>
       </c>
       <c r="P33" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.3">
@@ -3124,7 +3124,7 @@
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D34" t="s">
         <v>5</v>
@@ -3148,7 +3148,7 @@
         <v>1</v>
       </c>
       <c r="P34" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.3">
@@ -3159,7 +3159,7 @@
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D35" t="s">
         <v>5</v>
@@ -3183,7 +3183,7 @@
         <v>1</v>
       </c>
       <c r="P35" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.3">
@@ -3194,7 +3194,7 @@
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D36" t="s">
         <v>7</v>
@@ -3212,7 +3212,7 @@
         <v>1</v>
       </c>
       <c r="P36" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.3">
@@ -3223,7 +3223,7 @@
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D37" t="s">
         <v>4</v>
@@ -3244,7 +3244,7 @@
         <v>2</v>
       </c>
       <c r="P37" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.3">
@@ -3255,7 +3255,7 @@
         <v>3</v>
       </c>
       <c r="C38" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D38" t="s">
         <v>4</v>
@@ -3270,7 +3270,7 @@
         <v>1</v>
       </c>
       <c r="P38" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.3">
@@ -3281,7 +3281,7 @@
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D39" t="s">
         <v>3</v>
@@ -3299,7 +3299,7 @@
         <v>1</v>
       </c>
       <c r="P39" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.3">
@@ -3310,7 +3310,7 @@
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D40" t="s">
         <v>2</v>
@@ -3328,7 +3328,7 @@
         <v>1</v>
       </c>
       <c r="P40" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.3">
@@ -3339,7 +3339,7 @@
         <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D41" t="s">
         <v>3</v>
@@ -3357,7 +3357,7 @@
         <v>1</v>
       </c>
       <c r="P41" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.3">
@@ -3368,7 +3368,7 @@
         <v>3</v>
       </c>
       <c r="C42" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D42" t="s">
         <v>3</v>
@@ -3392,7 +3392,7 @@
         <v>3</v>
       </c>
       <c r="P42" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.3">
@@ -3403,7 +3403,7 @@
         <v>1</v>
       </c>
       <c r="C43" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D43" t="s">
         <v>6</v>
@@ -3435,7 +3435,7 @@
         <v>1</v>
       </c>
       <c r="C44" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D44" t="s">
         <v>6</v>
@@ -3470,13 +3470,13 @@
         <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D45" t="s">
         <v>5</v>
       </c>
       <c r="E45" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F45" t="s">
         <v>188</v>
@@ -3488,7 +3488,7 @@
         <v>1</v>
       </c>
       <c r="P45" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.3">
@@ -3499,7 +3499,7 @@
         <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D46" t="s">
         <v>2</v>
@@ -3520,7 +3520,7 @@
         <v>1</v>
       </c>
       <c r="P46" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.3">
@@ -3531,7 +3531,7 @@
         <v>3</v>
       </c>
       <c r="C47" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D47" t="s">
         <v>3</v>
@@ -3552,7 +3552,7 @@
         <v>3</v>
       </c>
       <c r="P47" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.3">
@@ -3563,7 +3563,7 @@
         <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D48" t="s">
         <v>5</v>
@@ -3581,7 +3581,7 @@
         <v>1</v>
       </c>
       <c r="P48" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.3">
@@ -3592,13 +3592,13 @@
         <v>1</v>
       </c>
       <c r="C49" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D49" t="s">
         <v>3</v>
       </c>
       <c r="E49" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F49" t="s">
         <v>8</v>
@@ -3621,7 +3621,7 @@
         <v>3</v>
       </c>
       <c r="C50" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D50" t="s">
         <v>3</v>
@@ -3642,7 +3642,7 @@
         <v>3</v>
       </c>
       <c r="P50" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.3">
@@ -3653,7 +3653,7 @@
         <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D51" t="s">
         <v>4</v>
@@ -3671,7 +3671,7 @@
         <v>2</v>
       </c>
       <c r="P51" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.3">
@@ -3682,7 +3682,7 @@
         <v>1</v>
       </c>
       <c r="C52" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D52" t="s">
         <v>5</v>
@@ -3700,7 +3700,7 @@
         <v>1</v>
       </c>
       <c r="P52" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.3">
@@ -3711,13 +3711,13 @@
         <v>1</v>
       </c>
       <c r="C53" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D53" t="s">
         <v>6</v>
       </c>
       <c r="E53" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F53" t="s">
         <v>8</v>
@@ -3746,13 +3746,13 @@
         <v>1</v>
       </c>
       <c r="C54" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D54" t="s">
         <v>2</v>
       </c>
       <c r="E54" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F54" t="s">
         <v>188</v>
@@ -3764,7 +3764,7 @@
         <v>1</v>
       </c>
       <c r="P54" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.3">
@@ -3775,7 +3775,7 @@
         <v>2</v>
       </c>
       <c r="C55" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D55" t="s">
         <v>7</v>
@@ -3796,7 +3796,7 @@
         <v>2</v>
       </c>
       <c r="P55" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.3">
@@ -3807,7 +3807,7 @@
         <v>1</v>
       </c>
       <c r="C56" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D56" t="s">
         <v>5</v>
@@ -3825,7 +3825,7 @@
         <v>1</v>
       </c>
       <c r="P56" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.3">
@@ -3836,7 +3836,7 @@
         <v>1</v>
       </c>
       <c r="C57" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D57" t="s">
         <v>3</v>
@@ -3860,7 +3860,7 @@
         <v>1</v>
       </c>
       <c r="P57" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.3">
@@ -3871,7 +3871,7 @@
         <v>1</v>
       </c>
       <c r="C58" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D58" t="s">
         <v>5</v>
@@ -3889,7 +3889,7 @@
         <v>1</v>
       </c>
       <c r="P58" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.3">
@@ -3900,7 +3900,7 @@
         <v>1</v>
       </c>
       <c r="C59" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D59" t="s">
         <v>5</v>
@@ -3918,7 +3918,7 @@
         <v>1</v>
       </c>
       <c r="P59" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.3">
@@ -3929,7 +3929,7 @@
         <v>1</v>
       </c>
       <c r="C60" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D60" t="s">
         <v>5</v>
@@ -3947,7 +3947,7 @@
         <v>1</v>
       </c>
       <c r="P60" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.3">
@@ -3958,7 +3958,7 @@
         <v>1</v>
       </c>
       <c r="C61" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D61" t="s">
         <v>5</v>
@@ -3987,7 +3987,7 @@
         <v>1</v>
       </c>
       <c r="C62" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D62" t="s">
         <v>7</v>
@@ -4005,7 +4005,7 @@
         <v>1</v>
       </c>
       <c r="P62" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.3">
@@ -4016,7 +4016,7 @@
         <v>1</v>
       </c>
       <c r="C63" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D63" t="s">
         <v>5</v>
@@ -4034,7 +4034,7 @@
         <v>1</v>
       </c>
       <c r="P63" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.3">
@@ -4045,7 +4045,7 @@
         <v>1</v>
       </c>
       <c r="C64" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D64" t="s">
         <v>4</v>
@@ -4072,7 +4072,7 @@
         <v>1</v>
       </c>
       <c r="P64" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.3">
@@ -4083,7 +4083,7 @@
         <v>3</v>
       </c>
       <c r="C65" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D65" t="s">
         <v>4</v>
@@ -4107,7 +4107,7 @@
         <v>1</v>
       </c>
       <c r="P65" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.3">
@@ -4118,13 +4118,13 @@
         <v>1</v>
       </c>
       <c r="C66" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D66" t="s">
         <v>4</v>
       </c>
       <c r="E66" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F66" t="s">
         <v>188</v>
@@ -4142,7 +4142,7 @@
         <v>2</v>
       </c>
       <c r="P66" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.3">
@@ -4153,7 +4153,7 @@
         <v>3</v>
       </c>
       <c r="C67" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D67" t="s">
         <v>5</v>
@@ -4174,7 +4174,7 @@
         <v>3</v>
       </c>
       <c r="P67" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.3">
@@ -4185,7 +4185,7 @@
         <v>1</v>
       </c>
       <c r="C68" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D68" t="s">
         <v>5</v>
@@ -4203,7 +4203,7 @@
         <v>1</v>
       </c>
       <c r="P68" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.3">
@@ -4214,7 +4214,7 @@
         <v>1</v>
       </c>
       <c r="C69" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D69" t="s">
         <v>5</v>
@@ -4232,7 +4232,7 @@
         <v>1</v>
       </c>
       <c r="P69" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.3">
@@ -4243,7 +4243,7 @@
         <v>1</v>
       </c>
       <c r="C70" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D70" t="s">
         <v>5</v>
@@ -4267,7 +4267,7 @@
         <v>1</v>
       </c>
       <c r="P70" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.3">
@@ -4278,7 +4278,7 @@
         <v>3</v>
       </c>
       <c r="C71" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D71" t="s">
         <v>3</v>
@@ -4299,7 +4299,7 @@
         <v>3</v>
       </c>
       <c r="P71" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.3">
@@ -4310,7 +4310,7 @@
         <v>3</v>
       </c>
       <c r="C72" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D72" t="s">
         <v>3</v>
@@ -4331,7 +4331,7 @@
         <v>3</v>
       </c>
       <c r="P72" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.3">
@@ -4342,7 +4342,7 @@
         <v>1</v>
       </c>
       <c r="C73" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D73" t="s">
         <v>7</v>
@@ -4360,7 +4360,7 @@
         <v>1</v>
       </c>
       <c r="P73" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.3">
@@ -4377,7 +4377,7 @@
         <v>6</v>
       </c>
       <c r="E74" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F74" t="s">
         <v>188</v>
@@ -4403,13 +4403,13 @@
         <v>1</v>
       </c>
       <c r="C75" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D75" t="s">
         <v>6</v>
       </c>
       <c r="E75" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F75" t="s">
         <v>8</v>
@@ -4435,7 +4435,7 @@
         <v>1</v>
       </c>
       <c r="C76" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D76" t="s">
         <v>6</v>
@@ -4467,7 +4467,7 @@
         <v>1</v>
       </c>
       <c r="C77" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D77" t="s">
         <v>5</v>
@@ -4485,7 +4485,7 @@
         <v>1</v>
       </c>
       <c r="P77" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.3">
@@ -4496,7 +4496,7 @@
         <v>1</v>
       </c>
       <c r="C78" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D78" t="s">
         <v>3</v>
@@ -4514,7 +4514,7 @@
         <v>1</v>
       </c>
       <c r="P78" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.3">
@@ -4525,13 +4525,13 @@
         <v>1</v>
       </c>
       <c r="C79" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D79" t="s">
         <v>5</v>
       </c>
       <c r="E79" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F79" t="s">
         <v>188</v>
@@ -4543,7 +4543,7 @@
         <v>1</v>
       </c>
       <c r="P79" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="80" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -4554,7 +4554,7 @@
         <v>3</v>
       </c>
       <c r="C80" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D80" t="s">
         <v>4</v>
@@ -4572,7 +4572,7 @@
         <v>1</v>
       </c>
       <c r="P80" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.3">
@@ -4583,7 +4583,7 @@
         <v>4</v>
       </c>
       <c r="C81" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D81" t="s">
         <v>7</v>
@@ -4604,7 +4604,7 @@
         <v>4</v>
       </c>
       <c r="P81" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.3">
@@ -4615,13 +4615,13 @@
         <v>1</v>
       </c>
       <c r="C82" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D82" t="s">
         <v>3</v>
       </c>
       <c r="E82" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F82" t="s">
         <v>8</v>
@@ -4633,7 +4633,7 @@
         <v>1</v>
       </c>
       <c r="P82" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.3">
@@ -4644,13 +4644,13 @@
         <v>1</v>
       </c>
       <c r="C83" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D83" t="s">
         <v>3</v>
       </c>
       <c r="E83" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F83" t="s">
         <v>188</v>
@@ -4665,7 +4665,7 @@
         <v>1</v>
       </c>
       <c r="P83" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.3">
@@ -4676,13 +4676,13 @@
         <v>1</v>
       </c>
       <c r="C84" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D84" t="s">
         <v>2</v>
       </c>
       <c r="E84" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F84" t="s">
         <v>188</v>
@@ -4694,7 +4694,7 @@
         <v>1</v>
       </c>
       <c r="P84" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.3">
@@ -4705,7 +4705,7 @@
         <v>1</v>
       </c>
       <c r="C85" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D85" t="s">
         <v>2</v>
@@ -4737,13 +4737,13 @@
         <v>1</v>
       </c>
       <c r="C86" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D86" t="s">
         <v>6</v>
       </c>
       <c r="E86" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F86" t="s">
         <v>188</v>
@@ -4775,13 +4775,13 @@
         <v>1</v>
       </c>
       <c r="C87" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D87" t="s">
         <v>5</v>
       </c>
       <c r="E87" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F87" t="s">
         <v>188</v>
@@ -4802,7 +4802,7 @@
         <v>1</v>
       </c>
       <c r="P87" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="88" spans="1:16" x14ac:dyDescent="0.3">
@@ -4813,7 +4813,7 @@
         <v>1</v>
       </c>
       <c r="C88" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D88" t="s">
         <v>2</v>
@@ -4831,7 +4831,7 @@
         <v>1</v>
       </c>
       <c r="P88" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.3">
@@ -4842,13 +4842,13 @@
         <v>1</v>
       </c>
       <c r="C89" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D89" t="s">
         <v>5</v>
       </c>
       <c r="E89" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F89" t="s">
         <v>8</v>
@@ -4860,7 +4860,7 @@
         <v>1</v>
       </c>
       <c r="P89" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.3">
@@ -4871,13 +4871,13 @@
         <v>1</v>
       </c>
       <c r="C90" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D90" t="s">
         <v>7</v>
       </c>
       <c r="E90" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F90" t="s">
         <v>188</v>
@@ -4889,7 +4889,7 @@
         <v>1</v>
       </c>
       <c r="P90" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.3">
@@ -4900,7 +4900,7 @@
         <v>3</v>
       </c>
       <c r="C91" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D91" t="s">
         <v>6</v>
@@ -4935,7 +4935,7 @@
         <v>1</v>
       </c>
       <c r="C92" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D92" t="s">
         <v>6</v>
@@ -4967,7 +4967,7 @@
         <v>5</v>
       </c>
       <c r="C93" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D93" t="s">
         <v>3</v>
@@ -4985,7 +4985,7 @@
         <v>5</v>
       </c>
       <c r="P93" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.3">
@@ -4996,7 +4996,7 @@
         <v>3</v>
       </c>
       <c r="C94" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D94" t="s">
         <v>6</v>
@@ -5025,13 +5025,13 @@
         <v>1</v>
       </c>
       <c r="C95" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D95" t="s">
         <v>7</v>
       </c>
       <c r="E95" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F95" t="s">
         <v>188</v>
@@ -5046,7 +5046,7 @@
         <v>1</v>
       </c>
       <c r="P95" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.3">
@@ -5057,7 +5057,7 @@
         <v>1</v>
       </c>
       <c r="C96" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D96" t="s">
         <v>3</v>
@@ -5078,7 +5078,7 @@
         <v>1</v>
       </c>
       <c r="P96" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.3">
@@ -5089,7 +5089,7 @@
         <v>1</v>
       </c>
       <c r="C97" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D97" t="s">
         <v>7</v>
@@ -5107,7 +5107,7 @@
         <v>1</v>
       </c>
       <c r="P97" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="98" spans="1:16" x14ac:dyDescent="0.3">
@@ -5118,13 +5118,13 @@
         <v>1</v>
       </c>
       <c r="C98" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D98" t="s">
         <v>7</v>
       </c>
       <c r="E98" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F98" t="s">
         <v>9</v>
@@ -5136,7 +5136,7 @@
         <v>1</v>
       </c>
       <c r="P98" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="99" spans="1:16" x14ac:dyDescent="0.3">
@@ -5147,13 +5147,13 @@
         <v>1</v>
       </c>
       <c r="C99" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D99" t="s">
         <v>4</v>
       </c>
       <c r="E99" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F99" t="s">
         <v>188</v>
@@ -5168,7 +5168,7 @@
         <v>2</v>
       </c>
       <c r="P99" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="100" spans="1:16" x14ac:dyDescent="0.3">
@@ -5179,7 +5179,7 @@
         <v>3</v>
       </c>
       <c r="C100" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D100" t="s">
         <v>7</v>
@@ -5197,7 +5197,7 @@
         <v>3</v>
       </c>
       <c r="P100" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="101" spans="1:16" x14ac:dyDescent="0.3">
@@ -5208,7 +5208,7 @@
         <v>3</v>
       </c>
       <c r="C101" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D101" t="s">
         <v>5</v>
@@ -5229,7 +5229,7 @@
         <v>3</v>
       </c>
       <c r="P101" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="102" spans="1:16" x14ac:dyDescent="0.3">
@@ -5240,7 +5240,7 @@
         <v>1</v>
       </c>
       <c r="C102" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D102" t="s">
         <v>6</v>
@@ -5281,7 +5281,7 @@
         <v>1</v>
       </c>
       <c r="C103" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D103" t="s">
         <v>4</v>
@@ -5311,7 +5311,7 @@
         <v>1</v>
       </c>
       <c r="P103" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="104" spans="1:16" x14ac:dyDescent="0.3">
@@ -5322,13 +5322,13 @@
         <v>1</v>
       </c>
       <c r="C104" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D104" t="s">
         <v>2</v>
       </c>
       <c r="E104" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F104" t="s">
         <v>8</v>
@@ -5340,7 +5340,7 @@
         <v>1</v>
       </c>
       <c r="P104" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="105" spans="1:16" x14ac:dyDescent="0.3">
@@ -5351,7 +5351,7 @@
         <v>1</v>
       </c>
       <c r="C105" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D105" t="s">
         <v>5</v>
@@ -5369,7 +5369,7 @@
         <v>1</v>
       </c>
       <c r="P105" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.3">
@@ -5380,7 +5380,7 @@
         <v>3</v>
       </c>
       <c r="C106" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D106" t="s">
         <v>2</v>
@@ -5401,7 +5401,7 @@
         <v>3</v>
       </c>
       <c r="P106" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.3">
@@ -5412,7 +5412,7 @@
         <v>1</v>
       </c>
       <c r="C107" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D107" t="s">
         <v>2</v>
@@ -5433,7 +5433,7 @@
         <v>1</v>
       </c>
       <c r="P107" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="108" spans="1:16" x14ac:dyDescent="0.3">
@@ -5444,7 +5444,7 @@
         <v>1</v>
       </c>
       <c r="C108" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D108" t="s">
         <v>7</v>
@@ -5462,7 +5462,7 @@
         <v>1</v>
       </c>
       <c r="P108" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="109" spans="1:16" x14ac:dyDescent="0.3">
@@ -5473,7 +5473,7 @@
         <v>1</v>
       </c>
       <c r="C109" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D109" t="s">
         <v>7</v>
@@ -5491,7 +5491,7 @@
         <v>1</v>
       </c>
       <c r="P109" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="110" spans="1:16" x14ac:dyDescent="0.3">
@@ -5502,7 +5502,7 @@
         <v>2</v>
       </c>
       <c r="C110" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D110" t="s">
         <v>2</v>
@@ -5520,7 +5520,7 @@
         <v>2</v>
       </c>
       <c r="P110" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.3">
@@ -5531,7 +5531,7 @@
         <v>1</v>
       </c>
       <c r="C111" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D111" t="s">
         <v>7</v>
@@ -5549,7 +5549,7 @@
         <v>1</v>
       </c>
       <c r="P111" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.3">
@@ -5560,7 +5560,7 @@
         <v>1</v>
       </c>
       <c r="C112" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D112" t="s">
         <v>3</v>
@@ -5578,7 +5578,7 @@
         <v>1</v>
       </c>
       <c r="P112" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="113" spans="1:16" x14ac:dyDescent="0.3">
@@ -5589,7 +5589,7 @@
         <v>1</v>
       </c>
       <c r="C113" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D113" t="s">
         <v>4</v>
@@ -5610,7 +5610,7 @@
         <v>1</v>
       </c>
       <c r="P113" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="114" spans="1:16" x14ac:dyDescent="0.3">
@@ -5621,7 +5621,7 @@
         <v>1</v>
       </c>
       <c r="C114" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D114" t="s">
         <v>7</v>
@@ -5639,7 +5639,7 @@
         <v>1</v>
       </c>
       <c r="P114" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="115" spans="1:16" x14ac:dyDescent="0.3">
@@ -5650,7 +5650,7 @@
         <v>1</v>
       </c>
       <c r="C115" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D115" t="s">
         <v>2</v>
@@ -5668,7 +5668,7 @@
         <v>1</v>
       </c>
       <c r="P115" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="116" spans="1:16" x14ac:dyDescent="0.3">
@@ -5679,13 +5679,13 @@
         <v>1</v>
       </c>
       <c r="C116" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D116" t="s">
         <v>3</v>
       </c>
       <c r="E116" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F116" t="s">
         <v>8</v>
@@ -5708,7 +5708,7 @@
         <v>1</v>
       </c>
       <c r="C117" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D117" t="s">
         <v>3</v>
@@ -5749,7 +5749,7 @@
         <v>3</v>
       </c>
       <c r="C118" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D118" t="s">
         <v>4</v>
@@ -5764,7 +5764,7 @@
         <v>1</v>
       </c>
       <c r="P118" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="119" spans="1:16" x14ac:dyDescent="0.3">
@@ -5775,7 +5775,7 @@
         <v>1</v>
       </c>
       <c r="C119" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D119" t="s">
         <v>2</v>
@@ -5793,7 +5793,7 @@
         <v>1</v>
       </c>
       <c r="P119" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="120" spans="1:16" x14ac:dyDescent="0.3">
@@ -5804,7 +5804,7 @@
         <v>1</v>
       </c>
       <c r="C120" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D120" t="s">
         <v>7</v>
@@ -5825,7 +5825,7 @@
         <v>1</v>
       </c>
       <c r="P120" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="121" spans="1:16" x14ac:dyDescent="0.3">
@@ -5836,7 +5836,7 @@
         <v>1</v>
       </c>
       <c r="C121" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D121" t="s">
         <v>7</v>
@@ -5854,7 +5854,7 @@
         <v>1</v>
       </c>
       <c r="P121" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="122" spans="1:16" x14ac:dyDescent="0.3">
@@ -5865,7 +5865,7 @@
         <v>1</v>
       </c>
       <c r="C122" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D122" t="s">
         <v>7</v>
@@ -5886,7 +5886,7 @@
         <v>1</v>
       </c>
       <c r="P122" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="123" spans="1:16" x14ac:dyDescent="0.3">
@@ -5897,7 +5897,7 @@
         <v>1</v>
       </c>
       <c r="C123" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D123" t="s">
         <v>2</v>
@@ -5926,7 +5926,7 @@
         <v>1</v>
       </c>
       <c r="C124" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D124" t="s">
         <v>2</v>
@@ -5944,7 +5944,7 @@
         <v>1</v>
       </c>
       <c r="P124" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="125" spans="1:16" x14ac:dyDescent="0.3">
@@ -5955,7 +5955,7 @@
         <v>1</v>
       </c>
       <c r="C125" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D125" t="s">
         <v>2</v>
@@ -5976,7 +5976,7 @@
         <v>1</v>
       </c>
       <c r="P125" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="126" spans="1:16" x14ac:dyDescent="0.3">
@@ -5987,7 +5987,7 @@
         <v>1</v>
       </c>
       <c r="C126" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D126" t="s">
         <v>2</v>
@@ -6005,7 +6005,7 @@
         <v>1</v>
       </c>
       <c r="P126" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="127" spans="1:16" x14ac:dyDescent="0.3">
@@ -6016,7 +6016,7 @@
         <v>3</v>
       </c>
       <c r="C127" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D127" t="s">
         <v>4</v>
@@ -6040,7 +6040,7 @@
         <v>1</v>
       </c>
       <c r="P127" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="128" spans="1:16" x14ac:dyDescent="0.3">
@@ -6051,7 +6051,7 @@
         <v>1</v>
       </c>
       <c r="C128" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D128" t="s">
         <v>7</v>
@@ -6072,7 +6072,7 @@
         <v>1</v>
       </c>
       <c r="P128" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="129" spans="1:16" x14ac:dyDescent="0.3">
@@ -6083,7 +6083,7 @@
         <v>1</v>
       </c>
       <c r="C129" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D129" t="s">
         <v>6</v>
@@ -6115,7 +6115,7 @@
         <v>1</v>
       </c>
       <c r="C130" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D130" t="s">
         <v>7</v>
@@ -6133,7 +6133,7 @@
         <v>1</v>
       </c>
       <c r="P130" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="131" spans="1:16" x14ac:dyDescent="0.3">
@@ -6144,7 +6144,7 @@
         <v>1</v>
       </c>
       <c r="C131" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D131" t="s">
         <v>2</v>
@@ -6165,7 +6165,7 @@
         <v>1</v>
       </c>
       <c r="P131" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="132" spans="1:16" x14ac:dyDescent="0.3">
@@ -6176,13 +6176,13 @@
         <v>1</v>
       </c>
       <c r="C132" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D132" t="s">
         <v>7</v>
       </c>
       <c r="E132" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F132" t="s">
         <v>8</v>
@@ -6194,7 +6194,7 @@
         <v>1</v>
       </c>
       <c r="P132" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="133" spans="1:16" x14ac:dyDescent="0.3">
@@ -6205,7 +6205,7 @@
         <v>1</v>
       </c>
       <c r="C133" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D133" t="s">
         <v>5</v>
@@ -6235,7 +6235,7 @@
         <v>1</v>
       </c>
       <c r="P133" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="134" spans="1:16" x14ac:dyDescent="0.3">
@@ -6246,7 +6246,7 @@
         <v>2</v>
       </c>
       <c r="C134" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D134" t="s">
         <v>4</v>
@@ -6264,7 +6264,7 @@
         <v>1</v>
       </c>
       <c r="P134" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="135" spans="1:16" x14ac:dyDescent="0.3">
@@ -6275,7 +6275,7 @@
         <v>1</v>
       </c>
       <c r="C135" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D135" t="s">
         <v>3</v>
@@ -6293,7 +6293,7 @@
         <v>1</v>
       </c>
       <c r="P135" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="136" spans="1:16" x14ac:dyDescent="0.3">
@@ -6328,7 +6328,7 @@
         <v>1</v>
       </c>
       <c r="P136" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="137" spans="1:16" x14ac:dyDescent="0.3">
@@ -6363,7 +6363,7 @@
         <v>1</v>
       </c>
       <c r="P137" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="138" spans="1:16" x14ac:dyDescent="0.3">
@@ -6374,7 +6374,7 @@
         <v>2</v>
       </c>
       <c r="C138" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D138" t="s">
         <v>2</v>
@@ -6392,7 +6392,7 @@
         <v>2</v>
       </c>
       <c r="P138" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="139" spans="1:16" x14ac:dyDescent="0.3">
@@ -6403,13 +6403,13 @@
         <v>1</v>
       </c>
       <c r="C139" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D139" t="s">
         <v>4</v>
       </c>
       <c r="E139" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F139" t="s">
         <v>188</v>
@@ -6421,7 +6421,7 @@
         <v>2</v>
       </c>
       <c r="P139" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="140" spans="1:16" x14ac:dyDescent="0.3">
@@ -6432,7 +6432,7 @@
         <v>1</v>
       </c>
       <c r="C140" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D140" t="s">
         <v>6</v>
@@ -6464,7 +6464,7 @@
         <v>1</v>
       </c>
       <c r="C141" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D141" t="s">
         <v>5</v>
@@ -6482,13 +6482,13 @@
         <v>15</v>
       </c>
       <c r="N141" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="O141">
         <v>1</v>
       </c>
       <c r="P141" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="142" spans="1:16" x14ac:dyDescent="0.3">
@@ -6499,7 +6499,7 @@
         <v>1</v>
       </c>
       <c r="C142" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D142" t="s">
         <v>5</v>
@@ -6517,13 +6517,13 @@
         <v>15</v>
       </c>
       <c r="N142" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="O142">
         <v>1</v>
       </c>
       <c r="P142" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="143" spans="1:16" x14ac:dyDescent="0.3">
@@ -6534,7 +6534,7 @@
         <v>1</v>
       </c>
       <c r="C143" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D143" t="s">
         <v>5</v>
@@ -6552,13 +6552,13 @@
         <v>15</v>
       </c>
       <c r="N143" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="O143">
         <v>1</v>
       </c>
       <c r="P143" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="144" spans="1:16" x14ac:dyDescent="0.3">
@@ -6569,7 +6569,7 @@
         <v>1</v>
       </c>
       <c r="C144" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D144" t="s">
         <v>5</v>
@@ -6587,13 +6587,13 @@
         <v>15</v>
       </c>
       <c r="N144" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="O144">
         <v>1</v>
       </c>
       <c r="P144" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="145" spans="1:16" x14ac:dyDescent="0.3">
@@ -6604,7 +6604,7 @@
         <v>1</v>
       </c>
       <c r="C145" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D145" t="s">
         <v>5</v>
@@ -6622,13 +6622,13 @@
         <v>15</v>
       </c>
       <c r="N145" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="O145">
         <v>1</v>
       </c>
       <c r="P145" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="146" spans="1:16" x14ac:dyDescent="0.3">
@@ -6639,7 +6639,7 @@
         <v>1</v>
       </c>
       <c r="C146" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D146" t="s">
         <v>7</v>
@@ -6657,7 +6657,7 @@
         <v>1</v>
       </c>
       <c r="P146" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="147" spans="1:16" x14ac:dyDescent="0.3">
@@ -6668,7 +6668,7 @@
         <v>1</v>
       </c>
       <c r="C147" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D147" t="s">
         <v>7</v>
@@ -6689,7 +6689,7 @@
         <v>1</v>
       </c>
       <c r="P147" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="148" spans="1:16" x14ac:dyDescent="0.3">
@@ -6700,13 +6700,13 @@
         <v>1</v>
       </c>
       <c r="C148" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D148" t="s">
         <v>2</v>
       </c>
       <c r="E148" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F148" t="s">
         <v>188</v>
@@ -6718,7 +6718,7 @@
         <v>1</v>
       </c>
       <c r="P148" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="149" spans="1:16" x14ac:dyDescent="0.3">
@@ -6729,7 +6729,7 @@
         <v>1</v>
       </c>
       <c r="C149" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D149" t="s">
         <v>2</v>
@@ -6747,7 +6747,7 @@
         <v>1</v>
       </c>
       <c r="P149" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="150" spans="1:16" x14ac:dyDescent="0.3">
@@ -6758,7 +6758,7 @@
         <v>1</v>
       </c>
       <c r="C150" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D150" t="s">
         <v>4</v>
@@ -6776,7 +6776,7 @@
         <v>2</v>
       </c>
       <c r="P150" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="151" spans="1:16" x14ac:dyDescent="0.3">
@@ -6787,7 +6787,7 @@
         <v>1</v>
       </c>
       <c r="C151" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D151" t="s">
         <v>4</v>
@@ -6814,7 +6814,7 @@
         <v>2</v>
       </c>
       <c r="P151" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="152" spans="1:16" x14ac:dyDescent="0.3">
@@ -6825,7 +6825,7 @@
         <v>1</v>
       </c>
       <c r="C152" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D152" t="s">
         <v>7</v>
@@ -6843,7 +6843,7 @@
         <v>1</v>
       </c>
       <c r="P152" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="153" spans="1:16" x14ac:dyDescent="0.3">
@@ -6854,7 +6854,7 @@
         <v>1</v>
       </c>
       <c r="C153" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D153" t="s">
         <v>3</v>
@@ -6883,7 +6883,7 @@
         <v>2</v>
       </c>
       <c r="C154" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D154" t="s">
         <v>3</v>
@@ -6918,7 +6918,7 @@
         <v>3</v>
       </c>
       <c r="C155" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D155" t="s">
         <v>6</v>
@@ -6953,7 +6953,7 @@
         <v>1</v>
       </c>
       <c r="C156" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D156" t="s">
         <v>5</v>
@@ -6971,7 +6971,7 @@
         <v>1</v>
       </c>
       <c r="P156" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="157" spans="1:16" x14ac:dyDescent="0.3">
@@ -6982,7 +6982,7 @@
         <v>1</v>
       </c>
       <c r="C157" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D157" t="s">
         <v>5</v>
@@ -7000,7 +7000,7 @@
         <v>1</v>
       </c>
       <c r="P157" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="158" spans="1:16" x14ac:dyDescent="0.3">
@@ -7011,7 +7011,7 @@
         <v>1</v>
       </c>
       <c r="C158" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D158" t="s">
         <v>3</v>
@@ -7035,7 +7035,7 @@
         <v>1</v>
       </c>
       <c r="P158" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="159" spans="1:16" x14ac:dyDescent="0.3">
@@ -7046,7 +7046,7 @@
         <v>1</v>
       </c>
       <c r="C159" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D159" t="s">
         <v>2</v>
@@ -7064,7 +7064,7 @@
         <v>1</v>
       </c>
       <c r="P159" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="160" spans="1:16" x14ac:dyDescent="0.3">
@@ -7075,13 +7075,13 @@
         <v>1</v>
       </c>
       <c r="C160" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D160" t="s">
         <v>4</v>
       </c>
       <c r="E160" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F160" t="s">
         <v>8</v>
@@ -7096,7 +7096,7 @@
         <v>2</v>
       </c>
       <c r="P160" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="161" spans="1:16" x14ac:dyDescent="0.3">
@@ -7107,7 +7107,7 @@
         <v>3</v>
       </c>
       <c r="C161" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D161" t="s">
         <v>6</v>
@@ -7142,7 +7142,7 @@
         <v>2</v>
       </c>
       <c r="C162" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D162" t="s">
         <v>7</v>
@@ -7163,7 +7163,7 @@
         <v>2</v>
       </c>
       <c r="P162" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="163" spans="1:16" x14ac:dyDescent="0.3">
@@ -7174,7 +7174,7 @@
         <v>1</v>
       </c>
       <c r="C163" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D163" t="s">
         <v>7</v>
@@ -7192,7 +7192,7 @@
         <v>1</v>
       </c>
       <c r="P163" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="164" spans="1:16" x14ac:dyDescent="0.3">
@@ -7203,7 +7203,7 @@
         <v>1</v>
       </c>
       <c r="C164" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D164" t="s">
         <v>4</v>
@@ -7221,7 +7221,7 @@
         <v>2</v>
       </c>
       <c r="P164" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
   </sheetData>
@@ -7277,7 +7277,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1260A867-074C-49A3-ACE9-5EA609B6D64C}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -7321,7 +7321,7 @@
         <v>223</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -7335,7 +7335,7 @@
         <v>215</v>
       </c>
       <c r="E3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -7350,7 +7350,7 @@
         <v>214</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -7367,7 +7367,7 @@
         <v>213</v>
       </c>
       <c r="E5" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -7382,7 +7382,7 @@
         <v>216</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -7396,7 +7396,7 @@
         <v>217</v>
       </c>
       <c r="E7" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -7413,7 +7413,7 @@
         <v>208</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -7427,7 +7427,7 @@
         <v>209</v>
       </c>
       <c r="E9" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -7442,7 +7442,7 @@
         <v>210</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -7456,7 +7456,7 @@
         <v>211</v>
       </c>
       <c r="E11" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -7471,7 +7471,7 @@
         <v>212</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -7485,7 +7485,7 @@
         <v>202</v>
       </c>
       <c r="E13" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -7500,7 +7500,7 @@
         <v>203</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -7517,7 +7517,7 @@
         <v>205</v>
       </c>
       <c r="E15" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -7532,7 +7532,7 @@
         <v>206</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -7546,7 +7546,7 @@
         <v>207</v>
       </c>
       <c r="E17" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -7561,7 +7561,7 @@
         <v>218</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -7578,7 +7578,7 @@
         <v>219</v>
       </c>
       <c r="E19" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -7593,7 +7593,7 @@
         <v>220</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -7607,7 +7607,7 @@
         <v>221</v>
       </c>
       <c r="E21" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -7622,7 +7622,7 @@
         <v>222</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -7639,7 +7639,7 @@
         <v>224</v>
       </c>
       <c r="E23" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
   </sheetData>
@@ -7766,8 +7766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12EC3BE3-3155-4E03-977A-4E9FD38F6559}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7789,7 +7789,7 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -7885,7 +7885,7 @@
         <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>296</v>
+        <v>452</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Explicit combats for Mardroeme, Commander's Horn and Decoy
</commit_message>
<xml_diff>
--- a/cards.xlsx
+++ b/cards.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\witcher-3-gwent-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9217A5B-3BFF-4E94-A253-9597E108B877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DAA4AD4-66F4-4A2A-AF2B-8340981BF7C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{C7211A38-802B-4C9D-8105-50DCB0156070}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1296" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1306" uniqueCount="454">
   <si>
     <t>Name</t>
   </si>
@@ -1399,13 +1399,16 @@
   </si>
   <si>
     <t>"I know how to carry out orders, so you can shove your advice up your coal chute."</t>
+  </si>
+  <si>
+    <t>Combat 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1417,6 +1420,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1646,12 +1655,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{60D01DD4-478E-4205-AEF9-F85464A53457}" name="Table2" displayName="Table2" ref="A1:P164" totalsRowShown="0" headerRowDxfId="10">
-  <autoFilter ref="A1:P164" xr:uid="{60D01DD4-478E-4205-AEF9-F85464A53457}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P164">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{60D01DD4-478E-4205-AEF9-F85464A53457}" name="Table2" displayName="Table2" ref="A1:Q164" totalsRowShown="0" headerRowDxfId="10">
+  <autoFilter ref="A1:Q164" xr:uid="{60D01DD4-478E-4205-AEF9-F85464A53457}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q164">
     <sortCondition ref="A1:A164"/>
   </sortState>
-  <tableColumns count="16">
+  <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{4610AC45-9F14-4FA0-AE17-310E1E3CEC88}" name="Name"/>
     <tableColumn id="2" xr3:uid="{3B3D3B39-7AE0-4A02-B928-703B22442C21}" name="Occurrences"/>
     <tableColumn id="17" xr3:uid="{58E805EF-E13B-488C-87D7-D1146695AF67}" name="Deckable"/>
@@ -1659,6 +1668,7 @@
     <tableColumn id="4" xr3:uid="{74F0380B-2395-4E96-9FD4-93049335AEE6}" name="Hero"/>
     <tableColumn id="5" xr3:uid="{D576723E-9131-4B41-AACC-B022C1A9059C}" name="Combat 1"/>
     <tableColumn id="14" xr3:uid="{231A8EEE-585D-4A80-94CA-F1FD152BB935}" name="Combat 2"/>
+    <tableColumn id="12" xr3:uid="{D949BC4F-7051-4524-B9AE-BE68DFD2A867}" name="Combat 3"/>
     <tableColumn id="6" xr3:uid="{91A0398F-EE19-4491-9FF2-C70C0DE8AC49}" name="Strength" dataDxfId="9"/>
     <tableColumn id="7" xr3:uid="{E24C035D-28B7-4376-A3BB-3BD4E59C185D}" name="Effect 1"/>
     <tableColumn id="13" xr3:uid="{FCF50C5C-BA9B-4B4D-B3EC-4BFF08A95686}" name="Effect 2"/>
@@ -2007,11 +2017,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D89E336D-773D-4B6A-9CD9-D024F295501B}">
-  <dimension ref="A1:P164"/>
+  <dimension ref="A1:Q164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P40" sqref="P40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2022,18 +2032,19 @@
     <col min="4" max="4" width="17.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="71.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" customWidth="1"/>
+    <col min="9" max="9" width="10.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="71.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2056,34 +2067,37 @@
         <v>199</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>1</v>
+        <v>453</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -2102,17 +2116,17 @@
       <c r="F2" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="2">
+      <c r="I2" s="2">
         <v>2</v>
       </c>
-      <c r="O2">
-        <v>1</v>
-      </c>
-      <c r="P2" t="s">
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>104</v>
       </c>
@@ -2131,20 +2145,20 @@
       <c r="F3" t="s">
         <v>188</v>
       </c>
-      <c r="H3" s="2">
+      <c r="I3" s="2">
         <v>4</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>15</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>3</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>105</v>
       </c>
@@ -2163,23 +2177,23 @@
       <c r="F4" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="2">
+      <c r="I4" s="2">
         <v>6</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>15</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>104</v>
       </c>
-      <c r="O4">
-        <v>1</v>
-      </c>
-      <c r="P4" t="s">
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -2198,17 +2212,17 @@
       <c r="F5" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="2">
+      <c r="I5" s="2">
         <v>6</v>
       </c>
-      <c r="O5">
-        <v>1</v>
-      </c>
-      <c r="P5" t="s">
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -2227,17 +2241,17 @@
       <c r="F6" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="2">
+      <c r="I6" s="2">
         <v>6</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>2</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>79</v>
       </c>
@@ -2259,20 +2273,20 @@
       <c r="G7" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="2">
+      <c r="I7" s="2">
         <v>6</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>12</v>
       </c>
-      <c r="O7">
-        <v>1</v>
-      </c>
-      <c r="P7" t="s">
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>159</v>
       </c>
@@ -2291,23 +2305,23 @@
       <c r="F8" t="s">
         <v>188</v>
       </c>
-      <c r="H8" s="2">
+      <c r="I8" s="2">
         <v>4</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>159</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>184</v>
       </c>
-      <c r="O8">
-        <v>1</v>
-      </c>
-      <c r="P8" t="s">
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Q8" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>160</v>
       </c>
@@ -2326,23 +2340,23 @@
       <c r="F9" t="s">
         <v>188</v>
       </c>
-      <c r="H9" s="2">
+      <c r="I9" s="2">
         <v>2</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>13</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>184</v>
       </c>
-      <c r="O9">
-        <v>1</v>
-      </c>
-      <c r="P9" t="s">
+      <c r="P9">
+        <v>1</v>
+      </c>
+      <c r="Q9" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>136</v>
       </c>
@@ -2361,17 +2375,17 @@
       <c r="F10" t="s">
         <v>188</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>23</v>
       </c>
-      <c r="O10">
-        <v>1</v>
-      </c>
-      <c r="P10" t="s">
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="Q10" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>54</v>
       </c>
@@ -2390,17 +2404,17 @@
       <c r="F11" t="s">
         <v>8</v>
       </c>
-      <c r="H11" s="2">
+      <c r="I11" s="2">
         <v>10</v>
       </c>
-      <c r="O11">
+      <c r="P11">
         <v>2</v>
       </c>
-      <c r="P11" t="s">
+      <c r="Q11" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -2419,20 +2433,20 @@
       <c r="F12" t="s">
         <v>188</v>
       </c>
-      <c r="H12" s="2">
+      <c r="I12" s="2">
         <v>4</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>17</v>
       </c>
-      <c r="O12">
+      <c r="P12">
         <v>3</v>
       </c>
-      <c r="P12" t="s">
+      <c r="Q12" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>161</v>
       </c>
@@ -2451,20 +2465,20 @@
       <c r="F13" t="s">
         <v>188</v>
       </c>
-      <c r="H13" s="2">
+      <c r="I13" s="2">
         <v>6</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>184</v>
       </c>
-      <c r="O13">
-        <v>1</v>
-      </c>
-      <c r="P13" t="s">
+      <c r="P13">
+        <v>1</v>
+      </c>
+      <c r="Q13" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>106</v>
       </c>
@@ -2483,17 +2497,17 @@
       <c r="F14" t="s">
         <v>188</v>
       </c>
-      <c r="H14" s="2">
+      <c r="I14" s="2">
         <v>4</v>
       </c>
-      <c r="O14">
-        <v>1</v>
-      </c>
-      <c r="P14" t="s">
+      <c r="P14">
+        <v>1</v>
+      </c>
+      <c r="Q14" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>236</v>
       </c>
@@ -2512,20 +2526,20 @@
       <c r="F15" t="s">
         <v>188</v>
       </c>
-      <c r="H15" s="2">
+      <c r="I15" s="2">
         <v>8</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>183</v>
       </c>
-      <c r="O15">
-        <v>1</v>
-      </c>
-      <c r="P15" t="s">
+      <c r="P15">
+        <v>1</v>
+      </c>
+      <c r="Q15" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>242</v>
       </c>
@@ -2544,17 +2558,17 @@
       <c r="F16" t="s">
         <v>188</v>
       </c>
-      <c r="H16" s="2">
+      <c r="I16" s="2">
         <v>6</v>
       </c>
-      <c r="O16">
-        <v>1</v>
-      </c>
-      <c r="P16" t="s">
+      <c r="P16">
+        <v>1</v>
+      </c>
+      <c r="Q16" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -2573,20 +2587,20 @@
       <c r="F17" t="s">
         <v>9</v>
       </c>
-      <c r="H17" s="2">
+      <c r="I17" s="2">
         <v>8</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>17</v>
       </c>
-      <c r="O17">
+      <c r="P17">
         <v>2</v>
       </c>
-      <c r="P17" t="s">
+      <c r="Q17" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>239</v>
       </c>
@@ -2608,20 +2622,20 @@
       <c r="G18" t="s">
         <v>8</v>
       </c>
-      <c r="H18" s="2">
+      <c r="I18" s="2">
         <v>2</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>12</v>
       </c>
-      <c r="O18">
-        <v>1</v>
-      </c>
-      <c r="P18" t="s">
+      <c r="P18">
+        <v>1</v>
+      </c>
+      <c r="Q18" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>162</v>
       </c>
@@ -2640,26 +2654,26 @@
       <c r="F19" t="s">
         <v>188</v>
       </c>
-      <c r="H19" s="2">
+      <c r="I19" s="2">
         <v>10</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>15</v>
       </c>
-      <c r="K19" t="s">
+      <c r="L19" t="s">
         <v>184</v>
       </c>
-      <c r="N19" t="s">
+      <c r="O19" t="s">
         <v>165</v>
       </c>
-      <c r="O19">
-        <v>1</v>
-      </c>
-      <c r="P19" t="s">
+      <c r="P19">
+        <v>1</v>
+      </c>
+      <c r="Q19" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>80</v>
       </c>
@@ -2681,20 +2695,20 @@
       <c r="G20" t="s">
         <v>8</v>
       </c>
-      <c r="H20" s="2">
+      <c r="I20" s="2">
         <v>3</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
         <v>12</v>
       </c>
-      <c r="O20">
-        <v>1</v>
-      </c>
-      <c r="P20" t="s">
+      <c r="P20">
+        <v>1</v>
+      </c>
+      <c r="Q20" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>240</v>
       </c>
@@ -2713,23 +2727,23 @@
       <c r="F21" t="s">
         <v>188</v>
       </c>
-      <c r="H21" s="2">
+      <c r="I21" s="2">
         <v>15</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>15</v>
       </c>
-      <c r="N21" t="s">
+      <c r="O21" t="s">
         <v>189</v>
       </c>
-      <c r="O21">
+      <c r="P21">
         <v>2</v>
       </c>
-      <c r="P21" t="s">
+      <c r="Q21" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>163</v>
       </c>
@@ -2748,23 +2762,23 @@
       <c r="F22" t="s">
         <v>188</v>
       </c>
-      <c r="H22" s="2">
+      <c r="I22" s="2">
         <v>6</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
         <v>17</v>
       </c>
-      <c r="K22" t="s">
+      <c r="L22" t="s">
         <v>184</v>
       </c>
-      <c r="O22">
-        <v>1</v>
-      </c>
-      <c r="P22" t="s">
+      <c r="P22">
+        <v>1</v>
+      </c>
+      <c r="Q22" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>164</v>
       </c>
@@ -2783,20 +2797,20 @@
       <c r="F23" t="s">
         <v>8</v>
       </c>
-      <c r="H23" s="2">
+      <c r="I23" s="2">
         <v>6</v>
       </c>
-      <c r="K23" t="s">
+      <c r="L23" t="s">
         <v>184</v>
       </c>
-      <c r="O23">
-        <v>1</v>
-      </c>
-      <c r="P23" t="s">
+      <c r="P23">
+        <v>1</v>
+      </c>
+      <c r="Q23" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>282</v>
       </c>
@@ -2815,23 +2829,23 @@
       <c r="F24" t="s">
         <v>8</v>
       </c>
-      <c r="H24" s="2">
+      <c r="I24" s="2">
         <v>6</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
         <v>19</v>
       </c>
-      <c r="K24" t="s">
+      <c r="L24" t="s">
         <v>184</v>
       </c>
-      <c r="O24">
-        <v>1</v>
-      </c>
-      <c r="P24" t="s">
+      <c r="P24">
+        <v>1</v>
+      </c>
+      <c r="Q24" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>165</v>
       </c>
@@ -2850,23 +2864,23 @@
       <c r="F25" t="s">
         <v>188</v>
       </c>
-      <c r="H25" s="2">
+      <c r="I25" s="2">
         <v>4</v>
       </c>
-      <c r="I25" t="s">
+      <c r="J25" t="s">
         <v>17</v>
       </c>
-      <c r="K25" t="s">
+      <c r="L25" t="s">
         <v>184</v>
       </c>
-      <c r="O25">
+      <c r="P25">
         <v>3</v>
       </c>
-      <c r="P25" t="s">
+      <c r="Q25" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>166</v>
       </c>
@@ -2885,20 +2899,20 @@
       <c r="F26" t="s">
         <v>188</v>
       </c>
-      <c r="H26" s="2">
+      <c r="I26" s="2">
         <v>4</v>
       </c>
-      <c r="K26" t="s">
+      <c r="L26" t="s">
         <v>184</v>
       </c>
-      <c r="O26">
-        <v>1</v>
-      </c>
-      <c r="P26" t="s">
+      <c r="P26">
+        <v>1</v>
+      </c>
+      <c r="Q26" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>167</v>
       </c>
@@ -2917,20 +2931,20 @@
       <c r="F27" t="s">
         <v>188</v>
       </c>
-      <c r="H27" s="2">
+      <c r="I27" s="2">
         <v>4</v>
       </c>
-      <c r="K27" t="s">
+      <c r="L27" t="s">
         <v>184</v>
       </c>
-      <c r="O27">
-        <v>1</v>
-      </c>
-      <c r="P27" t="s">
+      <c r="P27">
+        <v>1</v>
+      </c>
+      <c r="Q27" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>137</v>
       </c>
@@ -2946,17 +2960,17 @@
       <c r="E28" t="s">
         <v>238</v>
       </c>
-      <c r="I28" t="s">
+      <c r="J28" t="s">
         <v>23</v>
       </c>
-      <c r="O28">
-        <v>1</v>
-      </c>
-      <c r="P28" t="s">
+      <c r="P28">
+        <v>1</v>
+      </c>
+      <c r="Q28" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>107</v>
       </c>
@@ -2975,17 +2989,17 @@
       <c r="F29" t="s">
         <v>8</v>
       </c>
-      <c r="H29" s="2">
+      <c r="I29" s="2">
         <v>2</v>
       </c>
-      <c r="O29">
-        <v>1</v>
-      </c>
-      <c r="P29" t="s">
+      <c r="P29">
+        <v>1</v>
+      </c>
+      <c r="Q29" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>138</v>
       </c>
@@ -3001,17 +3015,26 @@
       <c r="E30" t="s">
         <v>238</v>
       </c>
-      <c r="I30" t="s">
+      <c r="F30" t="s">
+        <v>188</v>
+      </c>
+      <c r="G30" t="s">
+        <v>8</v>
+      </c>
+      <c r="H30" t="s">
+        <v>9</v>
+      </c>
+      <c r="J30" t="s">
         <v>18</v>
       </c>
-      <c r="O30">
-        <v>1</v>
-      </c>
-      <c r="P30" t="s">
+      <c r="P30">
+        <v>1</v>
+      </c>
+      <c r="Q30" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>151</v>
       </c>
@@ -3030,26 +3053,26 @@
       <c r="F31" t="s">
         <v>8</v>
       </c>
-      <c r="H31" s="2">
+      <c r="I31" s="2">
         <v>0</v>
       </c>
-      <c r="I31" t="s">
+      <c r="J31" t="s">
         <v>21</v>
       </c>
-      <c r="K31" t="s">
+      <c r="L31" t="s">
         <v>183</v>
       </c>
-      <c r="N31" t="s">
+      <c r="O31" t="s">
         <v>236</v>
       </c>
-      <c r="O31">
-        <v>1</v>
-      </c>
-      <c r="P31" t="s">
+      <c r="P31">
+        <v>1</v>
+      </c>
+      <c r="Q31" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>27</v>
       </c>
@@ -3068,20 +3091,20 @@
       <c r="F32" t="s">
         <v>8</v>
       </c>
-      <c r="H32" s="2">
+      <c r="I32" s="2">
         <v>5</v>
       </c>
-      <c r="I32" t="s">
+      <c r="J32" t="s">
         <v>17</v>
       </c>
-      <c r="O32">
+      <c r="P32">
         <v>3</v>
       </c>
-      <c r="P32" t="s">
+      <c r="Q32" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>108</v>
       </c>
@@ -3100,23 +3123,23 @@
       <c r="F33" t="s">
         <v>188</v>
       </c>
-      <c r="H33" s="2">
+      <c r="I33" s="2">
         <v>6</v>
       </c>
-      <c r="I33" t="s">
+      <c r="J33" t="s">
         <v>15</v>
       </c>
-      <c r="N33" t="s">
+      <c r="O33" t="s">
         <v>191</v>
       </c>
-      <c r="O33">
-        <v>1</v>
-      </c>
-      <c r="P33" t="s">
+      <c r="P33">
+        <v>1</v>
+      </c>
+      <c r="Q33" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>109</v>
       </c>
@@ -3135,23 +3158,23 @@
       <c r="F34" t="s">
         <v>188</v>
       </c>
-      <c r="H34" s="2">
+      <c r="I34" s="2">
         <v>6</v>
       </c>
-      <c r="I34" t="s">
+      <c r="J34" t="s">
         <v>15</v>
       </c>
-      <c r="N34" t="s">
+      <c r="O34" t="s">
         <v>191</v>
       </c>
-      <c r="O34">
-        <v>1</v>
-      </c>
-      <c r="P34" t="s">
+      <c r="P34">
+        <v>1</v>
+      </c>
+      <c r="Q34" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>110</v>
       </c>
@@ -3170,23 +3193,23 @@
       <c r="F35" t="s">
         <v>188</v>
       </c>
-      <c r="H35" s="2">
+      <c r="I35" s="2">
         <v>6</v>
       </c>
-      <c r="I35" t="s">
+      <c r="J35" t="s">
         <v>15</v>
       </c>
-      <c r="N35" t="s">
+      <c r="O35" t="s">
         <v>191</v>
       </c>
-      <c r="O35">
-        <v>1</v>
-      </c>
-      <c r="P35" t="s">
+      <c r="P35">
+        <v>1</v>
+      </c>
+      <c r="Q35" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>55</v>
       </c>
@@ -3205,17 +3228,17 @@
       <c r="F36" t="s">
         <v>8</v>
       </c>
-      <c r="H36" s="2">
+      <c r="I36" s="2">
         <v>4</v>
       </c>
-      <c r="O36">
-        <v>1</v>
-      </c>
-      <c r="P36" t="s">
+      <c r="P36">
+        <v>1</v>
+      </c>
+      <c r="Q36" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>139</v>
       </c>
@@ -3234,20 +3257,20 @@
       <c r="F37" t="s">
         <v>188</v>
       </c>
-      <c r="H37" s="2">
+      <c r="I37" s="2">
         <v>2</v>
       </c>
-      <c r="I37" t="s">
+      <c r="J37" t="s">
         <v>18</v>
       </c>
-      <c r="O37">
+      <c r="P37">
         <v>2</v>
       </c>
-      <c r="P37" t="s">
+      <c r="Q37" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>20</v>
       </c>
@@ -3263,17 +3286,26 @@
       <c r="E38" t="s">
         <v>238</v>
       </c>
-      <c r="I38" t="s">
+      <c r="F38" t="s">
+        <v>188</v>
+      </c>
+      <c r="G38" t="s">
+        <v>8</v>
+      </c>
+      <c r="H38" t="s">
+        <v>9</v>
+      </c>
+      <c r="J38" t="s">
         <v>20</v>
       </c>
-      <c r="O38">
-        <v>1</v>
-      </c>
-      <c r="P38" t="s">
+      <c r="P38">
+        <v>1</v>
+      </c>
+      <c r="Q38" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>81</v>
       </c>
@@ -3292,17 +3324,17 @@
       <c r="F39" t="s">
         <v>188</v>
       </c>
-      <c r="H39" s="2">
+      <c r="I39" s="2">
         <v>6</v>
       </c>
-      <c r="O39">
-        <v>1</v>
-      </c>
-      <c r="P39" t="s">
+      <c r="P39">
+        <v>1</v>
+      </c>
+      <c r="Q39" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>32</v>
       </c>
@@ -3321,17 +3353,17 @@
       <c r="F40" t="s">
         <v>8</v>
       </c>
-      <c r="H40" s="2">
+      <c r="I40" s="2">
         <v>6</v>
       </c>
-      <c r="O40">
-        <v>1</v>
-      </c>
-      <c r="P40" t="s">
+      <c r="P40">
+        <v>1</v>
+      </c>
+      <c r="Q40" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>82</v>
       </c>
@@ -3350,17 +3382,17 @@
       <c r="F41" t="s">
         <v>8</v>
       </c>
-      <c r="H41" s="2">
+      <c r="I41" s="2">
         <v>4</v>
       </c>
-      <c r="O41">
-        <v>1</v>
-      </c>
-      <c r="P41" t="s">
+      <c r="P41">
+        <v>1</v>
+      </c>
+      <c r="Q41" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>83</v>
       </c>
@@ -3382,20 +3414,20 @@
       <c r="G42" t="s">
         <v>8</v>
       </c>
-      <c r="H42" s="2">
+      <c r="I42" s="2">
         <v>6</v>
       </c>
-      <c r="I42" t="s">
+      <c r="J42" t="s">
         <v>12</v>
       </c>
-      <c r="O42">
+      <c r="P42">
         <v>3</v>
       </c>
-      <c r="P42" t="s">
+      <c r="Q42" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>169</v>
       </c>
@@ -3414,20 +3446,20 @@
       <c r="F43" t="s">
         <v>188</v>
       </c>
-      <c r="H43" s="2">
+      <c r="I43" s="2">
         <v>4</v>
       </c>
-      <c r="K43" t="s">
+      <c r="L43" t="s">
         <v>184</v>
       </c>
-      <c r="O43">
-        <v>1</v>
-      </c>
-      <c r="P43" t="s">
+      <c r="P43">
+        <v>1</v>
+      </c>
+      <c r="Q43" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>170</v>
       </c>
@@ -3446,23 +3478,23 @@
       <c r="F44" t="s">
         <v>9</v>
       </c>
-      <c r="H44" s="2">
+      <c r="I44" s="2">
         <v>2</v>
       </c>
-      <c r="I44" t="s">
+      <c r="J44" t="s">
         <v>18</v>
       </c>
-      <c r="K44" t="s">
+      <c r="L44" t="s">
         <v>184</v>
       </c>
-      <c r="O44">
-        <v>1</v>
-      </c>
-      <c r="P44" t="s">
+      <c r="P44">
+        <v>1</v>
+      </c>
+      <c r="Q44" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>111</v>
       </c>
@@ -3481,17 +3513,17 @@
       <c r="F45" t="s">
         <v>188</v>
       </c>
-      <c r="H45" s="2">
+      <c r="I45" s="2">
         <v>10</v>
       </c>
-      <c r="O45">
-        <v>1</v>
-      </c>
-      <c r="P45" t="s">
+      <c r="P45">
+        <v>1</v>
+      </c>
+      <c r="Q45" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>33</v>
       </c>
@@ -3510,20 +3542,20 @@
       <c r="F46" t="s">
         <v>9</v>
       </c>
-      <c r="H46" s="2">
+      <c r="I46" s="2">
         <v>5</v>
       </c>
-      <c r="I46" t="s">
+      <c r="J46" t="s">
         <v>13</v>
       </c>
-      <c r="O46">
-        <v>1</v>
-      </c>
-      <c r="P46" t="s">
+      <c r="P46">
+        <v>1</v>
+      </c>
+      <c r="Q46" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>84</v>
       </c>
@@ -3542,20 +3574,20 @@
       <c r="F47" t="s">
         <v>188</v>
       </c>
-      <c r="H47" s="2">
+      <c r="I47" s="2">
         <v>3</v>
       </c>
-      <c r="I47" t="s">
+      <c r="J47" t="s">
         <v>15</v>
       </c>
-      <c r="O47">
+      <c r="P47">
         <v>3</v>
       </c>
-      <c r="P47" t="s">
+      <c r="Q47" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>112</v>
       </c>
@@ -3574,17 +3606,17 @@
       <c r="F48" t="s">
         <v>9</v>
       </c>
-      <c r="H48" s="2">
+      <c r="I48" s="2">
         <v>6</v>
       </c>
-      <c r="O48">
-        <v>1</v>
-      </c>
-      <c r="P48" t="s">
+      <c r="P48">
+        <v>1</v>
+      </c>
+      <c r="Q48" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>85</v>
       </c>
@@ -3603,17 +3635,17 @@
       <c r="F49" t="s">
         <v>8</v>
       </c>
-      <c r="H49" s="2">
+      <c r="I49" s="2">
         <v>10</v>
       </c>
-      <c r="O49">
-        <v>1</v>
-      </c>
-      <c r="P49" t="s">
+      <c r="P49">
+        <v>1</v>
+      </c>
+      <c r="Q49" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>86</v>
       </c>
@@ -3632,20 +3664,20 @@
       <c r="F50" t="s">
         <v>8</v>
       </c>
-      <c r="H50" s="2">
+      <c r="I50" s="2">
         <v>2</v>
       </c>
-      <c r="I50" t="s">
+      <c r="J50" t="s">
         <v>15</v>
       </c>
-      <c r="O50">
+      <c r="P50">
         <v>3</v>
       </c>
-      <c r="P50" t="s">
+      <c r="Q50" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>140</v>
       </c>
@@ -3664,17 +3696,17 @@
       <c r="F51" t="s">
         <v>188</v>
       </c>
-      <c r="H51" s="2">
+      <c r="I51" s="2">
         <v>5</v>
       </c>
-      <c r="O51">
+      <c r="P51">
         <v>2</v>
       </c>
-      <c r="P51" t="s">
+      <c r="Q51" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>113</v>
       </c>
@@ -3693,17 +3725,17 @@
       <c r="F52" t="s">
         <v>8</v>
       </c>
-      <c r="H52" s="2">
+      <c r="I52" s="2">
         <v>2</v>
       </c>
-      <c r="O52">
-        <v>1</v>
-      </c>
-      <c r="P52" t="s">
+      <c r="P52">
+        <v>1</v>
+      </c>
+      <c r="Q52" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>171</v>
       </c>
@@ -3722,23 +3754,23 @@
       <c r="F53" t="s">
         <v>8</v>
       </c>
-      <c r="H53" s="2">
+      <c r="I53" s="2">
         <v>8</v>
       </c>
-      <c r="I53" t="s">
+      <c r="J53" t="s">
         <v>22</v>
       </c>
-      <c r="K53" t="s">
+      <c r="L53" t="s">
         <v>184</v>
       </c>
-      <c r="O53">
-        <v>1</v>
-      </c>
-      <c r="P53" t="s">
+      <c r="P53">
+        <v>1</v>
+      </c>
+      <c r="Q53" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>28</v>
       </c>
@@ -3757,17 +3789,17 @@
       <c r="F54" t="s">
         <v>188</v>
       </c>
-      <c r="H54" s="2">
+      <c r="I54" s="2">
         <v>10</v>
       </c>
-      <c r="O54">
-        <v>1</v>
-      </c>
-      <c r="P54" t="s">
+      <c r="P54">
+        <v>1</v>
+      </c>
+      <c r="Q54" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>59</v>
       </c>
@@ -3786,20 +3818,20 @@
       <c r="F55" t="s">
         <v>8</v>
       </c>
-      <c r="H55" s="2">
-        <v>1</v>
-      </c>
-      <c r="I55" t="s">
+      <c r="I55" s="2">
+        <v>1</v>
+      </c>
+      <c r="J55" t="s">
         <v>13</v>
       </c>
-      <c r="O55">
+      <c r="P55">
         <v>2</v>
       </c>
-      <c r="P55" t="s">
+      <c r="Q55" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>118</v>
       </c>
@@ -3818,17 +3850,17 @@
       <c r="F56" t="s">
         <v>188</v>
       </c>
-      <c r="H56" s="2">
+      <c r="I56" s="2">
         <v>6</v>
       </c>
-      <c r="O56">
-        <v>1</v>
-      </c>
-      <c r="P56" t="s">
+      <c r="P56">
+        <v>1</v>
+      </c>
+      <c r="Q56" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>87</v>
       </c>
@@ -3850,20 +3882,20 @@
       <c r="G57" t="s">
         <v>8</v>
       </c>
-      <c r="H57" s="2">
+      <c r="I57" s="2">
         <v>6</v>
       </c>
-      <c r="I57" t="s">
+      <c r="J57" t="s">
         <v>12</v>
       </c>
-      <c r="O57">
-        <v>1</v>
-      </c>
-      <c r="P57" t="s">
+      <c r="P57">
+        <v>1</v>
+      </c>
+      <c r="Q57" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>119</v>
       </c>
@@ -3882,17 +3914,17 @@
       <c r="F58" t="s">
         <v>9</v>
       </c>
-      <c r="H58" s="2">
+      <c r="I58" s="2">
         <v>6</v>
       </c>
-      <c r="O58">
-        <v>1</v>
-      </c>
-      <c r="P58" t="s">
+      <c r="P58">
+        <v>1</v>
+      </c>
+      <c r="Q58" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>120</v>
       </c>
@@ -3911,17 +3943,17 @@
       <c r="F59" t="s">
         <v>188</v>
       </c>
-      <c r="H59" s="2">
+      <c r="I59" s="2">
         <v>2</v>
       </c>
-      <c r="O59">
-        <v>1</v>
-      </c>
-      <c r="P59" t="s">
+      <c r="P59">
+        <v>1</v>
+      </c>
+      <c r="Q59" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>121</v>
       </c>
@@ -3940,17 +3972,17 @@
       <c r="F60" t="s">
         <v>188</v>
       </c>
-      <c r="H60" s="2">
+      <c r="I60" s="2">
         <v>5</v>
       </c>
-      <c r="O60">
-        <v>1</v>
-      </c>
-      <c r="P60" t="s">
+      <c r="P60">
+        <v>1</v>
+      </c>
+      <c r="Q60" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>122</v>
       </c>
@@ -3969,17 +4001,17 @@
       <c r="F61" t="s">
         <v>188</v>
       </c>
-      <c r="H61" s="2">
+      <c r="I61" s="2">
         <v>5</v>
       </c>
-      <c r="O61">
-        <v>1</v>
-      </c>
-      <c r="P61" t="s">
+      <c r="P61">
+        <v>1</v>
+      </c>
+      <c r="Q61" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>60</v>
       </c>
@@ -3998,17 +4030,17 @@
       <c r="F62" t="s">
         <v>8</v>
       </c>
-      <c r="H62" s="2">
+      <c r="I62" s="2">
         <v>6</v>
       </c>
-      <c r="O62">
-        <v>1</v>
-      </c>
-      <c r="P62" t="s">
+      <c r="P62">
+        <v>1</v>
+      </c>
+      <c r="Q62" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>123</v>
       </c>
@@ -4027,17 +4059,17 @@
       <c r="F63" t="s">
         <v>8</v>
       </c>
-      <c r="H63" s="2">
+      <c r="I63" s="2">
         <v>2</v>
       </c>
-      <c r="O63">
-        <v>1</v>
-      </c>
-      <c r="P63" t="s">
+      <c r="P63">
+        <v>1</v>
+      </c>
+      <c r="Q63" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>152</v>
       </c>
@@ -4056,26 +4088,26 @@
       <c r="F64" t="s">
         <v>9</v>
       </c>
-      <c r="H64" s="2">
+      <c r="I64" s="2">
         <v>2</v>
       </c>
-      <c r="I64" t="s">
+      <c r="J64" t="s">
         <v>15</v>
       </c>
-      <c r="K64" t="s">
+      <c r="L64" t="s">
         <v>183</v>
       </c>
-      <c r="N64" t="s">
+      <c r="O64" t="s">
         <v>153</v>
       </c>
-      <c r="O64">
-        <v>1</v>
-      </c>
-      <c r="P64" t="s">
+      <c r="P64">
+        <v>1</v>
+      </c>
+      <c r="Q64" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>153</v>
       </c>
@@ -4094,23 +4126,23 @@
       <c r="F65" t="s">
         <v>8</v>
       </c>
-      <c r="H65" s="2">
+      <c r="I65" s="2">
         <v>4</v>
       </c>
-      <c r="I65" t="s">
+      <c r="J65" t="s">
         <v>15</v>
       </c>
-      <c r="K65" t="s">
+      <c r="L65" t="s">
         <v>183</v>
       </c>
-      <c r="O65">
-        <v>1</v>
-      </c>
-      <c r="P65" t="s">
+      <c r="P65">
+        <v>1</v>
+      </c>
+      <c r="Q65" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>141</v>
       </c>
@@ -4129,23 +4161,23 @@
       <c r="F66" t="s">
         <v>188</v>
       </c>
-      <c r="H66" s="2">
+      <c r="I66" s="2">
         <v>15</v>
       </c>
-      <c r="I66" t="s">
+      <c r="J66" t="s">
         <v>15</v>
       </c>
-      <c r="N66" t="s">
+      <c r="O66" t="s">
         <v>189</v>
       </c>
-      <c r="O66">
+      <c r="P66">
         <v>2</v>
       </c>
-      <c r="P66" t="s">
+      <c r="Q66" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>124</v>
       </c>
@@ -4164,20 +4196,20 @@
       <c r="F67" t="s">
         <v>188</v>
       </c>
-      <c r="H67" s="2">
-        <v>1</v>
-      </c>
-      <c r="I67" t="s">
+      <c r="I67" s="2">
+        <v>1</v>
+      </c>
+      <c r="J67" t="s">
         <v>15</v>
       </c>
-      <c r="O67">
+      <c r="P67">
         <v>3</v>
       </c>
-      <c r="P67" t="s">
+      <c r="Q67" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>125</v>
       </c>
@@ -4196,17 +4228,17 @@
       <c r="F68" t="s">
         <v>8</v>
       </c>
-      <c r="H68" s="2">
+      <c r="I68" s="2">
         <v>5</v>
       </c>
-      <c r="O68">
-        <v>1</v>
-      </c>
-      <c r="P68" t="s">
+      <c r="P68">
+        <v>1</v>
+      </c>
+      <c r="Q68" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>126</v>
       </c>
@@ -4225,17 +4257,17 @@
       <c r="F69" t="s">
         <v>188</v>
       </c>
-      <c r="H69" s="2">
+      <c r="I69" s="2">
         <v>5</v>
       </c>
-      <c r="O69">
-        <v>1</v>
-      </c>
-      <c r="P69" t="s">
+      <c r="P69">
+        <v>1</v>
+      </c>
+      <c r="Q69" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>127</v>
       </c>
@@ -4257,20 +4289,20 @@
       <c r="G70" t="s">
         <v>8</v>
       </c>
-      <c r="H70" s="2">
+      <c r="I70" s="2">
         <v>2</v>
       </c>
-      <c r="I70" t="s">
+      <c r="J70" t="s">
         <v>12</v>
       </c>
-      <c r="O70">
-        <v>1</v>
-      </c>
-      <c r="P70" t="s">
+      <c r="P70">
+        <v>1</v>
+      </c>
+      <c r="Q70" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>92</v>
       </c>
@@ -4289,20 +4321,20 @@
       <c r="F71" t="s">
         <v>8</v>
       </c>
-      <c r="H71" s="2">
+      <c r="I71" s="2">
         <v>0</v>
       </c>
-      <c r="I71" t="s">
+      <c r="J71" t="s">
         <v>13</v>
       </c>
-      <c r="O71">
+      <c r="P71">
         <v>3</v>
       </c>
-      <c r="P71" t="s">
+      <c r="Q71" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>93</v>
       </c>
@@ -4321,20 +4353,20 @@
       <c r="F72" t="s">
         <v>188</v>
       </c>
-      <c r="H72" s="2">
+      <c r="I72" s="2">
         <v>5</v>
       </c>
-      <c r="I72" t="s">
+      <c r="J72" t="s">
         <v>15</v>
       </c>
-      <c r="O72">
+      <c r="P72">
         <v>3</v>
       </c>
-      <c r="P72" t="s">
+      <c r="Q72" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>61</v>
       </c>
@@ -4353,17 +4385,17 @@
       <c r="F73" t="s">
         <v>9</v>
       </c>
-      <c r="H73" s="2">
+      <c r="I73" s="2">
         <v>10</v>
       </c>
-      <c r="O73">
-        <v>1</v>
-      </c>
-      <c r="P73" t="s">
+      <c r="P73">
+        <v>1</v>
+      </c>
+      <c r="Q73" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>266</v>
       </c>
@@ -4382,20 +4414,20 @@
       <c r="F74" t="s">
         <v>188</v>
       </c>
-      <c r="H74" s="2">
+      <c r="I74" s="2">
         <v>11</v>
       </c>
-      <c r="K74" t="s">
+      <c r="L74" t="s">
         <v>184</v>
       </c>
-      <c r="O74">
-        <v>1</v>
-      </c>
-      <c r="P74" t="s">
+      <c r="P74">
+        <v>1</v>
+      </c>
+      <c r="Q74" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>172</v>
       </c>
@@ -4414,20 +4446,20 @@
       <c r="F75" t="s">
         <v>8</v>
       </c>
-      <c r="H75" s="2">
+      <c r="I75" s="2">
         <v>10</v>
       </c>
-      <c r="K75" t="s">
+      <c r="L75" t="s">
         <v>184</v>
       </c>
-      <c r="O75">
-        <v>1</v>
-      </c>
-      <c r="P75" t="s">
+      <c r="P75">
+        <v>1</v>
+      </c>
+      <c r="Q75" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>173</v>
       </c>
@@ -4446,20 +4478,20 @@
       <c r="F76" t="s">
         <v>9</v>
       </c>
-      <c r="H76" s="2">
+      <c r="I76" s="2">
         <v>4</v>
       </c>
-      <c r="K76" t="s">
+      <c r="L76" t="s">
         <v>184</v>
       </c>
-      <c r="O76">
-        <v>1</v>
-      </c>
-      <c r="P76" t="s">
+      <c r="P76">
+        <v>1</v>
+      </c>
+      <c r="Q76" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>128</v>
       </c>
@@ -4478,17 +4510,17 @@
       <c r="F77" t="s">
         <v>9</v>
       </c>
-      <c r="H77" s="2">
+      <c r="I77" s="2">
         <v>5</v>
       </c>
-      <c r="O77">
-        <v>1</v>
-      </c>
-      <c r="P77" t="s">
+      <c r="P77">
+        <v>1</v>
+      </c>
+      <c r="Q77" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>94</v>
       </c>
@@ -4507,17 +4539,17 @@
       <c r="F78" t="s">
         <v>8</v>
       </c>
-      <c r="H78" s="2">
+      <c r="I78" s="2">
         <v>6</v>
       </c>
-      <c r="O78">
-        <v>1</v>
-      </c>
-      <c r="P78" t="s">
+      <c r="P78">
+        <v>1</v>
+      </c>
+      <c r="Q78" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>129</v>
       </c>
@@ -4536,17 +4568,17 @@
       <c r="F79" t="s">
         <v>188</v>
       </c>
-      <c r="H79" s="2">
+      <c r="I79" s="2">
         <v>10</v>
       </c>
-      <c r="O79">
-        <v>1</v>
-      </c>
-      <c r="P79" t="s">
+      <c r="P79">
+        <v>1</v>
+      </c>
+      <c r="Q79" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="80" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>142</v>
       </c>
@@ -4565,17 +4597,17 @@
       <c r="F80" t="s">
         <v>8</v>
       </c>
-      <c r="I80" t="s">
+      <c r="J80" t="s">
         <v>23</v>
       </c>
-      <c r="O80">
-        <v>1</v>
-      </c>
-      <c r="P80" t="s">
+      <c r="P80">
+        <v>1</v>
+      </c>
+      <c r="Q80" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>62</v>
       </c>
@@ -4594,20 +4626,20 @@
       <c r="F81" t="s">
         <v>188</v>
       </c>
-      <c r="H81" s="2">
+      <c r="I81" s="2">
         <v>3</v>
       </c>
-      <c r="I81" t="s">
+      <c r="J81" t="s">
         <v>17</v>
       </c>
-      <c r="O81">
+      <c r="P81">
         <v>4</v>
       </c>
-      <c r="P81" t="s">
+      <c r="Q81" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>95</v>
       </c>
@@ -4626,17 +4658,17 @@
       <c r="F82" t="s">
         <v>8</v>
       </c>
-      <c r="H82" s="2">
+      <c r="I82" s="2">
         <v>10</v>
       </c>
-      <c r="O82">
-        <v>1</v>
-      </c>
-      <c r="P82" t="s">
+      <c r="P82">
+        <v>1</v>
+      </c>
+      <c r="Q82" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>283</v>
       </c>
@@ -4655,20 +4687,20 @@
       <c r="F83" t="s">
         <v>188</v>
       </c>
-      <c r="H83" s="2">
+      <c r="I83" s="2">
         <v>10</v>
       </c>
-      <c r="I83" t="s">
+      <c r="J83" t="s">
         <v>14</v>
       </c>
-      <c r="O83">
-        <v>1</v>
-      </c>
-      <c r="P83" t="s">
+      <c r="P83">
+        <v>1</v>
+      </c>
+      <c r="Q83" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>38</v>
       </c>
@@ -4687,17 +4719,17 @@
       <c r="F84" t="s">
         <v>188</v>
       </c>
-      <c r="H84" s="2">
+      <c r="I84" s="2">
         <v>10</v>
       </c>
-      <c r="O84">
-        <v>1</v>
-      </c>
-      <c r="P84" t="s">
+      <c r="P84">
+        <v>1</v>
+      </c>
+      <c r="Q84" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>29</v>
       </c>
@@ -4716,20 +4748,20 @@
       <c r="F85" t="s">
         <v>9</v>
       </c>
-      <c r="H85" s="2">
-        <v>1</v>
-      </c>
-      <c r="I85" t="s">
+      <c r="I85" s="2">
+        <v>1</v>
+      </c>
+      <c r="J85" t="s">
         <v>14</v>
       </c>
-      <c r="O85">
+      <c r="P85">
         <v>3</v>
       </c>
-      <c r="P85" t="s">
+      <c r="Q85" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>174</v>
       </c>
@@ -4748,26 +4780,26 @@
       <c r="F86" t="s">
         <v>188</v>
       </c>
-      <c r="H86" s="2">
+      <c r="I86" s="2">
         <v>0</v>
       </c>
-      <c r="I86" t="s">
+      <c r="J86" t="s">
         <v>21</v>
       </c>
-      <c r="K86" t="s">
+      <c r="L86" t="s">
         <v>184</v>
       </c>
-      <c r="N86" t="s">
+      <c r="O86" t="s">
         <v>266</v>
       </c>
-      <c r="O86">
-        <v>1</v>
-      </c>
-      <c r="P86" t="s">
+      <c r="P86">
+        <v>1</v>
+      </c>
+      <c r="Q86" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>130</v>
       </c>
@@ -4789,23 +4821,23 @@
       <c r="G87" t="s">
         <v>8</v>
       </c>
-      <c r="H87" s="2">
+      <c r="I87" s="2">
         <v>8</v>
       </c>
-      <c r="I87" t="s">
+      <c r="J87" t="s">
         <v>12</v>
       </c>
-      <c r="J87" t="s">
+      <c r="K87" t="s">
         <v>14</v>
       </c>
-      <c r="O87">
-        <v>1</v>
-      </c>
-      <c r="P87" t="s">
+      <c r="P87">
+        <v>1</v>
+      </c>
+      <c r="Q87" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>39</v>
       </c>
@@ -4824,17 +4856,17 @@
       <c r="F88" t="s">
         <v>8</v>
       </c>
-      <c r="H88" s="2">
+      <c r="I88" s="2">
         <v>5</v>
       </c>
-      <c r="O88">
-        <v>1</v>
-      </c>
-      <c r="P88" t="s">
+      <c r="P88">
+        <v>1</v>
+      </c>
+      <c r="Q88" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>131</v>
       </c>
@@ -4853,17 +4885,17 @@
       <c r="F89" t="s">
         <v>8</v>
       </c>
-      <c r="H89" s="2">
+      <c r="I89" s="2">
         <v>10</v>
       </c>
-      <c r="O89">
-        <v>1</v>
-      </c>
-      <c r="P89" t="s">
+      <c r="P89">
+        <v>1</v>
+      </c>
+      <c r="Q89" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>63</v>
       </c>
@@ -4882,17 +4914,17 @@
       <c r="F90" t="s">
         <v>188</v>
       </c>
-      <c r="H90" s="2">
+      <c r="I90" s="2">
         <v>10</v>
       </c>
-      <c r="O90">
-        <v>1</v>
-      </c>
-      <c r="P90" t="s">
+      <c r="P90">
+        <v>1</v>
+      </c>
+      <c r="Q90" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>176</v>
       </c>
@@ -4911,23 +4943,23 @@
       <c r="F91" t="s">
         <v>8</v>
       </c>
-      <c r="H91" s="2">
+      <c r="I91" s="2">
         <v>4</v>
       </c>
-      <c r="I91" t="s">
+      <c r="J91" t="s">
         <v>15</v>
       </c>
-      <c r="K91" t="s">
+      <c r="L91" t="s">
         <v>184</v>
       </c>
-      <c r="O91">
-        <v>1</v>
-      </c>
-      <c r="P91" t="s">
+      <c r="P91">
+        <v>1</v>
+      </c>
+      <c r="Q91" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>177</v>
       </c>
@@ -4946,20 +4978,20 @@
       <c r="F92" t="s">
         <v>188</v>
       </c>
-      <c r="H92" s="2">
+      <c r="I92" s="2">
         <v>6</v>
       </c>
-      <c r="K92" t="s">
+      <c r="L92" t="s">
         <v>184</v>
       </c>
-      <c r="O92">
-        <v>1</v>
-      </c>
-      <c r="P92" t="s">
+      <c r="P92">
+        <v>1</v>
+      </c>
+      <c r="Q92" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>96</v>
       </c>
@@ -4978,17 +5010,17 @@
       <c r="F93" t="s">
         <v>188</v>
       </c>
-      <c r="H93" s="2">
+      <c r="I93" s="2">
         <v>5</v>
       </c>
-      <c r="O93">
+      <c r="P93">
         <v>5</v>
       </c>
-      <c r="P93" t="s">
+      <c r="Q93" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>22</v>
       </c>
@@ -5004,20 +5036,29 @@
       <c r="E94" t="s">
         <v>238</v>
       </c>
-      <c r="I94" t="s">
+      <c r="F94" t="s">
+        <v>188</v>
+      </c>
+      <c r="G94" t="s">
+        <v>8</v>
+      </c>
+      <c r="H94" t="s">
+        <v>9</v>
+      </c>
+      <c r="J94" t="s">
         <v>22</v>
       </c>
-      <c r="K94" t="s">
+      <c r="L94" t="s">
         <v>184</v>
       </c>
-      <c r="O94">
-        <v>1</v>
-      </c>
-      <c r="P94" t="s">
+      <c r="P94">
+        <v>1</v>
+      </c>
+      <c r="Q94" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>245</v>
       </c>
@@ -5036,20 +5077,20 @@
       <c r="F95" t="s">
         <v>188</v>
       </c>
-      <c r="H95" s="2">
+      <c r="I95" s="2">
         <v>10</v>
       </c>
-      <c r="I95" t="s">
+      <c r="J95" t="s">
         <v>13</v>
       </c>
-      <c r="O95">
-        <v>1</v>
-      </c>
-      <c r="P95" t="s">
+      <c r="P95">
+        <v>1</v>
+      </c>
+      <c r="Q95" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>97</v>
       </c>
@@ -5068,20 +5109,20 @@
       <c r="F96" t="s">
         <v>8</v>
       </c>
-      <c r="H96" s="2">
+      <c r="I96" s="2">
         <v>10</v>
       </c>
-      <c r="I96" t="s">
+      <c r="J96" t="s">
         <v>14</v>
       </c>
-      <c r="O96">
-        <v>1</v>
-      </c>
-      <c r="P96" t="s">
+      <c r="P96">
+        <v>1</v>
+      </c>
+      <c r="Q96" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>64</v>
       </c>
@@ -5100,17 +5141,17 @@
       <c r="F97" t="s">
         <v>188</v>
       </c>
-      <c r="H97" s="2">
+      <c r="I97" s="2">
         <v>3</v>
       </c>
-      <c r="O97">
-        <v>1</v>
-      </c>
-      <c r="P97" t="s">
+      <c r="P97">
+        <v>1</v>
+      </c>
+      <c r="Q97" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>65</v>
       </c>
@@ -5129,17 +5170,17 @@
       <c r="F98" t="s">
         <v>9</v>
       </c>
-      <c r="H98" s="2">
+      <c r="I98" s="2">
         <v>10</v>
       </c>
-      <c r="O98">
-        <v>1</v>
-      </c>
-      <c r="P98" t="s">
+      <c r="P98">
+        <v>1</v>
+      </c>
+      <c r="Q98" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>235</v>
       </c>
@@ -5158,20 +5199,20 @@
       <c r="F99" t="s">
         <v>188</v>
       </c>
-      <c r="H99" s="2">
+      <c r="I99" s="2">
         <v>0</v>
       </c>
-      <c r="I99" t="s">
+      <c r="J99" t="s">
         <v>16</v>
       </c>
-      <c r="O99">
+      <c r="P99">
         <v>2</v>
       </c>
-      <c r="P99" t="s">
+      <c r="Q99" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>66</v>
       </c>
@@ -5190,20 +5231,20 @@
       <c r="F100" t="s">
         <v>188</v>
       </c>
-      <c r="H100" s="2">
+      <c r="I100" s="2">
         <v>2</v>
       </c>
-      <c r="I100" t="s">
+      <c r="J100" t="s">
         <v>17</v>
       </c>
-      <c r="O100">
+      <c r="P100">
         <v>3</v>
       </c>
-      <c r="P100" t="s">
+      <c r="Q100" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>132</v>
       </c>
@@ -5222,20 +5263,20 @@
       <c r="F101" t="s">
         <v>188</v>
       </c>
-      <c r="H101" s="2">
+      <c r="I101" s="2">
         <v>2</v>
       </c>
-      <c r="I101" t="s">
+      <c r="J101" t="s">
         <v>15</v>
       </c>
-      <c r="O101">
+      <c r="P101">
         <v>3</v>
       </c>
-      <c r="P101" t="s">
+      <c r="Q101" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>178</v>
       </c>
@@ -5257,26 +5298,26 @@
       <c r="G102" t="s">
         <v>8</v>
       </c>
-      <c r="H102" s="2">
+      <c r="I102" s="2">
         <v>12</v>
       </c>
-      <c r="I102" t="s">
+      <c r="J102" t="s">
         <v>12</v>
       </c>
-      <c r="J102" t="s">
+      <c r="K102" t="s">
         <v>14</v>
       </c>
-      <c r="K102" t="s">
+      <c r="L102" t="s">
         <v>184</v>
       </c>
-      <c r="O102">
-        <v>1</v>
-      </c>
-      <c r="P102" t="s">
+      <c r="P102">
+        <v>1</v>
+      </c>
+      <c r="Q102" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>154</v>
       </c>
@@ -5298,26 +5339,26 @@
       <c r="G103" t="s">
         <v>8</v>
       </c>
-      <c r="H103" s="2">
+      <c r="I103" s="2">
         <v>6</v>
       </c>
-      <c r="I103" t="s">
+      <c r="J103" t="s">
         <v>12</v>
       </c>
-      <c r="J103" t="s">
+      <c r="K103" t="s">
         <v>14</v>
       </c>
-      <c r="K103" t="s">
+      <c r="L103" t="s">
         <v>183</v>
       </c>
-      <c r="O103">
-        <v>1</v>
-      </c>
-      <c r="P103" t="s">
+      <c r="P103">
+        <v>1</v>
+      </c>
+      <c r="Q103" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>280</v>
       </c>
@@ -5336,17 +5377,17 @@
       <c r="F104" t="s">
         <v>8</v>
       </c>
-      <c r="H104" s="2">
+      <c r="I104" s="2">
         <v>10</v>
       </c>
-      <c r="O104">
-        <v>1</v>
-      </c>
-      <c r="P104" t="s">
+      <c r="P104">
+        <v>1</v>
+      </c>
+      <c r="Q104" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>133</v>
       </c>
@@ -5365,17 +5406,17 @@
       <c r="F105" t="s">
         <v>188</v>
       </c>
-      <c r="H105" s="2">
+      <c r="I105" s="2">
         <v>5</v>
       </c>
-      <c r="O105">
-        <v>1</v>
-      </c>
-      <c r="P105" t="s">
+      <c r="P105">
+        <v>1</v>
+      </c>
+      <c r="Q105" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>40</v>
       </c>
@@ -5394,20 +5435,20 @@
       <c r="F106" t="s">
         <v>188</v>
       </c>
-      <c r="H106" s="2">
-        <v>1</v>
-      </c>
-      <c r="I106" t="s">
+      <c r="I106" s="2">
+        <v>1</v>
+      </c>
+      <c r="J106" t="s">
         <v>17</v>
       </c>
-      <c r="O106">
+      <c r="P106">
         <v>3</v>
       </c>
-      <c r="P106" t="s">
+      <c r="Q106" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>41</v>
       </c>
@@ -5426,20 +5467,20 @@
       <c r="F107" t="s">
         <v>188</v>
       </c>
-      <c r="H107" s="2">
+      <c r="I107" s="2">
         <v>5</v>
       </c>
-      <c r="I107" t="s">
+      <c r="J107" t="s">
         <v>16</v>
       </c>
-      <c r="O107">
-        <v>1</v>
-      </c>
-      <c r="P107" t="s">
+      <c r="P107">
+        <v>1</v>
+      </c>
+      <c r="Q107" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>67</v>
       </c>
@@ -5458,17 +5499,17 @@
       <c r="F108" t="s">
         <v>8</v>
       </c>
-      <c r="H108" s="2">
+      <c r="I108" s="2">
         <v>3</v>
       </c>
-      <c r="O108">
-        <v>1</v>
-      </c>
-      <c r="P108" t="s">
+      <c r="P108">
+        <v>1</v>
+      </c>
+      <c r="Q108" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>68</v>
       </c>
@@ -5487,17 +5528,17 @@
       <c r="F109" t="s">
         <v>188</v>
       </c>
-      <c r="H109" s="2">
+      <c r="I109" s="2">
         <v>4</v>
       </c>
-      <c r="O109">
-        <v>1</v>
-      </c>
-      <c r="P109" t="s">
+      <c r="P109">
+        <v>1</v>
+      </c>
+      <c r="Q109" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>30</v>
       </c>
@@ -5516,17 +5557,17 @@
       <c r="F110" t="s">
         <v>188</v>
       </c>
-      <c r="H110" s="2">
-        <v>1</v>
-      </c>
-      <c r="O110">
+      <c r="I110" s="2">
+        <v>1</v>
+      </c>
+      <c r="P110">
         <v>2</v>
       </c>
-      <c r="P110" t="s">
+      <c r="Q110" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>244</v>
       </c>
@@ -5545,17 +5586,17 @@
       <c r="F111" t="s">
         <v>8</v>
       </c>
-      <c r="H111" s="2">
+      <c r="I111" s="2">
         <v>5</v>
       </c>
-      <c r="O111">
-        <v>1</v>
-      </c>
-      <c r="P111" t="s">
+      <c r="P111">
+        <v>1</v>
+      </c>
+      <c r="Q111" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>98</v>
       </c>
@@ -5574,17 +5615,17 @@
       <c r="F112" t="s">
         <v>8</v>
       </c>
-      <c r="H112" s="2">
-        <v>1</v>
-      </c>
-      <c r="O112">
-        <v>1</v>
-      </c>
-      <c r="P112" t="s">
+      <c r="I112" s="2">
+        <v>1</v>
+      </c>
+      <c r="P112">
+        <v>1</v>
+      </c>
+      <c r="Q112" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>189</v>
       </c>
@@ -5603,20 +5644,20 @@
       <c r="F113" t="s">
         <v>188</v>
       </c>
-      <c r="H113" s="2">
+      <c r="I113" s="2">
         <v>3</v>
       </c>
-      <c r="K113" t="s">
+      <c r="L113" t="s">
         <v>190</v>
       </c>
-      <c r="O113">
-        <v>1</v>
-      </c>
-      <c r="P113" t="s">
+      <c r="P113">
+        <v>1</v>
+      </c>
+      <c r="Q113" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>69</v>
       </c>
@@ -5635,17 +5676,17 @@
       <c r="F114" t="s">
         <v>9</v>
       </c>
-      <c r="H114" s="2">
+      <c r="I114" s="2">
         <v>3</v>
       </c>
-      <c r="O114">
-        <v>1</v>
-      </c>
-      <c r="P114" t="s">
+      <c r="P114">
+        <v>1</v>
+      </c>
+      <c r="Q114" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>42</v>
       </c>
@@ -5664,17 +5705,17 @@
       <c r="F115" t="s">
         <v>8</v>
       </c>
-      <c r="H115" s="2">
+      <c r="I115" s="2">
         <v>4</v>
       </c>
-      <c r="O115">
-        <v>1</v>
-      </c>
-      <c r="P115" t="s">
+      <c r="P115">
+        <v>1</v>
+      </c>
+      <c r="Q115" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>99</v>
       </c>
@@ -5693,17 +5734,17 @@
       <c r="F116" t="s">
         <v>8</v>
       </c>
-      <c r="H116" s="2">
+      <c r="I116" s="2">
         <v>10</v>
       </c>
-      <c r="O116">
-        <v>1</v>
-      </c>
-      <c r="P116" t="s">
+      <c r="P116">
+        <v>1</v>
+      </c>
+      <c r="Q116" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>158</v>
       </c>
@@ -5722,29 +5763,29 @@
       <c r="F117" t="s">
         <v>9</v>
       </c>
-      <c r="H117" s="2">
+      <c r="I117" s="2">
         <v>8</v>
       </c>
-      <c r="I117" t="s">
+      <c r="J117" t="s">
         <v>19</v>
       </c>
-      <c r="K117" t="s">
+      <c r="L117" t="s">
         <v>183</v>
       </c>
-      <c r="L117" t="s">
+      <c r="M117" t="s">
         <v>9</v>
       </c>
-      <c r="M117">
+      <c r="N117">
         <v>10</v>
       </c>
-      <c r="O117">
-        <v>1</v>
-      </c>
-      <c r="P117" t="s">
+      <c r="P117">
+        <v>1</v>
+      </c>
+      <c r="Q117" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>19</v>
       </c>
@@ -5760,17 +5801,17 @@
       <c r="E118" t="s">
         <v>238</v>
       </c>
-      <c r="I118" t="s">
+      <c r="J118" t="s">
         <v>19</v>
       </c>
-      <c r="O118">
-        <v>1</v>
-      </c>
-      <c r="P118" t="s">
+      <c r="P118">
+        <v>1</v>
+      </c>
+      <c r="Q118" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>43</v>
       </c>
@@ -5789,17 +5830,17 @@
       <c r="F119" t="s">
         <v>8</v>
       </c>
-      <c r="H119" s="2">
+      <c r="I119" s="2">
         <v>4</v>
       </c>
-      <c r="O119">
-        <v>1</v>
-      </c>
-      <c r="P119" t="s">
+      <c r="P119">
+        <v>1</v>
+      </c>
+      <c r="Q119" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>243</v>
       </c>
@@ -5818,20 +5859,20 @@
       <c r="F120" t="s">
         <v>188</v>
       </c>
-      <c r="H120" s="2">
+      <c r="I120" s="2">
         <v>7</v>
       </c>
-      <c r="I120" t="s">
+      <c r="J120" t="s">
         <v>16</v>
       </c>
-      <c r="O120">
-        <v>1</v>
-      </c>
-      <c r="P120" t="s">
+      <c r="P120">
+        <v>1</v>
+      </c>
+      <c r="Q120" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>70</v>
       </c>
@@ -5850,17 +5891,17 @@
       <c r="F121" t="s">
         <v>9</v>
       </c>
-      <c r="H121" s="2">
+      <c r="I121" s="2">
         <v>6</v>
       </c>
-      <c r="O121">
-        <v>1</v>
-      </c>
-      <c r="P121" t="s">
+      <c r="P121">
+        <v>1</v>
+      </c>
+      <c r="Q121" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>71</v>
       </c>
@@ -5879,20 +5920,20 @@
       <c r="F122" t="s">
         <v>9</v>
       </c>
-      <c r="H122" s="2">
+      <c r="I122" s="2">
         <v>0</v>
       </c>
-      <c r="I122" t="s">
+      <c r="J122" t="s">
         <v>13</v>
       </c>
-      <c r="O122">
-        <v>1</v>
-      </c>
-      <c r="P122" t="s">
+      <c r="P122">
+        <v>1</v>
+      </c>
+      <c r="Q122" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>44</v>
       </c>
@@ -5911,17 +5952,17 @@
       <c r="F123" t="s">
         <v>9</v>
       </c>
-      <c r="H123" s="2">
+      <c r="I123" s="2">
         <v>6</v>
       </c>
-      <c r="O123">
+      <c r="P123">
         <v>2</v>
       </c>
-      <c r="P123" t="s">
+      <c r="Q123" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>45</v>
       </c>
@@ -5940,17 +5981,17 @@
       <c r="F124" t="s">
         <v>188</v>
       </c>
-      <c r="H124" s="2">
+      <c r="I124" s="2">
         <v>5</v>
       </c>
-      <c r="O124">
-        <v>1</v>
-      </c>
-      <c r="P124" t="s">
+      <c r="P124">
+        <v>1</v>
+      </c>
+      <c r="Q124" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>281</v>
       </c>
@@ -5969,20 +6010,20 @@
       <c r="F125" t="s">
         <v>188</v>
       </c>
-      <c r="H125" s="2">
+      <c r="I125" s="2">
         <v>4</v>
       </c>
-      <c r="I125" t="s">
+      <c r="J125" t="s">
         <v>16</v>
       </c>
-      <c r="O125">
-        <v>1</v>
-      </c>
-      <c r="P125" t="s">
+      <c r="P125">
+        <v>1</v>
+      </c>
+      <c r="Q125" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>46</v>
       </c>
@@ -6001,17 +6042,17 @@
       <c r="F126" t="s">
         <v>188</v>
       </c>
-      <c r="H126" s="2">
+      <c r="I126" s="2">
         <v>4</v>
       </c>
-      <c r="O126">
-        <v>1</v>
-      </c>
-      <c r="P126" t="s">
+      <c r="P126">
+        <v>1</v>
+      </c>
+      <c r="Q126" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>155</v>
       </c>
@@ -6033,20 +6074,20 @@
       <c r="G127" t="s">
         <v>9</v>
       </c>
-      <c r="I127" t="s">
+      <c r="J127" t="s">
         <v>23</v>
       </c>
-      <c r="K127" t="s">
+      <c r="L127" t="s">
         <v>184</v>
       </c>
-      <c r="O127">
-        <v>1</v>
-      </c>
-      <c r="P127" t="s">
+      <c r="P127">
+        <v>1</v>
+      </c>
+      <c r="Q127" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>72</v>
       </c>
@@ -6065,20 +6106,20 @@
       <c r="F128" t="s">
         <v>188</v>
       </c>
-      <c r="H128" s="2">
+      <c r="I128" s="2">
         <v>9</v>
       </c>
-      <c r="I128" t="s">
+      <c r="J128" t="s">
         <v>16</v>
       </c>
-      <c r="O128">
-        <v>1</v>
-      </c>
-      <c r="P128" t="s">
+      <c r="P128">
+        <v>1</v>
+      </c>
+      <c r="Q128" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="129" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>179</v>
       </c>
@@ -6097,20 +6138,20 @@
       <c r="F129" t="s">
         <v>188</v>
       </c>
-      <c r="H129" s="2">
+      <c r="I129" s="2">
         <v>4</v>
       </c>
-      <c r="K129" t="s">
+      <c r="L129" t="s">
         <v>184</v>
       </c>
-      <c r="O129">
-        <v>1</v>
-      </c>
-      <c r="P129" t="s">
+      <c r="P129">
+        <v>1</v>
+      </c>
+      <c r="Q129" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="130" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>73</v>
       </c>
@@ -6129,17 +6170,17 @@
       <c r="F130" t="s">
         <v>8</v>
       </c>
-      <c r="H130" s="2">
+      <c r="I130" s="2">
         <v>2</v>
       </c>
-      <c r="O130">
-        <v>1</v>
-      </c>
-      <c r="P130" t="s">
+      <c r="P130">
+        <v>1</v>
+      </c>
+      <c r="Q130" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="131" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>47</v>
       </c>
@@ -6158,20 +6199,20 @@
       <c r="F131" t="s">
         <v>9</v>
       </c>
-      <c r="H131" s="2">
-        <v>1</v>
-      </c>
-      <c r="I131" t="s">
+      <c r="I131" s="2">
+        <v>1</v>
+      </c>
+      <c r="J131" t="s">
         <v>16</v>
       </c>
-      <c r="O131">
-        <v>1</v>
-      </c>
-      <c r="P131" t="s">
+      <c r="P131">
+        <v>1</v>
+      </c>
+      <c r="Q131" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="132" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>74</v>
       </c>
@@ -6190,17 +6231,17 @@
       <c r="F132" t="s">
         <v>8</v>
       </c>
-      <c r="H132" s="2">
+      <c r="I132" s="2">
         <v>10</v>
       </c>
-      <c r="O132">
-        <v>1</v>
-      </c>
-      <c r="P132" t="s">
+      <c r="P132">
+        <v>1</v>
+      </c>
+      <c r="Q132" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="133" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>150</v>
       </c>
@@ -6219,29 +6260,29 @@
       <c r="F133" t="s">
         <v>8</v>
       </c>
-      <c r="H133" s="2">
+      <c r="I133" s="2">
         <v>7</v>
       </c>
-      <c r="I133" t="s">
+      <c r="J133" t="s">
         <v>19</v>
       </c>
-      <c r="K133" t="s">
+      <c r="L133" t="s">
         <v>183</v>
       </c>
-      <c r="L133" t="s">
+      <c r="M133" t="s">
         <v>8</v>
       </c>
-      <c r="M133">
+      <c r="N133">
         <v>10</v>
       </c>
-      <c r="O133">
-        <v>1</v>
-      </c>
-      <c r="P133" t="s">
+      <c r="P133">
+        <v>1</v>
+      </c>
+      <c r="Q133" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="134" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>143</v>
       </c>
@@ -6260,17 +6301,17 @@
       <c r="F134" t="s">
         <v>9</v>
       </c>
-      <c r="I134" t="s">
+      <c r="J134" t="s">
         <v>23</v>
       </c>
-      <c r="O134">
-        <v>1</v>
-      </c>
-      <c r="P134" t="s">
+      <c r="P134">
+        <v>1</v>
+      </c>
+      <c r="Q134" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="135" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>100</v>
       </c>
@@ -6289,17 +6330,17 @@
       <c r="F135" t="s">
         <v>8</v>
       </c>
-      <c r="H135" s="2">
+      <c r="I135" s="2">
         <v>2</v>
       </c>
-      <c r="O135">
-        <v>1</v>
-      </c>
-      <c r="P135" t="s">
+      <c r="P135">
+        <v>1</v>
+      </c>
+      <c r="Q135" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="136" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>185</v>
       </c>
@@ -6318,23 +6359,23 @@
       <c r="F136" t="s">
         <v>188</v>
       </c>
-      <c r="H136" s="2">
+      <c r="I136" s="2">
         <v>14</v>
       </c>
-      <c r="I136" t="s">
+      <c r="J136" t="s">
         <v>14</v>
       </c>
-      <c r="K136" t="s">
+      <c r="L136" t="s">
         <v>184</v>
       </c>
-      <c r="O136">
-        <v>1</v>
-      </c>
-      <c r="P136" t="s">
+      <c r="P136">
+        <v>1</v>
+      </c>
+      <c r="Q136" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="137" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>279</v>
       </c>
@@ -6353,23 +6394,23 @@
       <c r="F137" t="s">
         <v>188</v>
       </c>
-      <c r="H137" s="2">
+      <c r="I137" s="2">
         <v>8</v>
       </c>
-      <c r="I137" t="s">
+      <c r="J137" t="s">
         <v>17</v>
       </c>
-      <c r="K137" t="s">
+      <c r="L137" t="s">
         <v>184</v>
       </c>
-      <c r="O137">
-        <v>1</v>
-      </c>
-      <c r="P137" t="s">
+      <c r="P137">
+        <v>1</v>
+      </c>
+      <c r="Q137" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="138" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>48</v>
       </c>
@@ -6388,17 +6429,17 @@
       <c r="F138" t="s">
         <v>9</v>
       </c>
-      <c r="H138" s="2">
+      <c r="I138" s="2">
         <v>6</v>
       </c>
-      <c r="O138">
+      <c r="P138">
         <v>2</v>
       </c>
-      <c r="P138" t="s">
+      <c r="Q138" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="139" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>144</v>
       </c>
@@ -6417,17 +6458,17 @@
       <c r="F139" t="s">
         <v>188</v>
       </c>
-      <c r="H139" s="2">
+      <c r="I139" s="2">
         <v>7</v>
       </c>
-      <c r="O139">
+      <c r="P139">
         <v>2</v>
       </c>
-      <c r="P139" t="s">
+      <c r="Q139" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="140" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>180</v>
       </c>
@@ -6446,20 +6487,20 @@
       <c r="F140" t="s">
         <v>188</v>
       </c>
-      <c r="H140" s="2">
+      <c r="I140" s="2">
         <v>4</v>
       </c>
-      <c r="K140" t="s">
+      <c r="L140" t="s">
         <v>184</v>
       </c>
-      <c r="O140">
-        <v>1</v>
-      </c>
-      <c r="P140" t="s">
+      <c r="P140">
+        <v>1</v>
+      </c>
+      <c r="Q140" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="141" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>192</v>
       </c>
@@ -6478,23 +6519,23 @@
       <c r="F141" t="s">
         <v>188</v>
       </c>
-      <c r="H141" s="2">
+      <c r="I141" s="2">
         <v>4</v>
       </c>
-      <c r="I141" t="s">
+      <c r="J141" t="s">
         <v>15</v>
       </c>
-      <c r="N141" t="s">
+      <c r="O141" t="s">
         <v>296</v>
       </c>
-      <c r="O141">
-        <v>1</v>
-      </c>
-      <c r="P141" t="s">
+      <c r="P141">
+        <v>1</v>
+      </c>
+      <c r="Q141" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="142" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>193</v>
       </c>
@@ -6513,23 +6554,23 @@
       <c r="F142" t="s">
         <v>188</v>
       </c>
-      <c r="H142" s="2">
+      <c r="I142" s="2">
         <v>4</v>
       </c>
-      <c r="I142" t="s">
+      <c r="J142" t="s">
         <v>15</v>
       </c>
-      <c r="N142" t="s">
+      <c r="O142" t="s">
         <v>296</v>
       </c>
-      <c r="O142">
-        <v>1</v>
-      </c>
-      <c r="P142" t="s">
+      <c r="P142">
+        <v>1</v>
+      </c>
+      <c r="Q142" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="143" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>194</v>
       </c>
@@ -6548,23 +6589,23 @@
       <c r="F143" t="s">
         <v>188</v>
       </c>
-      <c r="H143" s="2">
+      <c r="I143" s="2">
         <v>4</v>
       </c>
-      <c r="I143" t="s">
+      <c r="J143" t="s">
         <v>15</v>
       </c>
-      <c r="N143" t="s">
+      <c r="O143" t="s">
         <v>296</v>
       </c>
-      <c r="O143">
-        <v>1</v>
-      </c>
-      <c r="P143" t="s">
+      <c r="P143">
+        <v>1</v>
+      </c>
+      <c r="Q143" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="144" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>195</v>
       </c>
@@ -6583,23 +6624,23 @@
       <c r="F144" t="s">
         <v>188</v>
       </c>
-      <c r="H144" s="2">
+      <c r="I144" s="2">
         <v>4</v>
       </c>
-      <c r="I144" t="s">
+      <c r="J144" t="s">
         <v>15</v>
       </c>
-      <c r="N144" t="s">
+      <c r="O144" t="s">
         <v>296</v>
       </c>
-      <c r="O144">
-        <v>1</v>
-      </c>
-      <c r="P144" t="s">
+      <c r="P144">
+        <v>1</v>
+      </c>
+      <c r="Q144" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="145" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>196</v>
       </c>
@@ -6618,23 +6659,23 @@
       <c r="F145" t="s">
         <v>188</v>
       </c>
-      <c r="H145" s="2">
+      <c r="I145" s="2">
         <v>5</v>
       </c>
-      <c r="I145" t="s">
+      <c r="J145" t="s">
         <v>15</v>
       </c>
-      <c r="N145" t="s">
+      <c r="O145" t="s">
         <v>296</v>
       </c>
-      <c r="O145">
-        <v>1</v>
-      </c>
-      <c r="P145" t="s">
+      <c r="P145">
+        <v>1</v>
+      </c>
+      <c r="Q145" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="146" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>75</v>
       </c>
@@ -6653,17 +6694,17 @@
       <c r="F146" t="s">
         <v>8</v>
       </c>
-      <c r="H146" s="2">
+      <c r="I146" s="2">
         <v>4</v>
       </c>
-      <c r="O146">
-        <v>1</v>
-      </c>
-      <c r="P146" t="s">
+      <c r="P146">
+        <v>1</v>
+      </c>
+      <c r="Q146" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="147" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>76</v>
       </c>
@@ -6682,20 +6723,20 @@
       <c r="F147" t="s">
         <v>188</v>
       </c>
-      <c r="H147" s="2">
+      <c r="I147" s="2">
         <v>4</v>
       </c>
-      <c r="I147" t="s">
+      <c r="J147" t="s">
         <v>16</v>
       </c>
-      <c r="O147">
-        <v>1</v>
-      </c>
-      <c r="P147" t="s">
+      <c r="P147">
+        <v>1</v>
+      </c>
+      <c r="Q147" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="148" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>49</v>
       </c>
@@ -6714,17 +6755,17 @@
       <c r="F148" t="s">
         <v>188</v>
       </c>
-      <c r="H148" s="2">
+      <c r="I148" s="2">
         <v>10</v>
       </c>
-      <c r="O148">
-        <v>1</v>
-      </c>
-      <c r="P148" t="s">
+      <c r="P148">
+        <v>1</v>
+      </c>
+      <c r="Q148" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="149" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>50</v>
       </c>
@@ -6743,17 +6784,17 @@
       <c r="F149" t="s">
         <v>188</v>
       </c>
-      <c r="H149" s="2">
+      <c r="I149" s="2">
         <v>5</v>
       </c>
-      <c r="O149">
-        <v>1</v>
-      </c>
-      <c r="P149" t="s">
+      <c r="P149">
+        <v>1</v>
+      </c>
+      <c r="Q149" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="150" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>145</v>
       </c>
@@ -6772,17 +6813,17 @@
       <c r="F150" t="s">
         <v>188</v>
       </c>
-      <c r="H150" s="2">
+      <c r="I150" s="2">
         <v>6</v>
       </c>
-      <c r="O150">
+      <c r="P150">
         <v>2</v>
       </c>
-      <c r="P150" t="s">
+      <c r="Q150" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="151" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>146</v>
       </c>
@@ -6801,26 +6842,26 @@
       <c r="F151" t="s">
         <v>188</v>
       </c>
-      <c r="H151" s="2">
+      <c r="I151" s="2">
         <v>7</v>
       </c>
-      <c r="I151" t="s">
+      <c r="J151" t="s">
         <v>19</v>
       </c>
-      <c r="L151" t="s">
-        <v>188</v>
-      </c>
-      <c r="M151">
+      <c r="M151" t="s">
+        <v>188</v>
+      </c>
+      <c r="N151">
         <v>10</v>
       </c>
-      <c r="O151">
+      <c r="P151">
         <v>2</v>
       </c>
-      <c r="P151" t="s">
+      <c r="Q151" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="152" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>77</v>
       </c>
@@ -6839,17 +6880,17 @@
       <c r="F152" t="s">
         <v>188</v>
       </c>
-      <c r="H152" s="2">
+      <c r="I152" s="2">
         <v>2</v>
       </c>
-      <c r="O152">
-        <v>1</v>
-      </c>
-      <c r="P152" t="s">
+      <c r="P152">
+        <v>1</v>
+      </c>
+      <c r="Q152" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="153" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>101</v>
       </c>
@@ -6868,17 +6909,17 @@
       <c r="F153" t="s">
         <v>8</v>
       </c>
-      <c r="H153" s="2">
+      <c r="I153" s="2">
         <v>4</v>
       </c>
-      <c r="O153">
-        <v>1</v>
-      </c>
-      <c r="P153" t="s">
+      <c r="P153">
+        <v>1</v>
+      </c>
+      <c r="Q153" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="154" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>102</v>
       </c>
@@ -6900,20 +6941,20 @@
       <c r="G154" t="s">
         <v>8</v>
       </c>
-      <c r="H154" s="2">
+      <c r="I154" s="2">
         <v>5</v>
       </c>
-      <c r="I154" t="s">
+      <c r="J154" t="s">
         <v>12</v>
       </c>
-      <c r="O154">
+      <c r="P154">
         <v>2</v>
       </c>
-      <c r="P154" t="s">
+      <c r="Q154" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="155" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>181</v>
       </c>
@@ -6932,23 +6973,23 @@
       <c r="F155" t="s">
         <v>9</v>
       </c>
-      <c r="H155" s="2">
+      <c r="I155" s="2">
         <v>6</v>
       </c>
-      <c r="I155" t="s">
+      <c r="J155" t="s">
         <v>17</v>
       </c>
-      <c r="K155" t="s">
+      <c r="L155" t="s">
         <v>184</v>
       </c>
-      <c r="O155">
-        <v>1</v>
-      </c>
-      <c r="P155" t="s">
+      <c r="P155">
+        <v>1</v>
+      </c>
+      <c r="Q155" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="156" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>134</v>
       </c>
@@ -6967,17 +7008,17 @@
       <c r="F156" t="s">
         <v>188</v>
       </c>
-      <c r="H156" s="2">
+      <c r="I156" s="2">
         <v>5</v>
       </c>
-      <c r="O156">
-        <v>1</v>
-      </c>
-      <c r="P156" t="s">
+      <c r="P156">
+        <v>1</v>
+      </c>
+      <c r="Q156" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="157" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>135</v>
       </c>
@@ -6996,17 +7037,17 @@
       <c r="F157" t="s">
         <v>8</v>
       </c>
-      <c r="H157" s="2">
+      <c r="I157" s="2">
         <v>2</v>
       </c>
-      <c r="O157">
-        <v>1</v>
-      </c>
-      <c r="P157" t="s">
+      <c r="P157">
+        <v>1</v>
+      </c>
+      <c r="Q157" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="158" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>103</v>
       </c>
@@ -7028,20 +7069,20 @@
       <c r="G158" t="s">
         <v>8</v>
       </c>
-      <c r="H158" s="2">
+      <c r="I158" s="2">
         <v>6</v>
       </c>
-      <c r="I158" t="s">
+      <c r="J158" t="s">
         <v>12</v>
       </c>
-      <c r="O158">
-        <v>1</v>
-      </c>
-      <c r="P158" t="s">
+      <c r="P158">
+        <v>1</v>
+      </c>
+      <c r="Q158" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="159" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>51</v>
       </c>
@@ -7060,17 +7101,17 @@
       <c r="F159" t="s">
         <v>188</v>
       </c>
-      <c r="H159" s="2">
+      <c r="I159" s="2">
         <v>2</v>
       </c>
-      <c r="O159">
-        <v>1</v>
-      </c>
-      <c r="P159" t="s">
+      <c r="P159">
+        <v>1</v>
+      </c>
+      <c r="Q159" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="160" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>241</v>
       </c>
@@ -7089,20 +7130,20 @@
       <c r="F160" t="s">
         <v>8</v>
       </c>
-      <c r="H160" s="2">
+      <c r="I160" s="2">
         <v>7</v>
       </c>
-      <c r="I160" t="s">
+      <c r="J160" t="s">
         <v>13</v>
       </c>
-      <c r="O160">
+      <c r="P160">
         <v>2</v>
       </c>
-      <c r="P160" t="s">
+      <c r="Q160" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="161" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>182</v>
       </c>
@@ -7121,23 +7162,23 @@
       <c r="F161" t="s">
         <v>8</v>
       </c>
-      <c r="H161" s="2">
+      <c r="I161" s="2">
         <v>2</v>
       </c>
-      <c r="I161" t="s">
+      <c r="J161" t="s">
         <v>159</v>
       </c>
-      <c r="K161" t="s">
+      <c r="L161" t="s">
         <v>184</v>
       </c>
-      <c r="O161">
-        <v>1</v>
-      </c>
-      <c r="P161" t="s">
+      <c r="P161">
+        <v>1</v>
+      </c>
+      <c r="Q161" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="162" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>451</v>
       </c>
@@ -7156,20 +7197,20 @@
       <c r="F162" t="s">
         <v>188</v>
       </c>
-      <c r="H162" s="2">
+      <c r="I162" s="2">
         <v>5</v>
       </c>
-      <c r="I162" t="s">
+      <c r="J162" t="s">
         <v>17</v>
       </c>
-      <c r="O162">
+      <c r="P162">
         <v>2</v>
       </c>
-      <c r="P162" t="s">
+      <c r="Q162" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="163" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>78</v>
       </c>
@@ -7188,17 +7229,17 @@
       <c r="F163" t="s">
         <v>9</v>
       </c>
-      <c r="H163" s="2">
+      <c r="I163" s="2">
         <v>5</v>
       </c>
-      <c r="O163">
-        <v>1</v>
-      </c>
-      <c r="P163" t="s">
+      <c r="P163">
+        <v>1</v>
+      </c>
+      <c r="Q163" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="164" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>147</v>
       </c>
@@ -7217,17 +7258,18 @@
       <c r="F164" t="s">
         <v>188</v>
       </c>
-      <c r="H164" s="2">
+      <c r="I164" s="2">
         <v>5</v>
       </c>
-      <c r="O164">
+      <c r="P164">
         <v>2</v>
       </c>
-      <c r="P164" t="s">
+      <c r="Q164" t="s">
         <v>448</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576 E2:E1048576" xr:uid="{67751148-552D-428F-B986-68273F92E772}">
       <formula1>"Yes,No"</formula1>
@@ -7250,25 +7292,25 @@
           <x14:formula1>
             <xm:f>Types!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>L2:L1048576</xm:sqref>
+          <xm:sqref>M2:M1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FBBFEB1E-4E1B-4CB5-A3D3-437C1FE58F04}">
           <x14:formula1>
             <xm:f>Types!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>K2:K1048576</xm:sqref>
+          <xm:sqref>L2:L1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4A45EF90-835B-465D-80AD-C450C4F1AA0F}">
           <x14:formula1>
             <xm:f>Effects!$A$2:$A$14</xm:f>
           </x14:formula1>
-          <xm:sqref>I2:J1048576</xm:sqref>
+          <xm:sqref>J2:K1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{516B6739-FD2C-45E4-A26A-A4D6FD5141C9}">
           <x14:formula1>
             <xm:f>Types!$B$2:$B$5</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:G1048576</xm:sqref>
+          <xm:sqref>F2:H1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Fix combat for Transformed Young Vildkaarl
</commit_message>
<xml_diff>
--- a/cards.xlsx
+++ b/cards.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\witcher-3-gwent-list\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\witcher-3-gwent-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D6C0CAB-7182-4F9D-AB80-DBEA1C0C1FDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6A719ED-1AD9-4220-ACB7-58B84DFBCDC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{C7211A38-802B-4C9D-8105-50DCB0156070}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="21600" windowHeight="13749" xr2:uid="{C7211A38-802B-4C9D-8105-50DCB0156070}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -2021,30 +2021,30 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B137" sqref="B137"/>
+      <selection pane="bottomLeft" activeCell="F138" sqref="F138"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="28.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" customWidth="1"/>
-    <col min="9" max="9" width="10.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="71.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.07421875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.53515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.84375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.23046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.23046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.3046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.3046875" customWidth="1"/>
+    <col min="9" max="9" width="10.4609375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.69140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.53515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.07421875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.4609375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.53515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.3046875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.07421875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="71.84375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2097,7 +2097,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -2126,7 +2126,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>104</v>
       </c>
@@ -2158,7 +2158,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>105</v>
       </c>
@@ -2193,7 +2193,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -2222,7 +2222,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -2251,7 +2251,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>79</v>
       </c>
@@ -2286,7 +2286,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>159</v>
       </c>
@@ -2321,7 +2321,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>160</v>
       </c>
@@ -2356,7 +2356,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>136</v>
       </c>
@@ -2385,7 +2385,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>54</v>
       </c>
@@ -2414,7 +2414,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>161</v>
       </c>
@@ -2478,7 +2478,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>106</v>
       </c>
@@ -2507,7 +2507,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>236</v>
       </c>
@@ -2539,7 +2539,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>242</v>
       </c>
@@ -2568,7 +2568,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -2600,7 +2600,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>239</v>
       </c>
@@ -2635,7 +2635,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>162</v>
       </c>
@@ -2673,7 +2673,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>80</v>
       </c>
@@ -2708,7 +2708,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>240</v>
       </c>
@@ -2743,7 +2743,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>163</v>
       </c>
@@ -2778,7 +2778,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>164</v>
       </c>
@@ -2810,7 +2810,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>282</v>
       </c>
@@ -2845,7 +2845,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>165</v>
       </c>
@@ -2880,7 +2880,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>166</v>
       </c>
@@ -2912,7 +2912,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>167</v>
       </c>
@@ -2944,7 +2944,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>137</v>
       </c>
@@ -2970,7 +2970,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>107</v>
       </c>
@@ -2999,7 +2999,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>138</v>
       </c>
@@ -3034,7 +3034,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>151</v>
       </c>
@@ -3072,7 +3072,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>27</v>
       </c>
@@ -3104,7 +3104,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>108</v>
       </c>
@@ -3139,7 +3139,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>109</v>
       </c>
@@ -3174,7 +3174,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>110</v>
       </c>
@@ -3209,7 +3209,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>55</v>
       </c>
@@ -3238,7 +3238,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>139</v>
       </c>
@@ -3270,7 +3270,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>20</v>
       </c>
@@ -3305,7 +3305,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>81</v>
       </c>
@@ -3334,7 +3334,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>32</v>
       </c>
@@ -3363,7 +3363,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>82</v>
       </c>
@@ -3392,7 +3392,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
         <v>83</v>
       </c>
@@ -3427,7 +3427,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>169</v>
       </c>
@@ -3459,7 +3459,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
         <v>170</v>
       </c>
@@ -3494,7 +3494,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
         <v>111</v>
       </c>
@@ -3523,7 +3523,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
         <v>33</v>
       </c>
@@ -3555,7 +3555,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
         <v>84</v>
       </c>
@@ -3587,7 +3587,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
         <v>112</v>
       </c>
@@ -3616,7 +3616,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
         <v>85</v>
       </c>
@@ -3645,7 +3645,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
         <v>86</v>
       </c>
@@ -3677,7 +3677,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
         <v>140</v>
       </c>
@@ -3706,7 +3706,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A52" t="s">
         <v>113</v>
       </c>
@@ -3735,7 +3735,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
         <v>171</v>
       </c>
@@ -3770,7 +3770,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A54" t="s">
         <v>28</v>
       </c>
@@ -3799,7 +3799,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A55" t="s">
         <v>59</v>
       </c>
@@ -3831,7 +3831,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A56" t="s">
         <v>118</v>
       </c>
@@ -3860,7 +3860,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A57" t="s">
         <v>87</v>
       </c>
@@ -3895,7 +3895,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A58" t="s">
         <v>119</v>
       </c>
@@ -3924,7 +3924,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A59" t="s">
         <v>120</v>
       </c>
@@ -3953,7 +3953,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A60" t="s">
         <v>121</v>
       </c>
@@ -3982,7 +3982,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A61" t="s">
         <v>122</v>
       </c>
@@ -4011,7 +4011,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A62" t="s">
         <v>60</v>
       </c>
@@ -4040,7 +4040,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A63" t="s">
         <v>123</v>
       </c>
@@ -4069,7 +4069,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A64" t="s">
         <v>152</v>
       </c>
@@ -4107,7 +4107,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A65" t="s">
         <v>153</v>
       </c>
@@ -4142,7 +4142,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A66" t="s">
         <v>141</v>
       </c>
@@ -4177,7 +4177,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A67" t="s">
         <v>124</v>
       </c>
@@ -4209,7 +4209,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A68" t="s">
         <v>125</v>
       </c>
@@ -4238,7 +4238,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A69" t="s">
         <v>126</v>
       </c>
@@ -4267,7 +4267,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A70" t="s">
         <v>127</v>
       </c>
@@ -4302,7 +4302,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A71" t="s">
         <v>92</v>
       </c>
@@ -4334,7 +4334,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A72" t="s">
         <v>93</v>
       </c>
@@ -4366,7 +4366,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A73" t="s">
         <v>61</v>
       </c>
@@ -4395,7 +4395,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A74" t="s">
         <v>266</v>
       </c>
@@ -4427,7 +4427,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A75" t="s">
         <v>172</v>
       </c>
@@ -4459,7 +4459,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A76" t="s">
         <v>173</v>
       </c>
@@ -4491,7 +4491,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A77" t="s">
         <v>128</v>
       </c>
@@ -4520,7 +4520,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A78" t="s">
         <v>94</v>
       </c>
@@ -4549,7 +4549,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A79" t="s">
         <v>129</v>
       </c>
@@ -4578,7 +4578,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="80" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A80" t="s">
         <v>142</v>
       </c>
@@ -4607,7 +4607,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A81" t="s">
         <v>62</v>
       </c>
@@ -4639,7 +4639,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A82" t="s">
         <v>95</v>
       </c>
@@ -4668,7 +4668,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A83" t="s">
         <v>283</v>
       </c>
@@ -4700,7 +4700,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A84" t="s">
         <v>38</v>
       </c>
@@ -4729,7 +4729,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A85" t="s">
         <v>29</v>
       </c>
@@ -4761,7 +4761,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A86" t="s">
         <v>174</v>
       </c>
@@ -4799,7 +4799,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A87" t="s">
         <v>130</v>
       </c>
@@ -4837,7 +4837,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A88" t="s">
         <v>39</v>
       </c>
@@ -4866,7 +4866,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A89" t="s">
         <v>131</v>
       </c>
@@ -4895,7 +4895,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A90" t="s">
         <v>63</v>
       </c>
@@ -4924,7 +4924,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A91" t="s">
         <v>176</v>
       </c>
@@ -4959,7 +4959,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A92" t="s">
         <v>177</v>
       </c>
@@ -4991,7 +4991,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A93" t="s">
         <v>96</v>
       </c>
@@ -5020,7 +5020,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A94" t="s">
         <v>22</v>
       </c>
@@ -5058,7 +5058,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A95" t="s">
         <v>245</v>
       </c>
@@ -5090,7 +5090,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A96" t="s">
         <v>97</v>
       </c>
@@ -5122,7 +5122,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A97" t="s">
         <v>64</v>
       </c>
@@ -5151,7 +5151,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A98" t="s">
         <v>65</v>
       </c>
@@ -5180,7 +5180,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A99" t="s">
         <v>235</v>
       </c>
@@ -5212,7 +5212,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A100" t="s">
         <v>66</v>
       </c>
@@ -5244,7 +5244,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A101" t="s">
         <v>132</v>
       </c>
@@ -5276,7 +5276,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A102" t="s">
         <v>178</v>
       </c>
@@ -5317,7 +5317,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A103" t="s">
         <v>154</v>
       </c>
@@ -5358,7 +5358,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A104" t="s">
         <v>280</v>
       </c>
@@ -5387,7 +5387,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A105" t="s">
         <v>133</v>
       </c>
@@ -5416,7 +5416,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A106" t="s">
         <v>40</v>
       </c>
@@ -5448,7 +5448,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A107" t="s">
         <v>41</v>
       </c>
@@ -5480,7 +5480,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A108" t="s">
         <v>67</v>
       </c>
@@ -5509,7 +5509,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A109" t="s">
         <v>68</v>
       </c>
@@ -5538,7 +5538,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A110" t="s">
         <v>30</v>
       </c>
@@ -5567,7 +5567,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A111" t="s">
         <v>244</v>
       </c>
@@ -5596,7 +5596,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A112" t="s">
         <v>98</v>
       </c>
@@ -5625,7 +5625,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A113" t="s">
         <v>189</v>
       </c>
@@ -5657,7 +5657,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A114" t="s">
         <v>69</v>
       </c>
@@ -5686,7 +5686,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A115" t="s">
         <v>42</v>
       </c>
@@ -5715,7 +5715,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A116" t="s">
         <v>99</v>
       </c>
@@ -5744,7 +5744,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A117" t="s">
         <v>158</v>
       </c>
@@ -5785,7 +5785,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A118" t="s">
         <v>19</v>
       </c>
@@ -5811,7 +5811,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A119" t="s">
         <v>43</v>
       </c>
@@ -5840,7 +5840,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A120" t="s">
         <v>243</v>
       </c>
@@ -5872,7 +5872,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="121" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A121" t="s">
         <v>70</v>
       </c>
@@ -5901,7 +5901,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="122" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A122" t="s">
         <v>71</v>
       </c>
@@ -5933,7 +5933,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="123" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A123" t="s">
         <v>44</v>
       </c>
@@ -5962,7 +5962,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="124" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A124" t="s">
         <v>45</v>
       </c>
@@ -5991,7 +5991,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="125" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A125" t="s">
         <v>281</v>
       </c>
@@ -6023,7 +6023,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="126" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A126" t="s">
         <v>46</v>
       </c>
@@ -6052,7 +6052,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A127" t="s">
         <v>155</v>
       </c>
@@ -6087,7 +6087,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A128" t="s">
         <v>72</v>
       </c>
@@ -6119,7 +6119,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A129" t="s">
         <v>179</v>
       </c>
@@ -6151,7 +6151,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A130" t="s">
         <v>73</v>
       </c>
@@ -6180,7 +6180,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A131" t="s">
         <v>47</v>
       </c>
@@ -6212,7 +6212,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A132" t="s">
         <v>74</v>
       </c>
@@ -6241,7 +6241,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A133" t="s">
         <v>150</v>
       </c>
@@ -6282,7 +6282,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A134" t="s">
         <v>143</v>
       </c>
@@ -6311,7 +6311,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="135" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A135" t="s">
         <v>100</v>
       </c>
@@ -6340,7 +6340,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A136" t="s">
         <v>185</v>
       </c>
@@ -6375,7 +6375,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A137" t="s">
         <v>279</v>
       </c>
@@ -6392,7 +6392,7 @@
         <v>238</v>
       </c>
       <c r="F137" t="s">
-        <v>188</v>
+        <v>8</v>
       </c>
       <c r="I137" s="2">
         <v>8</v>
@@ -6410,7 +6410,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A138" t="s">
         <v>48</v>
       </c>
@@ -6439,7 +6439,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A139" t="s">
         <v>144</v>
       </c>
@@ -6468,7 +6468,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A140" t="s">
         <v>180</v>
       </c>
@@ -6500,7 +6500,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A141" t="s">
         <v>192</v>
       </c>
@@ -6535,7 +6535,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="142" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A142" t="s">
         <v>193</v>
       </c>
@@ -6570,7 +6570,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="143" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A143" t="s">
         <v>194</v>
       </c>
@@ -6605,7 +6605,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="144" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A144" t="s">
         <v>195</v>
       </c>
@@ -6640,7 +6640,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="145" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A145" t="s">
         <v>196</v>
       </c>
@@ -6675,7 +6675,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="146" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A146" t="s">
         <v>75</v>
       </c>
@@ -6704,7 +6704,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="147" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A147" t="s">
         <v>76</v>
       </c>
@@ -6736,7 +6736,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="148" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A148" t="s">
         <v>49</v>
       </c>
@@ -6765,7 +6765,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="149" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A149" t="s">
         <v>50</v>
       </c>
@@ -6794,7 +6794,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="150" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A150" t="s">
         <v>145</v>
       </c>
@@ -6823,7 +6823,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="151" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A151" t="s">
         <v>146</v>
       </c>
@@ -6861,7 +6861,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="152" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A152" t="s">
         <v>77</v>
       </c>
@@ -6890,7 +6890,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="153" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A153" t="s">
         <v>101</v>
       </c>
@@ -6919,7 +6919,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="154" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A154" t="s">
         <v>102</v>
       </c>
@@ -6954,7 +6954,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="155" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A155" t="s">
         <v>181</v>
       </c>
@@ -6989,7 +6989,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="156" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A156" t="s">
         <v>134</v>
       </c>
@@ -7018,7 +7018,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="157" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A157" t="s">
         <v>135</v>
       </c>
@@ -7047,7 +7047,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="158" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A158" t="s">
         <v>103</v>
       </c>
@@ -7082,7 +7082,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="159" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A159" t="s">
         <v>51</v>
       </c>
@@ -7111,7 +7111,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="160" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A160" t="s">
         <v>241</v>
       </c>
@@ -7143,7 +7143,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="161" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A161" t="s">
         <v>182</v>
       </c>
@@ -7178,7 +7178,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="162" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A162" t="s">
         <v>451</v>
       </c>
@@ -7210,7 +7210,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="163" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A163" t="s">
         <v>78</v>
       </c>
@@ -7239,7 +7239,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="164" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A164" t="s">
         <v>147</v>
       </c>
@@ -7326,16 +7326,16 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="37.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.53515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.23046875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="110.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="77.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="110.07421875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="77.84375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -7352,7 +7352,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>168</v>
       </c>
@@ -7369,7 +7369,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>231</v>
       </c>
@@ -7383,7 +7383,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
         <v>56</v>
       </c>
@@ -7398,7 +7398,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>156</v>
       </c>
@@ -7415,7 +7415,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
         <v>57</v>
       </c>
@@ -7430,7 +7430,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>58</v>
       </c>
@@ -7444,7 +7444,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
         <v>149</v>
       </c>
@@ -7461,7 +7461,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>114</v>
       </c>
@@ -7475,7 +7475,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
         <v>115</v>
       </c>
@@ -7490,7 +7490,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>116</v>
       </c>
@@ -7504,7 +7504,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" s="3" t="s">
         <v>117</v>
       </c>
@@ -7519,7 +7519,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -7533,7 +7533,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14" s="3" t="s">
         <v>35</v>
       </c>
@@ -7548,7 +7548,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>204</v>
       </c>
@@ -7565,7 +7565,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16" s="3" t="s">
         <v>36</v>
       </c>
@@ -7580,7 +7580,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -7594,7 +7594,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A18" s="3" t="s">
         <v>88</v>
       </c>
@@ -7609,7 +7609,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>157</v>
       </c>
@@ -7626,7 +7626,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A20" s="3" t="s">
         <v>89</v>
       </c>
@@ -7641,7 +7641,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>90</v>
       </c>
@@ -7655,7 +7655,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A22" s="3" t="s">
         <v>91</v>
       </c>
@@ -7670,7 +7670,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>175</v>
       </c>
@@ -7721,14 +7721,14 @@
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.21875" customWidth="1"/>
-    <col min="3" max="3" width="79.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.23046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.23046875" customWidth="1"/>
+    <col min="3" max="3" width="79.53515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7739,7 +7739,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -7747,12 +7747,12 @@
         <v>226</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -7760,7 +7760,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -7768,7 +7768,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -7776,7 +7776,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -7815,13 +7815,13 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.69140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="88" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7829,7 +7829,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -7837,7 +7837,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -7845,7 +7845,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>159</v>
       </c>
@@ -7853,7 +7853,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -7861,7 +7861,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -7869,7 +7869,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -7877,7 +7877,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -7885,7 +7885,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -7893,7 +7893,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -7901,7 +7901,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -7909,7 +7909,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -7917,7 +7917,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -7925,7 +7925,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -7949,13 +7949,13 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.23046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.07421875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>201</v>
       </c>
@@ -7966,7 +7966,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -7977,7 +7977,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -7988,7 +7988,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -7999,17 +7999,17 @@
         <v>183</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Fix scorch quote typo
</commit_message>
<xml_diff>
--- a/cards.xlsx
+++ b/cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\witcher-3-gwent-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6A719ED-1AD9-4220-ACB7-58B84DFBCDC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1048755-643D-444F-9591-0A767F2E1CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="21600" windowHeight="13749" xr2:uid="{C7211A38-802B-4C9D-8105-50DCB0156070}"/>
   </bookViews>
@@ -1269,9 +1269,6 @@
     <t>"Daughter of the Kaedweni Wilderness."</t>
   </si>
   <si>
-    <t>"Pillars of flame turn the mightiest to ash. All other tremble in shock and awe."</t>
-  </si>
-  <si>
     <t>"I was there, on the front lines! Right where the fightin' was thickest!"</t>
   </si>
   <si>
@@ -1402,6 +1399,9 @@
   </si>
   <si>
     <t>Combat 3</t>
+  </si>
+  <si>
+    <t>"Pillars of flame turn the mightiest to ash. All others tremble in shock and awe."</t>
   </si>
 </sst>
 </file>
@@ -2019,9 +2019,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D89E336D-773D-4B6A-9CD9-D024F295501B}">
   <dimension ref="A1:Q164"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F138" sqref="F138"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q119" sqref="Q119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2067,7 +2067,7 @@
         <v>199</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>1</v>
@@ -2105,7 +2105,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -2134,7 +2134,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -2166,7 +2166,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
@@ -2201,7 +2201,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -2230,7 +2230,7 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D6" t="s">
         <v>2</v>
@@ -2259,7 +2259,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D7" t="s">
         <v>3</v>
@@ -2294,7 +2294,7 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D8" t="s">
         <v>6</v>
@@ -2329,7 +2329,7 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D9" t="s">
         <v>6</v>
@@ -2364,7 +2364,7 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D10" t="s">
         <v>4</v>
@@ -2393,7 +2393,7 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D11" t="s">
         <v>7</v>
@@ -2422,7 +2422,7 @@
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D12" t="s">
         <v>2</v>
@@ -2454,7 +2454,7 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D13" t="s">
         <v>6</v>
@@ -2486,7 +2486,7 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>
@@ -2547,7 +2547,7 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D16" t="s">
         <v>7</v>
@@ -2576,7 +2576,7 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D17" t="s">
         <v>2</v>
@@ -2608,7 +2608,7 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D18" t="s">
         <v>5</v>
@@ -2643,13 +2643,13 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D19" t="s">
         <v>6</v>
       </c>
       <c r="E19" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F19" t="s">
         <v>188</v>
@@ -2681,7 +2681,7 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D20" t="s">
         <v>3</v>
@@ -2716,13 +2716,13 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D21" t="s">
         <v>4</v>
       </c>
       <c r="E21" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F21" t="s">
         <v>188</v>
@@ -2751,7 +2751,7 @@
         <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D22" t="s">
         <v>6</v>
@@ -2786,7 +2786,7 @@
         <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D23" t="s">
         <v>6</v>
@@ -2818,7 +2818,7 @@
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D24" t="s">
         <v>6</v>
@@ -2853,7 +2853,7 @@
         <v>3</v>
       </c>
       <c r="C25" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D25" t="s">
         <v>6</v>
@@ -2888,7 +2888,7 @@
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D26" t="s">
         <v>6</v>
@@ -2920,7 +2920,7 @@
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D27" t="s">
         <v>6</v>
@@ -2952,7 +2952,7 @@
         <v>2</v>
       </c>
       <c r="C28" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D28" t="s">
         <v>4</v>
@@ -2978,7 +2978,7 @@
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D29" t="s">
         <v>5</v>
@@ -3007,7 +3007,7 @@
         <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D30" t="s">
         <v>4</v>
@@ -3042,7 +3042,7 @@
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D31" t="s">
         <v>4</v>
@@ -3080,7 +3080,7 @@
         <v>3</v>
       </c>
       <c r="C32" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D32" t="s">
         <v>2</v>
@@ -3112,7 +3112,7 @@
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D33" t="s">
         <v>5</v>
@@ -3147,7 +3147,7 @@
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D34" t="s">
         <v>5</v>
@@ -3182,7 +3182,7 @@
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D35" t="s">
         <v>5</v>
@@ -3217,7 +3217,7 @@
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D36" t="s">
         <v>7</v>
@@ -3246,7 +3246,7 @@
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D37" t="s">
         <v>4</v>
@@ -3278,7 +3278,7 @@
         <v>3</v>
       </c>
       <c r="C38" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D38" t="s">
         <v>4</v>
@@ -3313,7 +3313,7 @@
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D39" t="s">
         <v>3</v>
@@ -3331,7 +3331,7 @@
         <v>1</v>
       </c>
       <c r="Q39" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.4">
@@ -3342,7 +3342,7 @@
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D40" t="s">
         <v>2</v>
@@ -3371,7 +3371,7 @@
         <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D41" t="s">
         <v>3</v>
@@ -3400,7 +3400,7 @@
         <v>3</v>
       </c>
       <c r="C42" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D42" t="s">
         <v>3</v>
@@ -3435,7 +3435,7 @@
         <v>1</v>
       </c>
       <c r="C43" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D43" t="s">
         <v>6</v>
@@ -3467,7 +3467,7 @@
         <v>1</v>
       </c>
       <c r="C44" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D44" t="s">
         <v>6</v>
@@ -3502,13 +3502,13 @@
         <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D45" t="s">
         <v>5</v>
       </c>
       <c r="E45" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F45" t="s">
         <v>188</v>
@@ -3531,7 +3531,7 @@
         <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D46" t="s">
         <v>2</v>
@@ -3563,7 +3563,7 @@
         <v>3</v>
       </c>
       <c r="C47" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D47" t="s">
         <v>3</v>
@@ -3595,7 +3595,7 @@
         <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D48" t="s">
         <v>5</v>
@@ -3624,13 +3624,13 @@
         <v>1</v>
       </c>
       <c r="C49" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D49" t="s">
         <v>3</v>
       </c>
       <c r="E49" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F49" t="s">
         <v>8</v>
@@ -3653,7 +3653,7 @@
         <v>3</v>
       </c>
       <c r="C50" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D50" t="s">
         <v>3</v>
@@ -3685,7 +3685,7 @@
         <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D51" t="s">
         <v>4</v>
@@ -3714,7 +3714,7 @@
         <v>1</v>
       </c>
       <c r="C52" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D52" t="s">
         <v>5</v>
@@ -3743,13 +3743,13 @@
         <v>1</v>
       </c>
       <c r="C53" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D53" t="s">
         <v>6</v>
       </c>
       <c r="E53" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F53" t="s">
         <v>8</v>
@@ -3778,13 +3778,13 @@
         <v>1</v>
       </c>
       <c r="C54" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D54" t="s">
         <v>2</v>
       </c>
       <c r="E54" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F54" t="s">
         <v>188</v>
@@ -3807,7 +3807,7 @@
         <v>2</v>
       </c>
       <c r="C55" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D55" t="s">
         <v>7</v>
@@ -3839,7 +3839,7 @@
         <v>1</v>
       </c>
       <c r="C56" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D56" t="s">
         <v>5</v>
@@ -3868,7 +3868,7 @@
         <v>1</v>
       </c>
       <c r="C57" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D57" t="s">
         <v>3</v>
@@ -3903,7 +3903,7 @@
         <v>1</v>
       </c>
       <c r="C58" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D58" t="s">
         <v>5</v>
@@ -3932,7 +3932,7 @@
         <v>1</v>
       </c>
       <c r="C59" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D59" t="s">
         <v>5</v>
@@ -3961,7 +3961,7 @@
         <v>1</v>
       </c>
       <c r="C60" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D60" t="s">
         <v>5</v>
@@ -3990,7 +3990,7 @@
         <v>1</v>
       </c>
       <c r="C61" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D61" t="s">
         <v>5</v>
@@ -4019,7 +4019,7 @@
         <v>1</v>
       </c>
       <c r="C62" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D62" t="s">
         <v>7</v>
@@ -4048,7 +4048,7 @@
         <v>1</v>
       </c>
       <c r="C63" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D63" t="s">
         <v>5</v>
@@ -4077,7 +4077,7 @@
         <v>1</v>
       </c>
       <c r="C64" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D64" t="s">
         <v>4</v>
@@ -4115,7 +4115,7 @@
         <v>3</v>
       </c>
       <c r="C65" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D65" t="s">
         <v>4</v>
@@ -4150,13 +4150,13 @@
         <v>1</v>
       </c>
       <c r="C66" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D66" t="s">
         <v>4</v>
       </c>
       <c r="E66" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F66" t="s">
         <v>188</v>
@@ -4185,7 +4185,7 @@
         <v>3</v>
       </c>
       <c r="C67" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D67" t="s">
         <v>5</v>
@@ -4217,7 +4217,7 @@
         <v>1</v>
       </c>
       <c r="C68" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D68" t="s">
         <v>5</v>
@@ -4246,7 +4246,7 @@
         <v>1</v>
       </c>
       <c r="C69" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D69" t="s">
         <v>5</v>
@@ -4275,7 +4275,7 @@
         <v>1</v>
       </c>
       <c r="C70" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D70" t="s">
         <v>5</v>
@@ -4310,7 +4310,7 @@
         <v>3</v>
       </c>
       <c r="C71" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D71" t="s">
         <v>3</v>
@@ -4342,7 +4342,7 @@
         <v>3</v>
       </c>
       <c r="C72" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D72" t="s">
         <v>3</v>
@@ -4374,7 +4374,7 @@
         <v>1</v>
       </c>
       <c r="C73" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D73" t="s">
         <v>7</v>
@@ -4409,7 +4409,7 @@
         <v>6</v>
       </c>
       <c r="E74" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F74" t="s">
         <v>188</v>
@@ -4435,13 +4435,13 @@
         <v>1</v>
       </c>
       <c r="C75" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D75" t="s">
         <v>6</v>
       </c>
       <c r="E75" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F75" t="s">
         <v>8</v>
@@ -4467,7 +4467,7 @@
         <v>1</v>
       </c>
       <c r="C76" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D76" t="s">
         <v>6</v>
@@ -4499,7 +4499,7 @@
         <v>1</v>
       </c>
       <c r="C77" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D77" t="s">
         <v>5</v>
@@ -4528,7 +4528,7 @@
         <v>1</v>
       </c>
       <c r="C78" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D78" t="s">
         <v>3</v>
@@ -4557,13 +4557,13 @@
         <v>1</v>
       </c>
       <c r="C79" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D79" t="s">
         <v>5</v>
       </c>
       <c r="E79" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F79" t="s">
         <v>188</v>
@@ -4586,7 +4586,7 @@
         <v>3</v>
       </c>
       <c r="C80" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D80" t="s">
         <v>4</v>
@@ -4615,7 +4615,7 @@
         <v>4</v>
       </c>
       <c r="C81" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D81" t="s">
         <v>7</v>
@@ -4647,13 +4647,13 @@
         <v>1</v>
       </c>
       <c r="C82" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D82" t="s">
         <v>3</v>
       </c>
       <c r="E82" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F82" t="s">
         <v>8</v>
@@ -4676,13 +4676,13 @@
         <v>1</v>
       </c>
       <c r="C83" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D83" t="s">
         <v>3</v>
       </c>
       <c r="E83" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F83" t="s">
         <v>188</v>
@@ -4708,13 +4708,13 @@
         <v>1</v>
       </c>
       <c r="C84" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D84" t="s">
         <v>2</v>
       </c>
       <c r="E84" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F84" t="s">
         <v>188</v>
@@ -4737,7 +4737,7 @@
         <v>1</v>
       </c>
       <c r="C85" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D85" t="s">
         <v>2</v>
@@ -4769,13 +4769,13 @@
         <v>1</v>
       </c>
       <c r="C86" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D86" t="s">
         <v>6</v>
       </c>
       <c r="E86" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F86" t="s">
         <v>188</v>
@@ -4807,13 +4807,13 @@
         <v>1</v>
       </c>
       <c r="C87" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D87" t="s">
         <v>5</v>
       </c>
       <c r="E87" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F87" t="s">
         <v>188</v>
@@ -4845,7 +4845,7 @@
         <v>1</v>
       </c>
       <c r="C88" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D88" t="s">
         <v>2</v>
@@ -4874,13 +4874,13 @@
         <v>1</v>
       </c>
       <c r="C89" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D89" t="s">
         <v>5</v>
       </c>
       <c r="E89" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F89" t="s">
         <v>8</v>
@@ -4903,13 +4903,13 @@
         <v>1</v>
       </c>
       <c r="C90" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D90" t="s">
         <v>7</v>
       </c>
       <c r="E90" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F90" t="s">
         <v>188</v>
@@ -4932,7 +4932,7 @@
         <v>3</v>
       </c>
       <c r="C91" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D91" t="s">
         <v>6</v>
@@ -4967,7 +4967,7 @@
         <v>1</v>
       </c>
       <c r="C92" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D92" t="s">
         <v>6</v>
@@ -4999,7 +4999,7 @@
         <v>5</v>
       </c>
       <c r="C93" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D93" t="s">
         <v>3</v>
@@ -5028,7 +5028,7 @@
         <v>3</v>
       </c>
       <c r="C94" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D94" t="s">
         <v>6</v>
@@ -5066,13 +5066,13 @@
         <v>1</v>
       </c>
       <c r="C95" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D95" t="s">
         <v>7</v>
       </c>
       <c r="E95" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F95" t="s">
         <v>188</v>
@@ -5098,7 +5098,7 @@
         <v>1</v>
       </c>
       <c r="C96" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D96" t="s">
         <v>3</v>
@@ -5130,7 +5130,7 @@
         <v>1</v>
       </c>
       <c r="C97" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D97" t="s">
         <v>7</v>
@@ -5159,13 +5159,13 @@
         <v>1</v>
       </c>
       <c r="C98" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D98" t="s">
         <v>7</v>
       </c>
       <c r="E98" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F98" t="s">
         <v>9</v>
@@ -5188,13 +5188,13 @@
         <v>1</v>
       </c>
       <c r="C99" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D99" t="s">
         <v>4</v>
       </c>
       <c r="E99" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F99" t="s">
         <v>188</v>
@@ -5220,7 +5220,7 @@
         <v>3</v>
       </c>
       <c r="C100" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D100" t="s">
         <v>7</v>
@@ -5252,7 +5252,7 @@
         <v>3</v>
       </c>
       <c r="C101" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D101" t="s">
         <v>5</v>
@@ -5284,7 +5284,7 @@
         <v>1</v>
       </c>
       <c r="C102" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D102" t="s">
         <v>6</v>
@@ -5325,7 +5325,7 @@
         <v>1</v>
       </c>
       <c r="C103" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D103" t="s">
         <v>4</v>
@@ -5366,13 +5366,13 @@
         <v>1</v>
       </c>
       <c r="C104" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D104" t="s">
         <v>2</v>
       </c>
       <c r="E104" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F104" t="s">
         <v>8</v>
@@ -5395,7 +5395,7 @@
         <v>1</v>
       </c>
       <c r="C105" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D105" t="s">
         <v>5</v>
@@ -5424,7 +5424,7 @@
         <v>3</v>
       </c>
       <c r="C106" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D106" t="s">
         <v>2</v>
@@ -5456,7 +5456,7 @@
         <v>1</v>
       </c>
       <c r="C107" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D107" t="s">
         <v>2</v>
@@ -5488,7 +5488,7 @@
         <v>1</v>
       </c>
       <c r="C108" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D108" t="s">
         <v>7</v>
@@ -5517,7 +5517,7 @@
         <v>1</v>
       </c>
       <c r="C109" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D109" t="s">
         <v>7</v>
@@ -5546,7 +5546,7 @@
         <v>2</v>
       </c>
       <c r="C110" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D110" t="s">
         <v>2</v>
@@ -5575,7 +5575,7 @@
         <v>1</v>
       </c>
       <c r="C111" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D111" t="s">
         <v>7</v>
@@ -5604,7 +5604,7 @@
         <v>1</v>
       </c>
       <c r="C112" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D112" t="s">
         <v>3</v>
@@ -5633,7 +5633,7 @@
         <v>1</v>
       </c>
       <c r="C113" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D113" t="s">
         <v>4</v>
@@ -5665,7 +5665,7 @@
         <v>1</v>
       </c>
       <c r="C114" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D114" t="s">
         <v>7</v>
@@ -5694,7 +5694,7 @@
         <v>1</v>
       </c>
       <c r="C115" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D115" t="s">
         <v>2</v>
@@ -5723,13 +5723,13 @@
         <v>1</v>
       </c>
       <c r="C116" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D116" t="s">
         <v>3</v>
       </c>
       <c r="E116" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F116" t="s">
         <v>8</v>
@@ -5752,7 +5752,7 @@
         <v>1</v>
       </c>
       <c r="C117" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D117" t="s">
         <v>3</v>
@@ -5793,7 +5793,7 @@
         <v>3</v>
       </c>
       <c r="C118" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D118" t="s">
         <v>4</v>
@@ -5808,7 +5808,7 @@
         <v>1</v>
       </c>
       <c r="Q118" t="s">
-        <v>409</v>
+        <v>453</v>
       </c>
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.4">
@@ -5819,7 +5819,7 @@
         <v>1</v>
       </c>
       <c r="C119" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D119" t="s">
         <v>2</v>
@@ -5837,7 +5837,7 @@
         <v>1</v>
       </c>
       <c r="Q119" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="120" spans="1:17" x14ac:dyDescent="0.4">
@@ -5848,7 +5848,7 @@
         <v>1</v>
       </c>
       <c r="C120" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D120" t="s">
         <v>7</v>
@@ -5869,7 +5869,7 @@
         <v>1</v>
       </c>
       <c r="Q120" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.4">
@@ -5880,7 +5880,7 @@
         <v>1</v>
       </c>
       <c r="C121" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D121" t="s">
         <v>7</v>
@@ -5898,7 +5898,7 @@
         <v>1</v>
       </c>
       <c r="Q121" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="122" spans="1:17" x14ac:dyDescent="0.4">
@@ -5909,7 +5909,7 @@
         <v>1</v>
       </c>
       <c r="C122" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D122" t="s">
         <v>7</v>
@@ -5930,7 +5930,7 @@
         <v>1</v>
       </c>
       <c r="Q122" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.4">
@@ -5941,7 +5941,7 @@
         <v>1</v>
       </c>
       <c r="C123" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D123" t="s">
         <v>2</v>
@@ -5970,7 +5970,7 @@
         <v>1</v>
       </c>
       <c r="C124" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D124" t="s">
         <v>2</v>
@@ -5988,7 +5988,7 @@
         <v>1</v>
       </c>
       <c r="Q124" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="125" spans="1:17" x14ac:dyDescent="0.4">
@@ -5999,7 +5999,7 @@
         <v>1</v>
       </c>
       <c r="C125" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D125" t="s">
         <v>2</v>
@@ -6020,7 +6020,7 @@
         <v>1</v>
       </c>
       <c r="Q125" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="126" spans="1:17" x14ac:dyDescent="0.4">
@@ -6031,7 +6031,7 @@
         <v>1</v>
       </c>
       <c r="C126" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D126" t="s">
         <v>2</v>
@@ -6049,7 +6049,7 @@
         <v>1</v>
       </c>
       <c r="Q126" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="127" spans="1:17" x14ac:dyDescent="0.4">
@@ -6060,7 +6060,7 @@
         <v>3</v>
       </c>
       <c r="C127" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D127" t="s">
         <v>4</v>
@@ -6084,7 +6084,7 @@
         <v>1</v>
       </c>
       <c r="Q127" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="128" spans="1:17" x14ac:dyDescent="0.4">
@@ -6095,7 +6095,7 @@
         <v>1</v>
       </c>
       <c r="C128" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D128" t="s">
         <v>7</v>
@@ -6116,7 +6116,7 @@
         <v>1</v>
       </c>
       <c r="Q128" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="129" spans="1:17" x14ac:dyDescent="0.4">
@@ -6127,7 +6127,7 @@
         <v>1</v>
       </c>
       <c r="C129" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D129" t="s">
         <v>6</v>
@@ -6159,7 +6159,7 @@
         <v>1</v>
       </c>
       <c r="C130" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D130" t="s">
         <v>7</v>
@@ -6177,7 +6177,7 @@
         <v>1</v>
       </c>
       <c r="Q130" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="131" spans="1:17" x14ac:dyDescent="0.4">
@@ -6188,7 +6188,7 @@
         <v>1</v>
       </c>
       <c r="C131" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D131" t="s">
         <v>2</v>
@@ -6209,7 +6209,7 @@
         <v>1</v>
       </c>
       <c r="Q131" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="132" spans="1:17" x14ac:dyDescent="0.4">
@@ -6220,13 +6220,13 @@
         <v>1</v>
       </c>
       <c r="C132" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D132" t="s">
         <v>7</v>
       </c>
       <c r="E132" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F132" t="s">
         <v>8</v>
@@ -6238,7 +6238,7 @@
         <v>1</v>
       </c>
       <c r="Q132" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="133" spans="1:17" x14ac:dyDescent="0.4">
@@ -6249,7 +6249,7 @@
         <v>1</v>
       </c>
       <c r="C133" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D133" t="s">
         <v>5</v>
@@ -6279,7 +6279,7 @@
         <v>1</v>
       </c>
       <c r="Q133" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="134" spans="1:17" x14ac:dyDescent="0.4">
@@ -6290,7 +6290,7 @@
         <v>2</v>
       </c>
       <c r="C134" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D134" t="s">
         <v>4</v>
@@ -6308,7 +6308,7 @@
         <v>1</v>
       </c>
       <c r="Q134" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="135" spans="1:17" x14ac:dyDescent="0.4">
@@ -6319,7 +6319,7 @@
         <v>1</v>
       </c>
       <c r="C135" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D135" t="s">
         <v>3</v>
@@ -6337,7 +6337,7 @@
         <v>1</v>
       </c>
       <c r="Q135" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="136" spans="1:17" x14ac:dyDescent="0.4">
@@ -6372,7 +6372,7 @@
         <v>1</v>
       </c>
       <c r="Q136" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="137" spans="1:17" x14ac:dyDescent="0.4">
@@ -6407,7 +6407,7 @@
         <v>1</v>
       </c>
       <c r="Q137" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="138" spans="1:17" x14ac:dyDescent="0.4">
@@ -6418,7 +6418,7 @@
         <v>2</v>
       </c>
       <c r="C138" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D138" t="s">
         <v>2</v>
@@ -6436,7 +6436,7 @@
         <v>2</v>
       </c>
       <c r="Q138" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="139" spans="1:17" x14ac:dyDescent="0.4">
@@ -6447,13 +6447,13 @@
         <v>1</v>
       </c>
       <c r="C139" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D139" t="s">
         <v>4</v>
       </c>
       <c r="E139" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F139" t="s">
         <v>188</v>
@@ -6465,7 +6465,7 @@
         <v>2</v>
       </c>
       <c r="Q139" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="140" spans="1:17" x14ac:dyDescent="0.4">
@@ -6476,7 +6476,7 @@
         <v>1</v>
       </c>
       <c r="C140" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D140" t="s">
         <v>6</v>
@@ -6508,7 +6508,7 @@
         <v>1</v>
       </c>
       <c r="C141" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D141" t="s">
         <v>5</v>
@@ -6532,7 +6532,7 @@
         <v>1</v>
       </c>
       <c r="Q141" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="142" spans="1:17" x14ac:dyDescent="0.4">
@@ -6543,7 +6543,7 @@
         <v>1</v>
       </c>
       <c r="C142" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D142" t="s">
         <v>5</v>
@@ -6567,7 +6567,7 @@
         <v>1</v>
       </c>
       <c r="Q142" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="143" spans="1:17" x14ac:dyDescent="0.4">
@@ -6578,7 +6578,7 @@
         <v>1</v>
       </c>
       <c r="C143" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D143" t="s">
         <v>5</v>
@@ -6602,7 +6602,7 @@
         <v>1</v>
       </c>
       <c r="Q143" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="144" spans="1:17" x14ac:dyDescent="0.4">
@@ -6613,7 +6613,7 @@
         <v>1</v>
       </c>
       <c r="C144" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D144" t="s">
         <v>5</v>
@@ -6637,7 +6637,7 @@
         <v>1</v>
       </c>
       <c r="Q144" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="145" spans="1:17" x14ac:dyDescent="0.4">
@@ -6648,7 +6648,7 @@
         <v>1</v>
       </c>
       <c r="C145" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D145" t="s">
         <v>5</v>
@@ -6672,7 +6672,7 @@
         <v>1</v>
       </c>
       <c r="Q145" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="146" spans="1:17" x14ac:dyDescent="0.4">
@@ -6683,7 +6683,7 @@
         <v>1</v>
       </c>
       <c r="C146" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D146" t="s">
         <v>7</v>
@@ -6701,7 +6701,7 @@
         <v>1</v>
       </c>
       <c r="Q146" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="147" spans="1:17" x14ac:dyDescent="0.4">
@@ -6712,7 +6712,7 @@
         <v>1</v>
       </c>
       <c r="C147" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D147" t="s">
         <v>7</v>
@@ -6733,7 +6733,7 @@
         <v>1</v>
       </c>
       <c r="Q147" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="148" spans="1:17" x14ac:dyDescent="0.4">
@@ -6744,13 +6744,13 @@
         <v>1</v>
       </c>
       <c r="C148" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D148" t="s">
         <v>2</v>
       </c>
       <c r="E148" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F148" t="s">
         <v>188</v>
@@ -6762,7 +6762,7 @@
         <v>1</v>
       </c>
       <c r="Q148" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="149" spans="1:17" x14ac:dyDescent="0.4">
@@ -6773,7 +6773,7 @@
         <v>1</v>
       </c>
       <c r="C149" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D149" t="s">
         <v>2</v>
@@ -6791,7 +6791,7 @@
         <v>1</v>
       </c>
       <c r="Q149" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="150" spans="1:17" x14ac:dyDescent="0.4">
@@ -6802,7 +6802,7 @@
         <v>1</v>
       </c>
       <c r="C150" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D150" t="s">
         <v>4</v>
@@ -6820,7 +6820,7 @@
         <v>2</v>
       </c>
       <c r="Q150" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="151" spans="1:17" x14ac:dyDescent="0.4">
@@ -6831,7 +6831,7 @@
         <v>1</v>
       </c>
       <c r="C151" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D151" t="s">
         <v>4</v>
@@ -6858,7 +6858,7 @@
         <v>2</v>
       </c>
       <c r="Q151" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="152" spans="1:17" x14ac:dyDescent="0.4">
@@ -6869,7 +6869,7 @@
         <v>1</v>
       </c>
       <c r="C152" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D152" t="s">
         <v>7</v>
@@ -6887,7 +6887,7 @@
         <v>1</v>
       </c>
       <c r="Q152" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="153" spans="1:17" x14ac:dyDescent="0.4">
@@ -6898,7 +6898,7 @@
         <v>1</v>
       </c>
       <c r="C153" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D153" t="s">
         <v>3</v>
@@ -6927,7 +6927,7 @@
         <v>2</v>
       </c>
       <c r="C154" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D154" t="s">
         <v>3</v>
@@ -6962,7 +6962,7 @@
         <v>3</v>
       </c>
       <c r="C155" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D155" t="s">
         <v>6</v>
@@ -6997,7 +6997,7 @@
         <v>1</v>
       </c>
       <c r="C156" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D156" t="s">
         <v>5</v>
@@ -7015,7 +7015,7 @@
         <v>1</v>
       </c>
       <c r="Q156" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="157" spans="1:17" x14ac:dyDescent="0.4">
@@ -7026,7 +7026,7 @@
         <v>1</v>
       </c>
       <c r="C157" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D157" t="s">
         <v>5</v>
@@ -7044,7 +7044,7 @@
         <v>1</v>
       </c>
       <c r="Q157" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="158" spans="1:17" x14ac:dyDescent="0.4">
@@ -7055,7 +7055,7 @@
         <v>1</v>
       </c>
       <c r="C158" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D158" t="s">
         <v>3</v>
@@ -7079,7 +7079,7 @@
         <v>1</v>
       </c>
       <c r="Q158" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="159" spans="1:17" x14ac:dyDescent="0.4">
@@ -7090,7 +7090,7 @@
         <v>1</v>
       </c>
       <c r="C159" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D159" t="s">
         <v>2</v>
@@ -7108,7 +7108,7 @@
         <v>1</v>
       </c>
       <c r="Q159" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="160" spans="1:17" x14ac:dyDescent="0.4">
@@ -7119,13 +7119,13 @@
         <v>1</v>
       </c>
       <c r="C160" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D160" t="s">
         <v>4</v>
       </c>
       <c r="E160" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F160" t="s">
         <v>8</v>
@@ -7140,7 +7140,7 @@
         <v>2</v>
       </c>
       <c r="Q160" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="161" spans="1:17" x14ac:dyDescent="0.4">
@@ -7151,7 +7151,7 @@
         <v>3</v>
       </c>
       <c r="C161" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D161" t="s">
         <v>6</v>
@@ -7180,13 +7180,13 @@
     </row>
     <row r="162" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A162" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B162">
         <v>2</v>
       </c>
       <c r="C162" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D162" t="s">
         <v>7</v>
@@ -7207,7 +7207,7 @@
         <v>2</v>
       </c>
       <c r="Q162" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="163" spans="1:17" x14ac:dyDescent="0.4">
@@ -7218,7 +7218,7 @@
         <v>1</v>
       </c>
       <c r="C163" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D163" t="s">
         <v>7</v>
@@ -7236,7 +7236,7 @@
         <v>1</v>
       </c>
       <c r="Q163" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="164" spans="1:17" x14ac:dyDescent="0.4">
@@ -7247,7 +7247,7 @@
         <v>1</v>
       </c>
       <c r="C164" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D164" t="s">
         <v>4</v>
@@ -7265,7 +7265,7 @@
         <v>2</v>
       </c>
       <c r="Q164" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
   </sheetData>
@@ -7930,7 +7930,7 @@
         <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
   </sheetData>

</xml_diff>